<commit_message>
new model - added reactions to gtoy3
</commit_message>
<xml_diff>
--- a/KineticModel/data/gtoyall.xlsx
+++ b/KineticModel/data/gtoyall.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shyam\Documents\Courses\CHE1125Project\IntegratedModels\KineticModel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shyam\Documents\Courses\CHE1125Project\IntegratedModels\KineticModel\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25590" windowHeight="7875" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25590" windowHeight="7875" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="gtoy1" sheetId="2" r:id="rId1"/>
@@ -18,11 +18,13 @@
     <sheet name="gtoy2C" sheetId="5" r:id="rId4"/>
     <sheet name="gtoy3" sheetId="6" r:id="rId5"/>
     <sheet name="gtoy3C" sheetId="7" r:id="rId6"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId7"/>
+    <sheet name="gtoy4" sheetId="8" r:id="rId7"/>
+    <sheet name="gtoy4C" sheetId="9" r:id="rId8"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId9"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId8"/>
-    <externalReference r:id="rId9"/>
+    <externalReference r:id="rId10"/>
+    <externalReference r:id="rId11"/>
   </externalReferences>
   <calcPr calcId="171027"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="125">
   <si>
     <t>Enzymes</t>
   </si>
@@ -415,6 +417,21 @@
   </si>
   <si>
     <t>ACex</t>
+  </si>
+  <si>
+    <t>[c] : 2pg &lt;==&gt; pep</t>
+  </si>
+  <si>
+    <t>pyr[c] ---&gt; pyr[e]</t>
+  </si>
+  <si>
+    <t>PYRex</t>
+  </si>
+  <si>
+    <t>[c] : g3p &lt;==&gt; 13dpg</t>
+  </si>
+  <si>
+    <t>g3p[c] ---&gt; fdp[c]</t>
   </si>
 </sst>
 </file>
@@ -583,6 +600,7 @@
       <sheetName val="red_test"/>
       <sheetName val="red_testC"/>
       <sheetName val="red_test2"/>
+      <sheetName val="Sheet3"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
@@ -636,9 +654,7 @@
           <cell r="D3" t="str">
             <v>Transport, Extracellular</v>
           </cell>
-          <cell r="E3">
-            <v>-8.2797927856445313</v>
-          </cell>
+          <cell r="E3"/>
           <cell r="F3">
             <v>0</v>
           </cell>
@@ -752,9 +768,7 @@
           <cell r="D7" t="str">
             <v>Transport, Extracellular</v>
           </cell>
-          <cell r="E7">
-            <v>0.22839999198913574</v>
-          </cell>
+          <cell r="E7"/>
           <cell r="F7">
             <v>0</v>
           </cell>
@@ -810,9 +824,7 @@
           <cell r="D9" t="str">
             <v>Citric Acid Cycle</v>
           </cell>
-          <cell r="E9">
-            <v>0</v>
-          </cell>
+          <cell r="E9"/>
           <cell r="F9">
             <v>-8.3000000000000007</v>
           </cell>
@@ -839,9 +851,7 @@
           <cell r="D10" t="str">
             <v>Transport, Extracellular</v>
           </cell>
-          <cell r="E10">
-            <v>0</v>
-          </cell>
+          <cell r="E10"/>
           <cell r="F10">
             <v>0</v>
           </cell>
@@ -897,9 +907,7 @@
           <cell r="D12" t="str">
             <v>Oxidative Phosphorylation</v>
           </cell>
-          <cell r="E12">
-            <v>-8.2797927856445313</v>
-          </cell>
+          <cell r="E12"/>
           <cell r="F12">
             <v>-6.6</v>
           </cell>
@@ -952,18 +960,10 @@
           <cell r="C14" t="str">
             <v>[c] : (1.496) 3pg + (3.7478) accoa + (59.8100) atp + (0.3610) e4p + (0.0709) f6p + (0.1290) g3p + (0.2050) g6p + (0.2557) gln-L + (4.9414) glu-L + (59.8100) h2o + (3.5470) nad + (13.0279) nadph + (1.7867) oaa + (0.5191) pep + (2.8328) pyr + (0.8977) r5p --&gt; (59.8100) adp + (4.1182) akg + (3.7478) coa + (59.8100) h + (3.5470) nadh + (13.0279) nadp + (59.8100) pi</v>
           </cell>
-          <cell r="D14">
-            <v>-5.4517974853515625</v>
-          </cell>
-          <cell r="E14">
-            <v>-5.4517974853515625</v>
-          </cell>
-          <cell r="F14">
-            <v>-5.4517974853515625</v>
-          </cell>
-          <cell r="G14">
-            <v>-5.4517974853515625</v>
-          </cell>
+          <cell r="D14"/>
+          <cell r="E14"/>
+          <cell r="F14"/>
+          <cell r="G14"/>
           <cell r="H14">
             <v>0.87390000000000001</v>
           </cell>
@@ -984,9 +984,7 @@
           <cell r="D15" t="str">
             <v>Transport, Extracellular</v>
           </cell>
-          <cell r="E15">
-            <v>0.2116999626159668</v>
-          </cell>
+          <cell r="E15"/>
           <cell r="F15">
             <v>0</v>
           </cell>
@@ -1013,9 +1011,7 @@
           <cell r="D16" t="str">
             <v>Citric Acid Cycle</v>
           </cell>
-          <cell r="E16">
-            <v>0.37749981880187988</v>
-          </cell>
+          <cell r="E16"/>
           <cell r="F16">
             <v>-8.6</v>
           </cell>
@@ -1042,9 +1038,7 @@
           <cell r="D17" t="str">
             <v>Oxidative Phosphorylation</v>
           </cell>
-          <cell r="E17">
-            <v>0.22839999198913574</v>
-          </cell>
+          <cell r="E17"/>
           <cell r="F17">
             <v>-37.200000000000003</v>
           </cell>
@@ -1071,9 +1065,7 @@
           <cell r="D18" t="str">
             <v>Transport, Extracellular</v>
           </cell>
-          <cell r="E18">
-            <v>0</v>
-          </cell>
+          <cell r="E18"/>
           <cell r="F18">
             <v>0</v>
           </cell>
@@ -1129,9 +1121,7 @@
           <cell r="D20" t="str">
             <v>Transport, Extracellular</v>
           </cell>
-          <cell r="E20">
-            <v>19.120697021484375</v>
-          </cell>
+          <cell r="E20"/>
           <cell r="F20">
             <v>0</v>
           </cell>
@@ -1158,15 +1148,9 @@
           <cell r="D21" t="str">
             <v>Exchange</v>
           </cell>
-          <cell r="E21">
-            <v>-8.2797927856445313</v>
-          </cell>
-          <cell r="F21">
-            <v>-8.2797927856445313</v>
-          </cell>
-          <cell r="G21">
-            <v>-8.2797927856445313</v>
-          </cell>
+          <cell r="E21"/>
+          <cell r="F21"/>
+          <cell r="G21"/>
           <cell r="H21">
             <v>0</v>
           </cell>
@@ -1187,15 +1171,9 @@
           <cell r="D22" t="str">
             <v>Exchange</v>
           </cell>
-          <cell r="E22">
-            <v>8.5031967163085938</v>
-          </cell>
-          <cell r="F22">
-            <v>8.5031967163085938</v>
-          </cell>
-          <cell r="G22">
-            <v>8.5031967163085938</v>
-          </cell>
+          <cell r="E22"/>
+          <cell r="F22"/>
+          <cell r="G22"/>
           <cell r="H22">
             <v>0</v>
           </cell>
@@ -1216,15 +1194,9 @@
           <cell r="D23" t="str">
             <v>Exchange</v>
           </cell>
-          <cell r="E23">
-            <v>0</v>
-          </cell>
-          <cell r="F23">
-            <v>0</v>
-          </cell>
-          <cell r="G23">
-            <v>0</v>
-          </cell>
+          <cell r="E23"/>
+          <cell r="F23"/>
+          <cell r="G23"/>
           <cell r="H23">
             <v>0</v>
           </cell>
@@ -1245,15 +1217,9 @@
           <cell r="D24" t="str">
             <v>Exchange</v>
           </cell>
-          <cell r="E24">
-            <v>0</v>
-          </cell>
-          <cell r="F24">
-            <v>0</v>
-          </cell>
-          <cell r="G24">
-            <v>0</v>
-          </cell>
+          <cell r="E24"/>
+          <cell r="F24"/>
+          <cell r="G24"/>
           <cell r="H24">
             <v>22.809799999999999</v>
           </cell>
@@ -1274,15 +1240,9 @@
           <cell r="D25" t="str">
             <v>Exchange</v>
           </cell>
-          <cell r="E25">
-            <v>-0.37749981880187988</v>
-          </cell>
-          <cell r="F25">
-            <v>-0.37749981880187988</v>
-          </cell>
-          <cell r="G25">
-            <v>-0.37749981880187988</v>
-          </cell>
+          <cell r="E25"/>
+          <cell r="F25"/>
+          <cell r="G25"/>
           <cell r="H25">
             <v>0</v>
           </cell>
@@ -1303,15 +1263,9 @@
           <cell r="D26" t="str">
             <v>Exchange</v>
           </cell>
-          <cell r="E26">
-            <v>8.2797927856445313</v>
-          </cell>
-          <cell r="F26">
-            <v>8.2797927856445313</v>
-          </cell>
-          <cell r="G26">
-            <v>8.2797927856445313</v>
-          </cell>
+          <cell r="E26"/>
+          <cell r="F26"/>
+          <cell r="G26"/>
           <cell r="H26">
             <v>0</v>
           </cell>
@@ -1332,15 +1286,9 @@
           <cell r="D27" t="str">
             <v>Exchange</v>
           </cell>
-          <cell r="E27">
-            <v>17.803985595703125</v>
-          </cell>
-          <cell r="F27">
-            <v>17.803985595703125</v>
-          </cell>
-          <cell r="G27">
-            <v>17.803985595703125</v>
-          </cell>
+          <cell r="E27"/>
+          <cell r="F27"/>
+          <cell r="G27"/>
           <cell r="H27">
             <v>0</v>
           </cell>
@@ -1361,15 +1309,9 @@
           <cell r="D28" t="str">
             <v>Exchange</v>
           </cell>
-          <cell r="E28">
-            <v>0</v>
-          </cell>
-          <cell r="F28">
-            <v>0</v>
-          </cell>
-          <cell r="G28">
-            <v>0</v>
-          </cell>
+          <cell r="E28"/>
+          <cell r="F28"/>
+          <cell r="G28"/>
           <cell r="H28">
             <v>0</v>
           </cell>
@@ -1390,15 +1332,9 @@
           <cell r="D29" t="str">
             <v>Exchange</v>
           </cell>
-          <cell r="E29">
-            <v>0</v>
-          </cell>
-          <cell r="F29">
-            <v>0</v>
-          </cell>
-          <cell r="G29">
-            <v>0</v>
-          </cell>
+          <cell r="E29"/>
+          <cell r="F29"/>
+          <cell r="G29"/>
           <cell r="H29">
             <v>-10</v>
           </cell>
@@ -1419,15 +1355,9 @@
           <cell r="D30" t="str">
             <v>Exchange</v>
           </cell>
-          <cell r="E30">
-            <v>-10</v>
-          </cell>
-          <cell r="F30">
-            <v>-10</v>
-          </cell>
-          <cell r="G30">
-            <v>-10</v>
-          </cell>
+          <cell r="E30"/>
+          <cell r="F30"/>
+          <cell r="G30"/>
           <cell r="H30">
             <v>0</v>
           </cell>
@@ -1448,15 +1378,9 @@
           <cell r="D31" t="str">
             <v>Exchange</v>
           </cell>
-          <cell r="E31">
-            <v>0</v>
-          </cell>
-          <cell r="F31">
-            <v>0</v>
-          </cell>
-          <cell r="G31">
-            <v>0</v>
-          </cell>
+          <cell r="E31"/>
+          <cell r="F31"/>
+          <cell r="G31"/>
           <cell r="H31">
             <v>0</v>
           </cell>
@@ -1477,15 +1401,9 @@
           <cell r="D32" t="str">
             <v>Exchange</v>
           </cell>
-          <cell r="E32">
-            <v>0</v>
-          </cell>
-          <cell r="F32">
-            <v>0</v>
-          </cell>
-          <cell r="G32">
-            <v>0</v>
-          </cell>
+          <cell r="E32"/>
+          <cell r="F32"/>
+          <cell r="G32"/>
           <cell r="H32">
             <v>17.530899999999999</v>
           </cell>
@@ -1506,15 +1424,9 @@
           <cell r="D33" t="str">
             <v>Exchange</v>
           </cell>
-          <cell r="E33">
-            <v>30.553192138671875</v>
-          </cell>
-          <cell r="F33">
-            <v>30.553192138671875</v>
-          </cell>
-          <cell r="G33">
-            <v>30.553192138671875</v>
-          </cell>
+          <cell r="E33"/>
+          <cell r="F33"/>
+          <cell r="G33"/>
           <cell r="H33">
             <v>29.175799999999999</v>
           </cell>
@@ -1535,15 +1447,9 @@
           <cell r="D34" t="str">
             <v>Exchange</v>
           </cell>
-          <cell r="E34">
-            <v>-7.1154975891113281</v>
-          </cell>
-          <cell r="F34">
-            <v>-7.1154975891113281</v>
-          </cell>
-          <cell r="G34">
-            <v>-7.1154975891113281</v>
-          </cell>
+          <cell r="E34"/>
+          <cell r="F34"/>
+          <cell r="G34"/>
           <cell r="H34">
             <v>0</v>
           </cell>
@@ -1564,15 +1470,9 @@
           <cell r="D35" t="str">
             <v>Exchange</v>
           </cell>
-          <cell r="E35">
-            <v>0</v>
-          </cell>
-          <cell r="F35">
-            <v>0</v>
-          </cell>
-          <cell r="G35">
-            <v>0</v>
-          </cell>
+          <cell r="E35"/>
+          <cell r="F35"/>
+          <cell r="G35"/>
           <cell r="H35">
             <v>0</v>
           </cell>
@@ -1593,15 +1493,9 @@
           <cell r="D36" t="str">
             <v>Exchange</v>
           </cell>
-          <cell r="E36">
-            <v>0</v>
-          </cell>
-          <cell r="F36">
-            <v>0</v>
-          </cell>
-          <cell r="G36">
-            <v>0</v>
-          </cell>
+          <cell r="E36"/>
+          <cell r="F36"/>
+          <cell r="G36"/>
           <cell r="H36">
             <v>-4.7652999999999999</v>
           </cell>
@@ -1622,15 +1516,9 @@
           <cell r="D37" t="str">
             <v>Exchange</v>
           </cell>
-          <cell r="E37">
-            <v>-1.1541996002197266</v>
-          </cell>
-          <cell r="F37">
-            <v>-1.1541996002197266</v>
-          </cell>
-          <cell r="G37">
-            <v>-1.1541996002197266</v>
-          </cell>
+          <cell r="E37"/>
+          <cell r="F37"/>
+          <cell r="G37"/>
           <cell r="H37">
             <v>-21.799499999999998</v>
           </cell>
@@ -1651,15 +1539,9 @@
           <cell r="D38" t="str">
             <v>Exchange</v>
           </cell>
-          <cell r="E38">
-            <v>0</v>
-          </cell>
-          <cell r="F38">
-            <v>0</v>
-          </cell>
-          <cell r="G38">
-            <v>0</v>
-          </cell>
+          <cell r="E38"/>
+          <cell r="F38"/>
+          <cell r="G38"/>
           <cell r="H38">
             <v>-3.2149000000000001</v>
           </cell>
@@ -1680,15 +1562,9 @@
           <cell r="D39" t="str">
             <v>Exchange</v>
           </cell>
-          <cell r="E39">
-            <v>-0.77859973907470703</v>
-          </cell>
-          <cell r="F39">
-            <v>-0.77859973907470703</v>
-          </cell>
-          <cell r="G39">
-            <v>-0.77859973907470703</v>
-          </cell>
+          <cell r="E39"/>
+          <cell r="F39"/>
+          <cell r="G39"/>
           <cell r="H39">
             <v>0</v>
           </cell>
@@ -1709,15 +1585,9 @@
           <cell r="D40" t="str">
             <v>Exchange</v>
           </cell>
-          <cell r="E40">
-            <v>0</v>
-          </cell>
-          <cell r="F40">
-            <v>0</v>
-          </cell>
-          <cell r="G40">
-            <v>0</v>
-          </cell>
+          <cell r="E40"/>
+          <cell r="F40"/>
+          <cell r="G40"/>
           <cell r="H40">
             <v>0</v>
           </cell>
@@ -1796,9 +1666,7 @@
           <cell r="D43" t="str">
             <v>Transport, Extracellular</v>
           </cell>
-          <cell r="E43">
-            <v>0</v>
-          </cell>
+          <cell r="E43"/>
           <cell r="F43">
             <v>0</v>
           </cell>
@@ -1825,9 +1693,7 @@
           <cell r="D44" t="str">
             <v>Transport, Extracellular</v>
           </cell>
-          <cell r="E44">
-            <v>0</v>
-          </cell>
+          <cell r="E44"/>
           <cell r="F44">
             <v>0</v>
           </cell>
@@ -1883,9 +1749,7 @@
           <cell r="D46" t="str">
             <v>Transport, Extracellular</v>
           </cell>
-          <cell r="E46">
-            <v>0</v>
-          </cell>
+          <cell r="E46"/>
           <cell r="F46">
             <v>-9.1</v>
           </cell>
@@ -1941,9 +1805,7 @@
           <cell r="D48" t="str">
             <v>Transport, Extracellular</v>
           </cell>
-          <cell r="E48">
-            <v>0</v>
-          </cell>
+          <cell r="E48"/>
           <cell r="F48">
             <v>0</v>
           </cell>
@@ -2028,9 +1890,7 @@
           <cell r="D51" t="str">
             <v>Transport, Extracellular</v>
           </cell>
-          <cell r="E51">
-            <v>19.437286376953125</v>
-          </cell>
+          <cell r="E51"/>
           <cell r="F51">
             <v>-9.1</v>
           </cell>
@@ -2086,9 +1946,7 @@
           <cell r="D53" t="str">
             <v>Transport, Extracellular</v>
           </cell>
-          <cell r="E53">
-            <v>5.4099977016448975E-2</v>
-          </cell>
+          <cell r="E53"/>
           <cell r="F53">
             <v>-6.6</v>
           </cell>
@@ -2202,9 +2060,7 @@
           <cell r="D57" t="str">
             <v>Transport, Extracellular</v>
           </cell>
-          <cell r="E57">
-            <v>0</v>
-          </cell>
+          <cell r="E57"/>
           <cell r="F57">
             <v>0</v>
           </cell>
@@ -2260,9 +2116,7 @@
           <cell r="D59" t="str">
             <v>Transport, Extracellular</v>
           </cell>
-          <cell r="E59">
-            <v>0</v>
-          </cell>
+          <cell r="E59"/>
           <cell r="F59">
             <v>0</v>
           </cell>
@@ -2405,9 +2259,7 @@
           <cell r="D64" t="str">
             <v>Transport, Extracellular</v>
           </cell>
-          <cell r="E64">
-            <v>0</v>
-          </cell>
+          <cell r="E64"/>
           <cell r="F64">
             <v>0</v>
           </cell>
@@ -2579,9 +2431,7 @@
           <cell r="D70" t="str">
             <v>Inorganic Ion Transport and Metabolism</v>
           </cell>
-          <cell r="E70">
-            <v>0</v>
-          </cell>
+          <cell r="E70"/>
           <cell r="F70">
             <v>0</v>
           </cell>
@@ -2608,9 +2458,7 @@
           <cell r="D71" t="str">
             <v>Transport, Extracellular</v>
           </cell>
-          <cell r="E71">
-            <v>1.1541996002197266</v>
-          </cell>
+          <cell r="E71"/>
           <cell r="F71">
             <v>0</v>
           </cell>
@@ -2637,9 +2485,7 @@
           <cell r="D72" t="str">
             <v>Glycolysis/Gluconeogenesis</v>
           </cell>
-          <cell r="E72">
-            <v>0</v>
-          </cell>
+          <cell r="E72"/>
           <cell r="F72">
             <v>-8.3000000000000007</v>
           </cell>
@@ -2695,9 +2541,7 @@
           <cell r="D74" t="str">
             <v>Pyruvate Metabolism</v>
           </cell>
-          <cell r="E74">
-            <v>9.7894973754882813</v>
-          </cell>
+          <cell r="E74"/>
           <cell r="F74">
             <v>-5.0999999999999996</v>
           </cell>
@@ -2840,9 +2684,7 @@
           <cell r="D79" t="str">
             <v>Inorganic Ion Transport and Metabolism</v>
           </cell>
-          <cell r="E79">
-            <v>-19.120697021484375</v>
-          </cell>
+          <cell r="E79"/>
           <cell r="F79">
             <v>0</v>
           </cell>
@@ -3013,6 +2855,7 @@
       <sheetData sheetId="17"/>
       <sheetData sheetId="18"/>
       <sheetData sheetId="19"/>
+      <sheetData sheetId="20" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -5752,8 +5595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10:O13"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:U13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6290,10 +6133,768 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection sqref="A1:U17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="25.5703125" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="13">
+        <f>VLOOKUP(A2,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="17">
+        <v>1</v>
+      </c>
+      <c r="J2" s="13">
+        <v>0</v>
+      </c>
+      <c r="K2" s="13"/>
+      <c r="L2" s="20">
+        <v>2.7799999999999998E-4</v>
+      </c>
+      <c r="M2" s="18"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13"/>
+      <c r="S2" s="13"/>
+      <c r="T2" s="13"/>
+      <c r="U2" s="13"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13">
+        <v>-30.5</v>
+      </c>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13">
+        <v>1</v>
+      </c>
+      <c r="J3" s="13">
+        <v>0</v>
+      </c>
+      <c r="K3" s="13"/>
+      <c r="L3" s="20">
+        <v>2.7799999999999998E-4</v>
+      </c>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="13"/>
+      <c r="R3" s="13"/>
+      <c r="S3" s="13"/>
+      <c r="T3" s="13"/>
+      <c r="U3" s="13"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13">
+        <v>-30.5</v>
+      </c>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13">
+        <v>1</v>
+      </c>
+      <c r="J4" s="13">
+        <v>0</v>
+      </c>
+      <c r="K4" s="13"/>
+      <c r="L4" s="20">
+        <v>2.7799999999999998E-4</v>
+      </c>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="P4" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q4" s="13"/>
+      <c r="R4" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="S4" s="13"/>
+      <c r="T4" s="13"/>
+      <c r="U4" s="13"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13">
+        <v>0</v>
+      </c>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13">
+        <v>1</v>
+      </c>
+      <c r="J5" s="13">
+        <v>1</v>
+      </c>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="13"/>
+      <c r="R5" s="13"/>
+      <c r="S5" s="13"/>
+      <c r="T5" s="13"/>
+      <c r="U5" s="13"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13">
+        <v>0</v>
+      </c>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13">
+        <v>1</v>
+      </c>
+      <c r="J6" s="13">
+        <v>0</v>
+      </c>
+      <c r="K6" s="13"/>
+      <c r="L6" s="20">
+        <v>2.7799999999999998E-4</v>
+      </c>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="13"/>
+      <c r="S6" s="13"/>
+      <c r="T6" s="13"/>
+      <c r="U6" s="13"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13">
+        <v>0</v>
+      </c>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13">
+        <v>1</v>
+      </c>
+      <c r="J7" s="13">
+        <v>0</v>
+      </c>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="13"/>
+      <c r="R7" s="13"/>
+      <c r="S7" s="13"/>
+      <c r="T7" s="13"/>
+      <c r="U7" s="13"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13">
+        <v>0</v>
+      </c>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13">
+        <v>1</v>
+      </c>
+      <c r="J8" s="13">
+        <v>1</v>
+      </c>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="13"/>
+      <c r="R8" s="13"/>
+      <c r="S8" s="13"/>
+      <c r="T8" s="13"/>
+      <c r="U8" s="13"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13">
+        <v>0</v>
+      </c>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13">
+        <v>1</v>
+      </c>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+      <c r="R9" s="13"/>
+      <c r="S9" s="13"/>
+      <c r="T9" s="13"/>
+      <c r="U9" s="13"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="13"/>
+      <c r="C10" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13">
+        <f>VLOOKUP(A10,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>4.3</v>
+      </c>
+      <c r="F10" s="13">
+        <v>-24.3</v>
+      </c>
+      <c r="G10" s="13">
+        <v>52.1</v>
+      </c>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13">
+        <v>280</v>
+      </c>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="16" t="str">
+        <f>VLOOKUP(A10,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>2.7.2.1</v>
+      </c>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="13"/>
+      <c r="R10" s="13"/>
+      <c r="S10" s="13"/>
+      <c r="T10" s="13"/>
+      <c r="U10" s="13"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="13"/>
+      <c r="C11" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="13">
+        <f>VLOOKUP(A11,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>3.8</v>
+      </c>
+      <c r="F11" s="13">
+        <v>-20.399999999999999</v>
+      </c>
+      <c r="G11" s="13">
+        <v>28.7</v>
+      </c>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13">
+        <v>120</v>
+      </c>
+      <c r="J11" s="13">
+        <v>0.02</v>
+      </c>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="16" t="str">
+        <f>VLOOKUP(A11,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>2.3.1.8</v>
+      </c>
+      <c r="O11" s="13"/>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="13"/>
+      <c r="R11" s="13"/>
+      <c r="S11" s="13"/>
+      <c r="T11" s="13"/>
+      <c r="U11" s="13"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" s="13"/>
+      <c r="C12" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="13">
+        <v>-8.3000000000000007</v>
+      </c>
+      <c r="F12" s="13">
+        <v>-73</v>
+      </c>
+      <c r="G12" s="13">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13">
+        <v>6.32</v>
+      </c>
+      <c r="J12" s="13">
+        <v>0</v>
+      </c>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="O12" s="13"/>
+      <c r="P12" s="13"/>
+      <c r="Q12" s="13"/>
+      <c r="R12" s="13"/>
+      <c r="S12" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="T12" s="13">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="U12" s="13">
+        <v>0.27600000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="13"/>
+      <c r="C13" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="13">
+        <v>-31.12</v>
+      </c>
+      <c r="F13" s="13">
+        <v>-10.8</v>
+      </c>
+      <c r="G13" s="13">
+        <v>65.3</v>
+      </c>
+      <c r="H13" s="20"/>
+      <c r="I13" s="13">
+        <v>2540</v>
+      </c>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="18"/>
+      <c r="N13" s="16" t="str">
+        <f>VLOOKUP(A13,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>2.7.1.40</v>
+      </c>
+      <c r="O13" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="P13" s="13"/>
+      <c r="Q13" s="13"/>
+      <c r="R13" s="13"/>
+      <c r="S13" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="T13" s="13">
+        <v>0.111</v>
+      </c>
+      <c r="U13" s="13">
+        <v>0.111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="E14" s="13">
+        <f>VLOOKUP(A14,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>-0.9</v>
+      </c>
+      <c r="F14" s="13">
+        <v>-22.9</v>
+      </c>
+      <c r="G14" s="13">
+        <v>14.7</v>
+      </c>
+      <c r="I14" s="13">
+        <v>355.79</v>
+      </c>
+      <c r="M14" s="18">
+        <v>24.294625983764298</v>
+      </c>
+      <c r="N14" s="16" t="str">
+        <f>VLOOKUP(A14,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>4.2.1.11</v>
+      </c>
+      <c r="S14" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="T14" s="13">
+        <v>2.67</v>
+      </c>
+      <c r="U14" s="13">
+        <v>2.67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="13">
+        <v>6.2290000000000001</v>
+      </c>
+      <c r="F15" s="13">
+        <v>-23.1</v>
+      </c>
+      <c r="G15" s="13">
+        <v>14.6</v>
+      </c>
+      <c r="J15" s="13">
+        <v>530</v>
+      </c>
+      <c r="M15" s="18">
+        <v>-24.294625983764298</v>
+      </c>
+      <c r="N15" s="16" t="str">
+        <f>VLOOKUP(A15,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>5.4.2.1</v>
+      </c>
+      <c r="S15" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="T15" s="13">
+        <v>2.67</v>
+      </c>
+      <c r="U15" s="13">
+        <v>2.67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" s="13">
+        <v>-10.51</v>
+      </c>
+      <c r="F16" s="13">
+        <v>-19.2</v>
+      </c>
+      <c r="G16" s="13">
+        <v>56.1</v>
+      </c>
+      <c r="H16" s="20"/>
+      <c r="J16" s="13">
+        <v>654</v>
+      </c>
+      <c r="M16" s="18">
+        <v>-27.772223526897601</v>
+      </c>
+      <c r="N16" s="16" t="str">
+        <f>VLOOKUP(A16,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>2.7.2.3</v>
+      </c>
+      <c r="S16" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="T16" s="13">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="U16" s="13">
+        <v>0.39900000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" s="13" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="13">
+        <f>VLOOKUP(A17,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>-0.1</v>
+      </c>
+      <c r="F17" s="13">
+        <v>-12.8</v>
+      </c>
+      <c r="G17" s="13">
+        <v>62.6</v>
+      </c>
+      <c r="I17" s="13">
+        <v>268</v>
+      </c>
+      <c r="M17" s="18">
+        <v>27.772223526897601</v>
+      </c>
+      <c r="N17" s="16" t="str">
+        <f>VLOOKUP(A17,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>1.2.1.12</v>
+      </c>
+      <c r="S17" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="T17" s="13">
+        <v>2.13</v>
+      </c>
+      <c r="U17" s="13">
+        <v>2.13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="E18" s="17"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="16"/>
+    </row>
+    <row r="19" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="16"/>
+      <c r="C19" s="16"/>
+      <c r="H19" s="20"/>
+      <c r="L19" s="20"/>
+      <c r="M19" s="18"/>
+      <c r="N19" s="16"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" s="13">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A9" sqref="A9:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add new rxns in upper glycolysis
</commit_message>
<xml_diff>
--- a/KineticModel/data/gtoyall.xlsx
+++ b/KineticModel/data/gtoyall.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shyam\Documents\Courses\CHE1125Project\IntegratedModels\KineticModel\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shyam\Documents\Courses\CHE1125Project\IntegratedModels\KineticModel\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
     <externalReference r:id="rId10"/>
     <externalReference r:id="rId11"/>
   </externalReferences>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="124">
   <si>
     <t>Enzymes</t>
   </si>
@@ -429,9 +429,6 @@
   </si>
   <si>
     <t>[c] : g3p &lt;==&gt; 13dpg</t>
-  </si>
-  <si>
-    <t>g3p[c] ---&gt; fdp[c]</t>
   </si>
 </sst>
 </file>
@@ -4442,23 +4439,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -4494,23 +4474,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -6135,8 +6098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection sqref="A1:U17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6250,42 +6213,41 @@
       <c r="T2" s="13"/>
       <c r="U2" s="13"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="D3" s="13"/>
+    <row r="3" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>31</v>
+      </c>
       <c r="E3" s="13">
-        <v>-30.5</v>
-      </c>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
+        <f>VLOOKUP(A3,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>4.2</v>
+      </c>
+      <c r="F3" s="13">
+        <v>-29.4</v>
+      </c>
+      <c r="G3" s="13">
+        <v>27.1</v>
+      </c>
+      <c r="H3" s="20"/>
       <c r="I3" s="13">
-        <v>1</v>
-      </c>
-      <c r="J3" s="13">
-        <v>0</v>
-      </c>
-      <c r="K3" s="13"/>
-      <c r="L3" s="20">
-        <v>2.7799999999999998E-4</v>
-      </c>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="13"/>
-      <c r="R3" s="13"/>
-      <c r="S3" s="13"/>
-      <c r="T3" s="13"/>
-      <c r="U3" s="13"/>
+        <v>8.5</v>
+      </c>
+      <c r="M3" s="18"/>
+      <c r="N3" s="16" t="str">
+        <f>VLOOKUP(A3,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>4.1.2.13</v>
+      </c>
+      <c r="S3" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="T3" s="13">
+        <v>0.218</v>
+      </c>
+      <c r="U3" s="13">
+        <v>0.218</v>
+      </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
@@ -6692,9 +6654,7 @@
       <c r="I14" s="13">
         <v>355.79</v>
       </c>
-      <c r="M14" s="18">
-        <v>24.294625983764298</v>
-      </c>
+      <c r="M14" s="18"/>
       <c r="N14" s="16" t="str">
         <f>VLOOKUP(A14,[2]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>4.2.1.11</v>
@@ -6728,9 +6688,7 @@
       <c r="J15" s="13">
         <v>530</v>
       </c>
-      <c r="M15" s="18">
-        <v>-24.294625983764298</v>
-      </c>
+      <c r="M15" s="18"/>
       <c r="N15" s="16" t="str">
         <f>VLOOKUP(A15,[2]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>5.4.2.1</v>
@@ -6765,9 +6723,7 @@
       <c r="J16" s="13">
         <v>654</v>
       </c>
-      <c r="M16" s="18">
-        <v>-27.772223526897601</v>
-      </c>
+      <c r="M16" s="18"/>
       <c r="N16" s="16" t="str">
         <f>VLOOKUP(A16,[2]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>2.7.2.3</v>
@@ -6805,9 +6761,7 @@
       <c r="I17" s="13">
         <v>268</v>
       </c>
-      <c r="M17" s="18">
-        <v>27.772223526897601</v>
-      </c>
+      <c r="M17" s="18"/>
       <c r="N17" s="16" t="str">
         <f>VLOOKUP(A17,[2]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>1.2.1.12</v>
@@ -6823,11 +6777,38 @@
       </c>
     </row>
     <row r="18" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="E18" s="17"/>
+      <c r="A18" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="17">
+        <v>7.5979999999999999</v>
+      </c>
+      <c r="F18" s="13">
+        <v>-24.3</v>
+      </c>
+      <c r="G18" s="13">
+        <v>13.4</v>
+      </c>
+      <c r="J18" s="13">
+        <v>9000</v>
+      </c>
       <c r="M18" s="7"/>
-      <c r="N18" s="16"/>
+      <c r="N18" s="16" t="str">
+        <f>VLOOKUP(A18,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>5.3.1.1</v>
+      </c>
+      <c r="S18" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="T18" s="13">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="U18" s="13">
+        <v>0.16700000000000001</v>
+      </c>
     </row>
     <row r="19" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16"/>
@@ -6894,7 +6875,7 @@
   <dimension ref="A1:U25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD11"/>
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add all reactions till g6p in upper glycolysis
</commit_message>
<xml_diff>
--- a/KineticModel/data/gtoyall.xlsx
+++ b/KineticModel/data/gtoyall.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="128">
   <si>
     <t>Enzymes</t>
   </si>
@@ -429,6 +429,18 @@
   </si>
   <si>
     <t>[c] : g3p &lt;==&gt; 13dpg</t>
+  </si>
+  <si>
+    <t>[c] : fdp --&gt; f6p</t>
+  </si>
+  <si>
+    <t>G6Pt2r</t>
+  </si>
+  <si>
+    <t>G6Pex</t>
+  </si>
+  <si>
+    <t>g6p[c] ---&gt; g6p[e]</t>
   </si>
 </sst>
 </file>
@@ -6099,13 +6111,13 @@
   <dimension ref="A1:U19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="25.5703125" customWidth="1"/>
-    <col min="15" max="15" width="9.140625" customWidth="1"/>
+    <col min="15" max="15" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="18" x14ac:dyDescent="0.35">
@@ -6249,46 +6261,45 @@
         <v>0.218</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+    <row r="4" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="D4" s="13"/>
+      <c r="C4" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>28</v>
+      </c>
       <c r="E4" s="13">
-        <v>-30.5</v>
-      </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
+        <f>VLOOKUP(A4,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>-2.8</v>
+      </c>
+      <c r="F4" s="13">
+        <v>-48.8</v>
+      </c>
+      <c r="G4" s="13">
+        <v>-9.6999999999999993</v>
+      </c>
       <c r="I4" s="13">
-        <v>1</v>
-      </c>
-      <c r="J4" s="13">
+        <v>22</v>
+      </c>
+      <c r="M4" s="18">
         <v>0</v>
       </c>
-      <c r="K4" s="13"/>
-      <c r="L4" s="20">
-        <v>2.7799999999999998E-4</v>
-      </c>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="P4" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q4" s="13"/>
-      <c r="R4" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="S4" s="13"/>
-      <c r="T4" s="13"/>
-      <c r="U4" s="13"/>
+      <c r="N4" s="16" t="str">
+        <f>VLOOKUP(A4,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>3.1.3.11</v>
+      </c>
+      <c r="S4" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="T4" s="13">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="U4" s="13">
+        <v>0.27200000000000002</v>
+      </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
@@ -6325,11 +6336,11 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>106</v>
+        <v>125</v>
       </c>
       <c r="B6" s="13"/>
       <c r="C6" s="13" t="s">
-        <v>107</v>
+        <v>127</v>
       </c>
       <c r="D6" s="13"/>
       <c r="E6" s="13">
@@ -6428,11 +6439,11 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>112</v>
+        <v>126</v>
       </c>
       <c r="B9" s="13"/>
       <c r="C9" s="13" t="s">
-        <v>113</v>
+        <v>87</v>
       </c>
       <c r="D9" s="13"/>
       <c r="E9" s="13">
@@ -6811,12 +6822,43 @@
       </c>
     </row>
     <row r="19" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="H19" s="20"/>
-      <c r="L19" s="20"/>
-      <c r="M19" s="18"/>
-      <c r="N19" s="16"/>
+      <c r="A19" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="13">
+        <v>3.1320000000000001</v>
+      </c>
+      <c r="F19" s="13">
+        <v>-17.100000000000001</v>
+      </c>
+      <c r="G19" s="13">
+        <v>20.6</v>
+      </c>
+      <c r="I19" s="13">
+        <v>120</v>
+      </c>
+      <c r="M19" s="18">
+        <v>11.639423575531699</v>
+      </c>
+      <c r="N19" s="16" t="str">
+        <f>VLOOKUP(A19,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>5.3.1.9</v>
+      </c>
+      <c r="O19" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="S19" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="T19" s="13">
+        <v>3.48</v>
+      </c>
+      <c r="U19" s="13">
+        <v>3.48</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6859,7 +6901,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="B4" s="13">
         <v>0</v>
@@ -6875,7 +6917,7 @@
   <dimension ref="A1:U25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
change acetate concentration and add fdp regulation
</commit_message>
<xml_diff>
--- a/KineticModel/data/gtoyall.xlsx
+++ b/KineticModel/data/gtoyall.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shyam\Documents\Courses\CHE1125Project\IntegratedModels\KineticModel\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shyam\Documents\Courses\CHE1125Project\IntegratedModels\KineticModel\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
     <externalReference r:id="rId10"/>
     <externalReference r:id="rId11"/>
   </externalReferences>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="128">
   <si>
     <t>Enzymes</t>
   </si>
@@ -4451,6 +4451,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -4486,6 +4503,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -6111,13 +6145,15 @@
   <dimension ref="A1:U19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection sqref="A1:U19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="25.5703125" customWidth="1"/>
     <col min="15" max="15" width="17.28515625" customWidth="1"/>
+    <col min="16" max="16" width="13.28515625" customWidth="1"/>
+    <col min="17" max="17" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="18" x14ac:dyDescent="0.35">
@@ -6290,6 +6326,12 @@
       <c r="N4" s="16" t="str">
         <f>VLOOKUP(A4,[2]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>3.1.3.11</v>
+      </c>
+      <c r="P4" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="R4" s="13">
+        <v>0.1</v>
       </c>
       <c r="S4" s="13" t="s">
         <v>29</v>
@@ -6888,7 +6930,7 @@
         <v>94</v>
       </c>
       <c r="B2" s="13">
-        <v>2</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
gtoy5 with hc and he for acetate uptake
</commit_message>
<xml_diff>
--- a/KineticModel/data/gtoyall.xlsx
+++ b/KineticModel/data/gtoyall.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shyam\Documents\Courses\CHE1125Project\IntegratedModels\KineticModel\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shyam\Documents\Courses\CHE1125Project\IntegratedModels\KineticModel\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25590" windowHeight="7875" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25590" windowHeight="7875" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="gtoy1" sheetId="2" r:id="rId1"/>
@@ -20,13 +20,14 @@
     <sheet name="gtoy3C" sheetId="7" r:id="rId6"/>
     <sheet name="gtoy4" sheetId="8" r:id="rId7"/>
     <sheet name="gtoy4C" sheetId="9" r:id="rId8"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId9"/>
+    <sheet name="gtoy5" sheetId="10" r:id="rId9"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId10"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId10"/>
     <externalReference r:id="rId11"/>
+    <externalReference r:id="rId12"/>
   </externalReferences>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="128">
   <si>
     <t>Enzymes</t>
   </si>
@@ -4451,23 +4452,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -4503,23 +4487,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -5093,6 +5060,748 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:XFD14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2">
+        <f>VLOOKUP(A2,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>4.3</v>
+      </c>
+      <c r="F2">
+        <v>-24.3</v>
+      </c>
+      <c r="G2">
+        <v>52.1</v>
+      </c>
+      <c r="I2">
+        <v>280</v>
+      </c>
+      <c r="M2" s="5">
+        <v>-19.215657194822899</v>
+      </c>
+      <c r="N2" s="3" t="str">
+        <f>VLOOKUP(A2,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>2.7.2.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3">
+        <f>VLOOKUP(A3,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>3.8</v>
+      </c>
+      <c r="F3">
+        <v>-20.399999999999999</v>
+      </c>
+      <c r="G3">
+        <v>28.7</v>
+      </c>
+      <c r="I3">
+        <v>120</v>
+      </c>
+      <c r="J3">
+        <v>0.02</v>
+      </c>
+      <c r="M3" s="7">
+        <v>19.215657194822899</v>
+      </c>
+      <c r="N3" s="3" t="str">
+        <f>VLOOKUP(A3,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>2.3.1.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4">
+        <v>-8.3000000000000007</v>
+      </c>
+      <c r="F4">
+        <v>-73</v>
+      </c>
+      <c r="G4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="I4">
+        <v>6.32</v>
+      </c>
+      <c r="M4" s="5">
+        <v>0</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S4" t="s">
+        <v>52</v>
+      </c>
+      <c r="T4">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="U4">
+        <v>0.27600000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5">
+        <v>-31.12</v>
+      </c>
+      <c r="F5">
+        <v>-10.8</v>
+      </c>
+      <c r="G5">
+        <v>65.3</v>
+      </c>
+      <c r="H5" s="6"/>
+      <c r="I5">
+        <v>2540</v>
+      </c>
+      <c r="M5" s="5">
+        <v>-8.5077261088811902</v>
+      </c>
+      <c r="N5" s="3" t="str">
+        <f>VLOOKUP(A5,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>2.7.1.40</v>
+      </c>
+      <c r="O5" t="s">
+        <v>48</v>
+      </c>
+      <c r="S5" t="s">
+        <v>49</v>
+      </c>
+      <c r="T5">
+        <v>0.111</v>
+      </c>
+      <c r="U5">
+        <v>0.111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6">
+        <f>VLOOKUP(A6,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>-0.9</v>
+      </c>
+      <c r="F6">
+        <v>-22.9</v>
+      </c>
+      <c r="G6">
+        <v>14.7</v>
+      </c>
+      <c r="I6">
+        <v>355.79</v>
+      </c>
+      <c r="M6" s="5">
+        <v>24.294625983764298</v>
+      </c>
+      <c r="N6" s="3" t="str">
+        <f>VLOOKUP(A6,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>4.2.1.11</v>
+      </c>
+      <c r="S6" t="s">
+        <v>46</v>
+      </c>
+      <c r="T6">
+        <v>2.67</v>
+      </c>
+      <c r="U6">
+        <v>2.67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7">
+        <v>6.2290000000000001</v>
+      </c>
+      <c r="F7">
+        <v>-23.1</v>
+      </c>
+      <c r="G7">
+        <v>14.6</v>
+      </c>
+      <c r="J7">
+        <v>530</v>
+      </c>
+      <c r="M7" s="5">
+        <v>-24.294625983764298</v>
+      </c>
+      <c r="N7" s="3" t="str">
+        <f>VLOOKUP(A7,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>5.4.2.1</v>
+      </c>
+      <c r="S7" t="s">
+        <v>43</v>
+      </c>
+      <c r="T7">
+        <v>2.67</v>
+      </c>
+      <c r="U7">
+        <v>2.67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8">
+        <v>-10.51</v>
+      </c>
+      <c r="F8">
+        <v>-19.2</v>
+      </c>
+      <c r="G8">
+        <v>56.1</v>
+      </c>
+      <c r="H8" s="6"/>
+      <c r="J8">
+        <v>654</v>
+      </c>
+      <c r="M8" s="5">
+        <v>-27.772223526897601</v>
+      </c>
+      <c r="N8" s="3" t="str">
+        <f>VLOOKUP(A8,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>2.7.2.3</v>
+      </c>
+      <c r="S8" t="s">
+        <v>40</v>
+      </c>
+      <c r="T8">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="U8">
+        <v>0.39900000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9">
+        <f>VLOOKUP(A9,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>-0.1</v>
+      </c>
+      <c r="F9">
+        <v>-12.8</v>
+      </c>
+      <c r="G9">
+        <v>62.6</v>
+      </c>
+      <c r="I9">
+        <v>268</v>
+      </c>
+      <c r="M9" s="5">
+        <v>27.772223526897601</v>
+      </c>
+      <c r="N9" s="3" t="str">
+        <f>VLOOKUP(A9,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>1.2.1.12</v>
+      </c>
+      <c r="S9" t="s">
+        <v>38</v>
+      </c>
+      <c r="T9">
+        <v>2.13</v>
+      </c>
+      <c r="U9">
+        <v>2.13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="4">
+        <v>7.5979999999999999</v>
+      </c>
+      <c r="F10">
+        <v>-24.3</v>
+      </c>
+      <c r="G10">
+        <v>13.4</v>
+      </c>
+      <c r="J10">
+        <v>9000</v>
+      </c>
+      <c r="M10" s="7">
+        <v>-11.639423575531699</v>
+      </c>
+      <c r="N10" s="3" t="str">
+        <f>VLOOKUP(A10,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>5.3.1.1</v>
+      </c>
+      <c r="S10" t="s">
+        <v>35</v>
+      </c>
+      <c r="T10">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="U10">
+        <v>0.16700000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11">
+        <f>VLOOKUP(A11,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>4.2</v>
+      </c>
+      <c r="F11">
+        <v>-29.4</v>
+      </c>
+      <c r="G11">
+        <v>27.1</v>
+      </c>
+      <c r="H11" s="6"/>
+      <c r="I11">
+        <v>8.5</v>
+      </c>
+      <c r="M11" s="5">
+        <v>11.639423575531699</v>
+      </c>
+      <c r="N11" s="3" t="str">
+        <f>VLOOKUP(A11,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>4.1.2.13</v>
+      </c>
+      <c r="S11" t="s">
+        <v>32</v>
+      </c>
+      <c r="T11">
+        <v>0.218</v>
+      </c>
+      <c r="U11">
+        <v>0.218</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12">
+        <f>VLOOKUP(A12,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>-2.8</v>
+      </c>
+      <c r="F12">
+        <v>-48.8</v>
+      </c>
+      <c r="G12">
+        <v>-9.6999999999999993</v>
+      </c>
+      <c r="I12">
+        <v>22</v>
+      </c>
+      <c r="M12" s="5">
+        <v>0</v>
+      </c>
+      <c r="N12" s="3" t="str">
+        <f>VLOOKUP(A12,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>3.1.3.11</v>
+      </c>
+      <c r="S12" t="s">
+        <v>29</v>
+      </c>
+      <c r="T12">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="U12">
+        <v>0.27200000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13">
+        <v>3.1320000000000001</v>
+      </c>
+      <c r="F13">
+        <v>-17.100000000000001</v>
+      </c>
+      <c r="G13">
+        <v>20.6</v>
+      </c>
+      <c r="I13">
+        <v>120</v>
+      </c>
+      <c r="M13" s="5">
+        <v>11.639423575531699</v>
+      </c>
+      <c r="N13" s="3" t="str">
+        <f>VLOOKUP(A13,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>5.3.1.9</v>
+      </c>
+      <c r="O13" t="s">
+        <v>23</v>
+      </c>
+      <c r="S13" t="s">
+        <v>24</v>
+      </c>
+      <c r="T13">
+        <v>3.48</v>
+      </c>
+      <c r="U13">
+        <v>3.48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14">
+        <f>VLOOKUP(A14,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="I14" s="4">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="M14" s="5">
+        <v>-19.215657194822899</v>
+      </c>
+      <c r="N14" s="3"/>
+      <c r="O14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="9"/>
+      <c r="C15" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="I15" s="4">
+        <v>2540</v>
+      </c>
+      <c r="J15">
+        <v>2540</v>
+      </c>
+      <c r="M15" s="5">
+        <v>-8.5077261088811902</v>
+      </c>
+      <c r="N15" s="3"/>
+      <c r="O15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="9"/>
+      <c r="C16" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="E16">
+        <f>VLOOKUP(A16,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="I16" s="6">
+        <v>100</v>
+      </c>
+      <c r="J16" s="6">
+        <v>100</v>
+      </c>
+      <c r="M16" s="5">
+        <v>8.5514960440672301</v>
+      </c>
+      <c r="N16" s="3"/>
+      <c r="O16" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E17">
+        <f>VLOOKUP(A17,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>2</v>
+      </c>
+      <c r="M17" s="5">
+        <v>-13.3040694607334</v>
+      </c>
+      <c r="N17" s="3"/>
+      <c r="O17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="M19" s="5">
+        <v>19.215657194822899</v>
+      </c>
+      <c r="N19" s="3"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="M20" s="5">
+        <v>63.607356573910501</v>
+      </c>
+      <c r="N20" s="3"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="M21" s="5">
+        <v>13.304069460733899</v>
+      </c>
+      <c r="N21" s="3"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="M22" s="5">
+        <v>-8.5514960440672301</v>
+      </c>
+      <c r="N22" s="3"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="M23" s="5">
+        <v>0</v>
+      </c>
+      <c r="N23" s="3"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="M24" s="5">
+        <v>-20</v>
+      </c>
+      <c r="N24" s="3"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C25" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
@@ -6144,13 +6853,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:U19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="25.5703125" customWidth="1"/>
+    <col min="13" max="13" width="9.85546875" customWidth="1"/>
     <col min="15" max="15" width="17.28515625" customWidth="1"/>
     <col min="16" max="16" width="13.28515625" customWidth="1"/>
     <col min="17" max="17" width="13.5703125" customWidth="1"/>
@@ -6956,742 +7666,825 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U25"/>
+  <dimension ref="A1:U19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="39.7109375" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" customWidth="1"/>
+    <col min="3" max="3" width="28.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="13">
+        <f>VLOOKUP(A2,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="I2" s="17">
+        <v>1</v>
+      </c>
+      <c r="J2" s="13">
+        <v>1</v>
+      </c>
+      <c r="M2" s="18">
+        <v>-19.215657194822899</v>
+      </c>
+      <c r="N2" s="16"/>
+      <c r="O2" s="13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="13"/>
+      <c r="C3" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13">
+        <f>VLOOKUP(A3,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>4.2</v>
+      </c>
+      <c r="F3" s="13">
+        <v>-29.4</v>
+      </c>
+      <c r="G3" s="13">
+        <v>27.1</v>
+      </c>
+      <c r="H3" s="20"/>
+      <c r="I3" s="13">
+        <v>8.5</v>
+      </c>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="16" t="str">
+        <f>VLOOKUP(A3,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>4.1.2.13</v>
+      </c>
+      <c r="O3" s="13"/>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="13"/>
+      <c r="R3" s="13"/>
+      <c r="S3" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="T3" s="13">
+        <v>0.218</v>
+      </c>
+      <c r="U3" s="13">
+        <v>0.218</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="C4" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="13">
+        <f>VLOOKUP(A4,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>-2.8</v>
+      </c>
+      <c r="F4" s="13">
+        <v>-48.8</v>
+      </c>
+      <c r="G4" s="13">
+        <v>-9.6999999999999993</v>
+      </c>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13">
+        <v>22</v>
+      </c>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="18">
+        <v>0</v>
+      </c>
+      <c r="N4" s="16" t="str">
+        <f>VLOOKUP(A4,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>3.1.3.11</v>
+      </c>
+      <c r="O4" s="13"/>
+      <c r="P4" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q4" s="13"/>
+      <c r="R4" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="S4" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="T4" s="13">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="U4" s="13">
+        <v>0.27200000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13">
+        <v>0</v>
+      </c>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13">
+        <v>1</v>
+      </c>
+      <c r="J5" s="13">
+        <v>1</v>
+      </c>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="13"/>
+      <c r="R5" s="13"/>
+      <c r="S5" s="13"/>
+      <c r="T5" s="13"/>
+      <c r="U5" s="13"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13">
+        <v>0</v>
+      </c>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13">
+        <v>1</v>
+      </c>
+      <c r="J6" s="13">
+        <v>0</v>
+      </c>
+      <c r="K6" s="13"/>
+      <c r="L6" s="20">
+        <v>2.7799999999999998E-4</v>
+      </c>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="13"/>
+      <c r="S6" s="13"/>
+      <c r="T6" s="13"/>
+      <c r="U6" s="13"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13">
+        <v>0</v>
+      </c>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13">
+        <v>1</v>
+      </c>
+      <c r="J7" s="13">
+        <v>0</v>
+      </c>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="13"/>
+      <c r="R7" s="13"/>
+      <c r="S7" s="13"/>
+      <c r="T7" s="13"/>
+      <c r="U7" s="13"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13">
+        <v>0</v>
+      </c>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13">
+        <v>1</v>
+      </c>
+      <c r="J8" s="13">
+        <v>1</v>
+      </c>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="13"/>
+      <c r="R8" s="13"/>
+      <c r="S8" s="13"/>
+      <c r="T8" s="13"/>
+      <c r="U8" s="13"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13">
+        <v>0</v>
+      </c>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13">
+        <v>1</v>
+      </c>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+      <c r="R9" s="13"/>
+      <c r="S9" s="13"/>
+      <c r="T9" s="13"/>
+      <c r="U9" s="13"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="E2">
-        <f>VLOOKUP(A2,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13">
+        <f>VLOOKUP(A10,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
         <v>4.3</v>
       </c>
-      <c r="F2">
+      <c r="F10" s="13">
         <v>-24.3</v>
       </c>
-      <c r="G2">
+      <c r="G10" s="13">
         <v>52.1</v>
       </c>
-      <c r="I2">
+      <c r="H10" s="13"/>
+      <c r="I10" s="13">
         <v>280</v>
       </c>
-      <c r="M2" s="5">
-        <v>-19.215657194822899</v>
-      </c>
-      <c r="N2" s="3" t="str">
-        <f>VLOOKUP(A2,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="16" t="str">
+        <f>VLOOKUP(A10,[2]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>2.7.2.1</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="O10" s="13"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="13"/>
+      <c r="R10" s="13"/>
+      <c r="S10" s="13"/>
+      <c r="T10" s="13"/>
+      <c r="U10" s="13"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="B11" s="13"/>
+      <c r="C11" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="D11" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="E3">
-        <f>VLOOKUP(A3,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+      <c r="E11" s="13">
+        <f>VLOOKUP(A11,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
         <v>3.8</v>
       </c>
-      <c r="F3">
+      <c r="F11" s="13">
         <v>-20.399999999999999</v>
       </c>
-      <c r="G3">
+      <c r="G11" s="13">
         <v>28.7</v>
       </c>
-      <c r="I3">
+      <c r="H11" s="13"/>
+      <c r="I11" s="13">
         <v>120</v>
       </c>
-      <c r="J3">
+      <c r="J11" s="13">
         <v>0.02</v>
       </c>
-      <c r="M3" s="7">
-        <v>19.215657194822899</v>
-      </c>
-      <c r="N3" s="3" t="str">
-        <f>VLOOKUP(A3,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="16" t="str">
+        <f>VLOOKUP(A11,[2]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>2.3.1.8</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="O11" s="13"/>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="13"/>
+      <c r="R11" s="13"/>
+      <c r="S11" s="13"/>
+      <c r="T11" s="13"/>
+      <c r="U11" s="13"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="B12" s="13"/>
+      <c r="C12" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D12" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="E4">
+      <c r="E12" s="13">
         <v>-8.3000000000000007</v>
       </c>
-      <c r="F4">
+      <c r="F12" s="13">
         <v>-73</v>
       </c>
-      <c r="G4">
+      <c r="G12" s="13">
         <v>2.2999999999999998</v>
       </c>
-      <c r="I4">
+      <c r="H12" s="13"/>
+      <c r="I12" s="13">
         <v>6.32</v>
       </c>
-      <c r="M4" s="5">
+      <c r="J12" s="13">
         <v>0</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="S4" t="s">
+      <c r="O12" s="13"/>
+      <c r="P12" s="13"/>
+      <c r="Q12" s="13"/>
+      <c r="R12" s="13"/>
+      <c r="S12" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="T4">
+      <c r="T12" s="13">
         <v>0.27600000000000002</v>
       </c>
-      <c r="U4">
+      <c r="U12" s="13">
         <v>0.27600000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="B13" s="13"/>
+      <c r="C13" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="D13" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E5">
+      <c r="E13" s="13">
         <v>-31.12</v>
       </c>
-      <c r="F5">
+      <c r="F13" s="13">
         <v>-10.8</v>
       </c>
-      <c r="G5">
+      <c r="G13" s="13">
         <v>65.3</v>
       </c>
-      <c r="H5" s="6"/>
-      <c r="I5">
+      <c r="H13" s="20"/>
+      <c r="I13" s="13">
         <v>2540</v>
       </c>
-      <c r="M5" s="5">
-        <v>-8.5077261088811902</v>
-      </c>
-      <c r="N5" s="3" t="str">
-        <f>VLOOKUP(A5,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="18"/>
+      <c r="N13" s="16" t="str">
+        <f>VLOOKUP(A13,[2]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>2.7.1.40</v>
       </c>
-      <c r="O5" t="s">
+      <c r="O13" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="S5" t="s">
+      <c r="P13" s="13"/>
+      <c r="Q13" s="13"/>
+      <c r="R13" s="13"/>
+      <c r="S13" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="T5">
+      <c r="T13" s="13">
         <v>0.111</v>
       </c>
-      <c r="U5">
+      <c r="U13" s="13">
         <v>0.111</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6">
-        <f>VLOOKUP(A6,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+      <c r="B14" s="13"/>
+      <c r="C14" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13">
+        <f>VLOOKUP(A14,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
         <v>-0.9</v>
       </c>
-      <c r="F6">
+      <c r="F14" s="13">
         <v>-22.9</v>
       </c>
-      <c r="G6">
+      <c r="G14" s="13">
         <v>14.7</v>
       </c>
-      <c r="I6">
+      <c r="H14" s="13"/>
+      <c r="I14" s="13">
         <v>355.79</v>
       </c>
-      <c r="M6" s="5">
-        <v>24.294625983764298</v>
-      </c>
-      <c r="N6" s="3" t="str">
-        <f>VLOOKUP(A6,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="16" t="str">
+        <f>VLOOKUP(A14,[2]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>4.2.1.11</v>
       </c>
-      <c r="S6" t="s">
+      <c r="O14" s="13"/>
+      <c r="P14" s="13"/>
+      <c r="Q14" s="13"/>
+      <c r="R14" s="13"/>
+      <c r="S14" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="T6">
+      <c r="T14" s="13">
         <v>2.67</v>
       </c>
-      <c r="U6">
+      <c r="U14" s="13">
         <v>2.67</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="B15" s="13"/>
+      <c r="C15" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="E7">
+      <c r="D15" s="13"/>
+      <c r="E15" s="13">
         <v>6.2290000000000001</v>
       </c>
-      <c r="F7">
+      <c r="F15" s="13">
         <v>-23.1</v>
       </c>
-      <c r="G7">
+      <c r="G15" s="13">
         <v>14.6</v>
       </c>
-      <c r="J7">
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13">
         <v>530</v>
       </c>
-      <c r="M7" s="5">
-        <v>-24.294625983764298</v>
-      </c>
-      <c r="N7" s="3" t="str">
-        <f>VLOOKUP(A7,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="16" t="str">
+        <f>VLOOKUP(A15,[2]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>5.4.2.1</v>
       </c>
-      <c r="S7" t="s">
+      <c r="O15" s="13"/>
+      <c r="P15" s="13"/>
+      <c r="Q15" s="13"/>
+      <c r="R15" s="13"/>
+      <c r="S15" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="T7">
+      <c r="T15" s="13">
         <v>2.67</v>
       </c>
-      <c r="U7">
+      <c r="U15" s="13">
         <v>2.67</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="B16" s="13"/>
+      <c r="C16" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="E8">
+      <c r="D16" s="13"/>
+      <c r="E16" s="13">
         <v>-10.51</v>
       </c>
-      <c r="F8">
+      <c r="F16" s="13">
         <v>-19.2</v>
       </c>
-      <c r="G8">
+      <c r="G16" s="13">
         <v>56.1</v>
       </c>
-      <c r="H8" s="6"/>
-      <c r="J8">
+      <c r="H16" s="20"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13">
         <v>654</v>
       </c>
-      <c r="M8" s="5">
-        <v>-27.772223526897601</v>
-      </c>
-      <c r="N8" s="3" t="str">
-        <f>VLOOKUP(A8,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="18"/>
+      <c r="N16" s="16" t="str">
+        <f>VLOOKUP(A16,[2]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>2.7.2.3</v>
       </c>
-      <c r="S8" t="s">
+      <c r="O16" s="13"/>
+      <c r="P16" s="13"/>
+      <c r="Q16" s="13"/>
+      <c r="R16" s="13"/>
+      <c r="S16" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="T8">
+      <c r="T16" s="13">
         <v>0.39900000000000002</v>
       </c>
-      <c r="U8">
+      <c r="U16" s="13">
         <v>0.39900000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="B17" s="13"/>
+      <c r="C17" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="D17" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E9">
-        <f>VLOOKUP(A9,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+      <c r="E17" s="13">
+        <f>VLOOKUP(A17,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
         <v>-0.1</v>
       </c>
-      <c r="F9">
+      <c r="F17" s="13">
         <v>-12.8</v>
       </c>
-      <c r="G9">
+      <c r="G17" s="13">
         <v>62.6</v>
       </c>
-      <c r="I9">
+      <c r="H17" s="13"/>
+      <c r="I17" s="13">
         <v>268</v>
       </c>
-      <c r="M9" s="5">
-        <v>27.772223526897601</v>
-      </c>
-      <c r="N9" s="3" t="str">
-        <f>VLOOKUP(A9,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="18"/>
+      <c r="N17" s="16" t="str">
+        <f>VLOOKUP(A17,[2]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>1.2.1.12</v>
       </c>
-      <c r="S9" t="s">
+      <c r="O17" s="13"/>
+      <c r="P17" s="13"/>
+      <c r="Q17" s="13"/>
+      <c r="R17" s="13"/>
+      <c r="S17" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="T9">
+      <c r="T17" s="13">
         <v>2.13</v>
       </c>
-      <c r="U9">
+      <c r="U17" s="13">
         <v>2.13</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="B18" s="13"/>
+      <c r="C18" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="4">
+      <c r="D18" s="13"/>
+      <c r="E18" s="17">
         <v>7.5979999999999999</v>
       </c>
-      <c r="F10">
+      <c r="F18" s="13">
         <v>-24.3</v>
       </c>
-      <c r="G10">
+      <c r="G18" s="13">
         <v>13.4</v>
       </c>
-      <c r="J10">
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13">
         <v>9000</v>
       </c>
-      <c r="M10" s="7">
-        <v>-11.639423575531699</v>
-      </c>
-      <c r="N10" s="3" t="str">
-        <f>VLOOKUP(A10,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="16" t="str">
+        <f>VLOOKUP(A18,[2]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>5.3.1.1</v>
       </c>
-      <c r="S10" t="s">
+      <c r="O18" s="13"/>
+      <c r="P18" s="13"/>
+      <c r="Q18" s="13"/>
+      <c r="R18" s="13"/>
+      <c r="S18" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="T10">
+      <c r="T18" s="13">
         <v>0.16700000000000001</v>
       </c>
-      <c r="U10">
+      <c r="U18" s="13">
         <v>0.16700000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11">
-        <f>VLOOKUP(A11,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
-        <v>4.2</v>
-      </c>
-      <c r="F11">
-        <v>-29.4</v>
-      </c>
-      <c r="G11">
-        <v>27.1</v>
-      </c>
-      <c r="H11" s="6"/>
-      <c r="I11">
-        <v>8.5</v>
-      </c>
-      <c r="M11" s="5">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="13"/>
+      <c r="C19" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13">
+        <v>3.1320000000000001</v>
+      </c>
+      <c r="F19" s="13">
+        <v>-17.100000000000001</v>
+      </c>
+      <c r="G19" s="13">
+        <v>20.6</v>
+      </c>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13">
+        <v>120</v>
+      </c>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="18">
         <v>11.639423575531699</v>
       </c>
-      <c r="N11" s="3" t="str">
-        <f>VLOOKUP(A11,[2]reactions!$A$1:$E$96,5,FALSE)</f>
-        <v>4.1.2.13</v>
-      </c>
-      <c r="S11" t="s">
-        <v>32</v>
-      </c>
-      <c r="T11">
-        <v>0.218</v>
-      </c>
-      <c r="U11">
-        <v>0.218</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12">
-        <f>VLOOKUP(A12,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
-        <v>-2.8</v>
-      </c>
-      <c r="F12">
-        <v>-48.8</v>
-      </c>
-      <c r="G12">
-        <v>-9.6999999999999993</v>
-      </c>
-      <c r="I12">
-        <v>22</v>
-      </c>
-      <c r="M12" s="5">
-        <v>0</v>
-      </c>
-      <c r="N12" s="3" t="str">
-        <f>VLOOKUP(A12,[2]reactions!$A$1:$E$96,5,FALSE)</f>
-        <v>3.1.3.11</v>
-      </c>
-      <c r="S12" t="s">
-        <v>29</v>
-      </c>
-      <c r="T12">
-        <v>0.27200000000000002</v>
-      </c>
-      <c r="U12">
-        <v>0.27200000000000002</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13">
-        <v>3.1320000000000001</v>
-      </c>
-      <c r="F13">
-        <v>-17.100000000000001</v>
-      </c>
-      <c r="G13">
-        <v>20.6</v>
-      </c>
-      <c r="I13">
-        <v>120</v>
-      </c>
-      <c r="M13" s="5">
-        <v>11.639423575531699</v>
-      </c>
-      <c r="N13" s="3" t="str">
-        <f>VLOOKUP(A13,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+      <c r="N19" s="16" t="str">
+        <f>VLOOKUP(A19,[2]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>5.3.1.9</v>
       </c>
-      <c r="O13" t="s">
+      <c r="O19" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="S13" t="s">
+      <c r="P19" s="13"/>
+      <c r="Q19" s="13"/>
+      <c r="R19" s="13"/>
+      <c r="S19" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="T13">
+      <c r="T19" s="13">
         <v>3.48</v>
       </c>
-      <c r="U13">
+      <c r="U19" s="13">
         <v>3.48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="D14" t="s">
-        <v>65</v>
-      </c>
-      <c r="E14">
-        <f>VLOOKUP(A14,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="I14" s="4">
-        <v>1</v>
-      </c>
-      <c r="J14">
-        <v>1</v>
-      </c>
-      <c r="M14" s="5">
-        <v>-19.215657194822899</v>
-      </c>
-      <c r="N14" s="3"/>
-      <c r="O14" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="D15" t="s">
-        <v>65</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="I15" s="4">
-        <v>2540</v>
-      </c>
-      <c r="J15">
-        <v>2540</v>
-      </c>
-      <c r="M15" s="5">
-        <v>-8.5077261088811902</v>
-      </c>
-      <c r="N15" s="3"/>
-      <c r="O15" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="E16">
-        <f>VLOOKUP(A16,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="I16" s="6">
-        <v>100</v>
-      </c>
-      <c r="J16" s="6">
-        <v>100</v>
-      </c>
-      <c r="M16" s="5">
-        <v>8.5514960440672301</v>
-      </c>
-      <c r="N16" s="3"/>
-      <c r="O16" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="E17">
-        <f>VLOOKUP(A17,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <v>1</v>
-      </c>
-      <c r="J17">
-        <v>2</v>
-      </c>
-      <c r="M17" s="5">
-        <v>-13.3040694607334</v>
-      </c>
-      <c r="N17" s="3"/>
-      <c r="O17" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="M19" s="5">
-        <v>19.215657194822899</v>
-      </c>
-      <c r="N19" s="3"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="M20" s="5">
-        <v>63.607356573910501</v>
-      </c>
-      <c r="N20" s="3"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="M21" s="5">
-        <v>13.304069460733899</v>
-      </c>
-      <c r="N21" s="3"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="M22" s="5">
-        <v>-8.5514960440672301</v>
-      </c>
-      <c r="N22" s="3"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="M23" s="5">
-        <v>0</v>
-      </c>
-      <c r="N23" s="3"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="M24" s="5">
-        <v>-20</v>
-      </c>
-      <c r="N24" s="3"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C25" s="12" t="s">
-        <v>96</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new model file with hc and he
</commit_message>
<xml_diff>
--- a/KineticModel/data/gtoyall.xlsx
+++ b/KineticModel/data/gtoyall.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shyam\Documents\Courses\CHE1125Project\IntegratedModels\KineticModel\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shyam\Documents\Courses\CHE1125Project\IntegratedModels\KineticModel\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,13 +21,14 @@
     <sheet name="gtoy4" sheetId="8" r:id="rId7"/>
     <sheet name="gtoy4C" sheetId="9" r:id="rId8"/>
     <sheet name="gtoy5" sheetId="10" r:id="rId9"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId10"/>
+    <sheet name="gtoy5C" sheetId="11" r:id="rId10"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId11"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId11"/>
     <externalReference r:id="rId12"/>
+    <externalReference r:id="rId13"/>
   </externalReferences>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="133">
   <si>
     <t>Enzymes</t>
   </si>
@@ -442,6 +443,21 @@
   </si>
   <si>
     <t>g6p[c] ---&gt; g6p[e]</t>
+  </si>
+  <si>
+    <t>g6p[c] + h[c] ---&gt; g6p[e] + h[e]</t>
+  </si>
+  <si>
+    <t>Ht2r</t>
+  </si>
+  <si>
+    <t>h[e] &lt;==&gt; h[c]</t>
+  </si>
+  <si>
+    <t>1,1</t>
+  </si>
+  <si>
+    <t>1e-2,1,1e-5,1</t>
   </si>
 </sst>
 </file>
@@ -545,7 +561,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -568,6 +584,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -4452,6 +4469,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -4487,6 +4521,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -5062,10 +5113,57 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" s="13">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD14"/>
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6854,7 +6952,7 @@
   <dimension ref="A1:U19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:U19"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7661,20 +7759,22 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U19"/>
+  <dimension ref="A1:U21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection sqref="A1:U21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="28.85546875" customWidth="1"/>
+    <col min="15" max="15" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="18" x14ac:dyDescent="0.35">
@@ -7743,9 +7843,10 @@
       </c>
     </row>
     <row r="2" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="8" t="s">
         <v>63</v>
       </c>
+      <c r="B2" s="9"/>
       <c r="C2" s="8" t="s">
         <v>64</v>
       </c>
@@ -7762,12 +7863,15 @@
       <c r="J2" s="13">
         <v>1</v>
       </c>
+      <c r="L2" s="20">
+        <v>1E-3</v>
+      </c>
       <c r="M2" s="18">
         <v>-19.215657194822899</v>
       </c>
       <c r="N2" s="16"/>
       <c r="O2" s="13" t="s">
-        <v>66</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
@@ -7869,11 +7973,11 @@
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="22" t="s">
         <v>119</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13" t="s">
+      <c r="B5" s="22"/>
+      <c r="C5" s="22" t="s">
         <v>77</v>
       </c>
       <c r="D5" s="13"/>
@@ -7902,12 +8006,12 @@
       <c r="U5" s="13"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13" t="s">
-        <v>127</v>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9" t="s">
+        <v>128</v>
       </c>
       <c r="D6" s="13"/>
       <c r="E6" s="13">
@@ -7924,7 +8028,7 @@
       </c>
       <c r="K6" s="13"/>
       <c r="L6" s="20">
-        <v>2.7799999999999998E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="M6" s="13"/>
       <c r="N6" s="13"/>
@@ -7936,47 +8040,43 @@
       <c r="T6" s="13"/>
       <c r="U6" s="13"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+    <row r="7" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="D7" s="13"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>65</v>
+      </c>
       <c r="E7" s="13">
         <v>0</v>
       </c>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13">
-        <v>1</v>
+      <c r="I7" s="17">
+        <v>2540</v>
       </c>
       <c r="J7" s="13">
-        <v>0</v>
-      </c>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
+        <v>2540</v>
+      </c>
+      <c r="L7" s="20">
+        <v>1E-3</v>
+      </c>
+      <c r="M7" s="18">
+        <v>-8.5077261088811902</v>
+      </c>
+      <c r="N7" s="16"/>
       <c r="O7" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="13"/>
-      <c r="R7" s="13"/>
-      <c r="S7" s="13"/>
-      <c r="T7" s="13"/>
-      <c r="U7" s="13"/>
+        <v>69</v>
+      </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="22" t="s">
         <v>122</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13" t="s">
+      <c r="B8" s="22"/>
+      <c r="C8" s="22" t="s">
         <v>85</v>
       </c>
       <c r="D8" s="13"/>
@@ -8005,11 +8105,11 @@
       <c r="U8" s="13"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13" t="s">
+      <c r="B9" s="22"/>
+      <c r="C9" s="22" t="s">
         <v>87</v>
       </c>
       <c r="D9" s="13"/>
@@ -8484,7 +8584,55 @@
         <v>3.48</v>
       </c>
     </row>
+    <row r="20" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" s="22"/>
+      <c r="C20" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="E20" s="13">
+        <v>0</v>
+      </c>
+      <c r="M20" s="18">
+        <v>63.607356573910501</v>
+      </c>
+      <c r="N20" s="16"/>
+    </row>
+    <row r="21" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B21" s="9"/>
+      <c r="C21" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="E21" s="13">
+        <v>0</v>
+      </c>
+      <c r="I21" s="17">
+        <v>1</v>
+      </c>
+      <c r="J21" s="13">
+        <v>1</v>
+      </c>
+      <c r="L21" s="20">
+        <v>2.7799999999999998E-4</v>
+      </c>
+      <c r="M21" s="18">
+        <v>-19.215657194822899</v>
+      </c>
+      <c r="N21" s="16"/>
+      <c r="O21" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add pi[c] and pi[e] to model
</commit_message>
<xml_diff>
--- a/KineticModel/data/gtoyall.xlsx
+++ b/KineticModel/data/gtoyall.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25590" windowHeight="7875" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25590" windowHeight="7875" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="gtoy1" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="131">
   <si>
     <t>Enzymes</t>
   </si>
@@ -445,19 +445,13 @@
     <t>g6p[c] ---&gt; g6p[e]</t>
   </si>
   <si>
-    <t>g6p[c] + h[c] ---&gt; g6p[e] + h[e]</t>
-  </si>
-  <si>
-    <t>Ht2r</t>
-  </si>
-  <si>
-    <t>h[e] &lt;==&gt; h[c]</t>
-  </si>
-  <si>
-    <t>1,1</t>
-  </si>
-  <si>
     <t>1e-2,1,1e-5,1</t>
+  </si>
+  <si>
+    <t>1,1e-3,1,1e-3</t>
+  </si>
+  <si>
+    <t>1,0.1,1,0.1</t>
   </si>
 </sst>
 </file>
@@ -4693,7 +4687,7 @@
   <dimension ref="A1:U21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5113,10 +5107,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5151,6 +5145,14 @@
       </c>
       <c r="B4" s="13">
         <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" s="20">
+        <v>1E-4</v>
       </c>
     </row>
   </sheetData>
@@ -5163,7 +5165,7 @@
   <dimension ref="A1:U25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD15"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5905,7 +5907,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B5"/>
+      <selection activeCell="A4" sqref="A4:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6412,7 +6414,7 @@
   <dimension ref="A1:U13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:U13"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7765,15 +7767,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U21"/>
+  <dimension ref="A1:U22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:U21"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:U22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="28.85546875" customWidth="1"/>
+    <col min="3" max="3" width="33.28515625" customWidth="1"/>
     <col min="15" max="15" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7863,15 +7865,13 @@
       <c r="J2" s="13">
         <v>1</v>
       </c>
-      <c r="L2" s="20">
-        <v>1E-3</v>
-      </c>
+      <c r="L2" s="20"/>
       <c r="M2" s="18">
         <v>-19.215657194822899</v>
       </c>
       <c r="N2" s="16"/>
       <c r="O2" s="13" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
@@ -8011,7 +8011,7 @@
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D6" s="13"/>
       <c r="E6" s="13">
@@ -8027,9 +8027,7 @@
         <v>0</v>
       </c>
       <c r="K6" s="13"/>
-      <c r="L6" s="20">
-        <v>1E-3</v>
-      </c>
+      <c r="L6" s="20"/>
       <c r="M6" s="13"/>
       <c r="N6" s="13"/>
       <c r="O6" s="13"/>
@@ -8068,7 +8066,7 @@
       </c>
       <c r="N7" s="16"/>
       <c r="O7" s="13" t="s">
-        <v>69</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
@@ -8180,7 +8178,7 @@
       </c>
       <c r="B11" s="13"/>
       <c r="C11" s="16" t="s">
-        <v>117</v>
+        <v>54</v>
       </c>
       <c r="D11" s="13" t="s">
         <v>55</v>
@@ -8270,7 +8268,7 @@
       </c>
       <c r="B13" s="13"/>
       <c r="C13" s="16" t="s">
-        <v>118</v>
+        <v>60</v>
       </c>
       <c r="D13" s="13" t="s">
         <v>25</v>
@@ -8602,34 +8600,45 @@
     </row>
     <row r="21" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>129</v>
+        <v>70</v>
       </c>
       <c r="B21" s="9"/>
       <c r="C21" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="E21" s="13">
+        <f>VLOOKUP(A21,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="I21" s="17">
-        <v>1</v>
-      </c>
-      <c r="J21" s="13">
-        <v>1</v>
-      </c>
-      <c r="L21" s="20">
-        <v>2.7799999999999998E-4</v>
+      <c r="I21" s="20">
+        <v>100</v>
+      </c>
+      <c r="J21" s="20">
+        <v>100</v>
       </c>
       <c r="M21" s="18">
-        <v>-19.215657194822899</v>
+        <v>8.5514960440672301</v>
       </c>
       <c r="N21" s="16"/>
-      <c r="O21" s="13" t="s">
-        <v>131</v>
-      </c>
+      <c r="O21" s="20" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B22" s="22"/>
+      <c r="C22" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E22" s="13">
+        <v>0</v>
+      </c>
+      <c r="M22" s="18">
+        <v>-8.5514960440672301</v>
+      </c>
+      <c r="N22" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add necessary hc and he in the small network with additional hc <--> he rxn
</commit_message>
<xml_diff>
--- a/KineticModel/data/gtoyall.xlsx
+++ b/KineticModel/data/gtoyall.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17127"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="135">
   <si>
     <t>Enzymes</t>
   </si>
@@ -448,10 +448,22 @@
     <t>1e-2,1,1e-5,1</t>
   </si>
   <si>
-    <t>1,1e-3,1,1e-3</t>
-  </si>
-  <si>
     <t>1,0.1,1,0.1</t>
+  </si>
+  <si>
+    <t>h[e] &lt;==&gt; h[c]</t>
+  </si>
+  <si>
+    <t>Ht2r</t>
+  </si>
+  <si>
+    <t>1,1</t>
+  </si>
+  <si>
+    <t>[c] : g3p &lt;==&gt; 13dpg + h</t>
+  </si>
+  <si>
+    <t>h[e]</t>
   </si>
 </sst>
 </file>
@@ -555,7 +567,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -579,6 +591,8 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -5107,10 +5121,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B5"/>
+      <selection sqref="A1:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5148,10 +5162,18 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="B5" s="20">
+      <c r="A5" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="B5" s="24">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="24">
         <v>1E-4</v>
       </c>
     </row>
@@ -7770,7 +7792,7 @@
   <dimension ref="A1:U22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:U22"/>
+      <selection sqref="A1:U21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8066,7 +8088,7 @@
       </c>
       <c r="N7" s="16"/>
       <c r="O7" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
@@ -8178,7 +8200,7 @@
       </c>
       <c r="B11" s="13"/>
       <c r="C11" s="16" t="s">
-        <v>54</v>
+        <v>117</v>
       </c>
       <c r="D11" s="13" t="s">
         <v>55</v>
@@ -8449,7 +8471,7 @@
       </c>
       <c r="B17" s="13"/>
       <c r="C17" s="16" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="D17" s="13" t="s">
         <v>37</v>
@@ -8600,14 +8622,13 @@
     </row>
     <row r="21" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>70</v>
+        <v>131</v>
       </c>
       <c r="B21" s="9"/>
       <c r="C21" s="8" t="s">
-        <v>71</v>
+        <v>130</v>
       </c>
       <c r="E21" s="13">
-        <f>VLOOKUP(A21,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
         <v>0</v>
       </c>
       <c r="I21" s="20">
@@ -8621,23 +8642,14 @@
       </c>
       <c r="N21" s="16"/>
       <c r="O21" s="20" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="22" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
-        <v>82</v>
-      </c>
+      <c r="A22" s="10"/>
       <c r="B22" s="22"/>
-      <c r="C22" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="E22" s="13">
-        <v>0</v>
-      </c>
-      <c r="M22" s="18">
-        <v>-8.5514960440672301</v>
-      </c>
+      <c r="C22" s="10"/>
+      <c r="M22" s="18"/>
       <c r="N22" s="16"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
only provide one kcat to sample other
</commit_message>
<xml_diff>
--- a/KineticModel/data/gtoyall.xlsx
+++ b/KineticModel/data/gtoyall.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25590" windowHeight="7875" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25590" windowHeight="7875" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="gtoy1" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="136">
   <si>
     <t>Enzymes</t>
   </si>
@@ -464,6 +464,9 @@
   </si>
   <si>
     <t>h[e]</t>
+  </si>
+  <si>
+    <t>1,1,0.01</t>
   </si>
 </sst>
 </file>
@@ -567,7 +570,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -593,6 +596,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -5123,7 +5129,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B6"/>
     </sheetView>
   </sheetViews>
@@ -6976,12 +6982,12 @@
   <dimension ref="A1:U19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="25.5703125" customWidth="1"/>
+    <col min="3" max="3" width="33.42578125" customWidth="1"/>
     <col min="13" max="13" width="9.85546875" customWidth="1"/>
     <col min="15" max="15" width="17.28515625" customWidth="1"/>
     <col min="16" max="16" width="13.28515625" customWidth="1"/>
@@ -7054,11 +7060,11 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="8" t="s">
+      <c r="B2" s="26"/>
+      <c r="C2" s="25" t="s">
         <v>116</v>
       </c>
       <c r="D2" s="13" t="s">
@@ -7176,11 +7182,11 @@
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13" t="s">
+      <c r="B5" s="27"/>
+      <c r="C5" s="27" t="s">
         <v>77</v>
       </c>
       <c r="D5" s="13"/>
@@ -7209,11 +7215,11 @@
       <c r="U5" s="13"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13" t="s">
+      <c r="B6" s="26"/>
+      <c r="C6" s="26" t="s">
         <v>127</v>
       </c>
       <c r="D6" s="13"/>
@@ -7244,11 +7250,11 @@
       <c r="U6" s="13"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13" t="s">
+      <c r="B7" s="26"/>
+      <c r="C7" s="26" t="s">
         <v>121</v>
       </c>
       <c r="D7" s="13"/>
@@ -7279,11 +7285,11 @@
       <c r="U7" s="13"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13" t="s">
+      <c r="B8" s="27"/>
+      <c r="C8" s="27" t="s">
         <v>85</v>
       </c>
       <c r="D8" s="13"/>
@@ -7312,11 +7318,11 @@
       <c r="U8" s="13"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13" t="s">
+      <c r="B9" s="27"/>
+      <c r="C9" s="27" t="s">
         <v>87</v>
       </c>
       <c r="D9" s="13"/>
@@ -7791,7 +7797,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:U21"/>
     </sheetView>
   </sheetViews>
@@ -8219,9 +8225,7 @@
       <c r="I11" s="13">
         <v>120</v>
       </c>
-      <c r="J11" s="13">
-        <v>0.02</v>
-      </c>
+      <c r="J11" s="13"/>
       <c r="K11" s="13"/>
       <c r="L11" s="13"/>
       <c r="M11" s="7"/>
@@ -8270,7 +8274,9 @@
       <c r="N12" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="O12" s="13"/>
+      <c r="O12" s="13" t="s">
+        <v>135</v>
+      </c>
       <c r="P12" s="13"/>
       <c r="Q12" s="13"/>
       <c r="R12" s="13"/>

</xml_diff>

<commit_message>
changes to ace and acc binding in rxn 1
</commit_message>
<xml_diff>
--- a/KineticModel/data/gtoyall.xlsx
+++ b/KineticModel/data/gtoyall.xlsx
@@ -445,9 +445,6 @@
     <t>g6p[c] ---&gt; g6p[e]</t>
   </si>
   <si>
-    <t>1e-2,1,1e-5,1</t>
-  </si>
-  <si>
     <t>1,0.1,1,0.1</t>
   </si>
   <si>
@@ -467,6 +464,9 @@
   </si>
   <si>
     <t>1,1,0.01</t>
+  </si>
+  <si>
+    <t>1e-5,1,1e-3,1</t>
   </si>
 </sst>
 </file>
@@ -5169,7 +5169,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B5" s="24">
         <v>1E-4</v>
@@ -7899,7 +7899,7 @@
       </c>
       <c r="N2" s="16"/>
       <c r="O2" s="13" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
@@ -8094,7 +8094,7 @@
       </c>
       <c r="N7" s="16"/>
       <c r="O7" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
@@ -8275,7 +8275,7 @@
         <v>51</v>
       </c>
       <c r="O12" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P12" s="13"/>
       <c r="Q12" s="13"/>
@@ -8477,7 +8477,7 @@
       </c>
       <c r="B17" s="13"/>
       <c r="C17" s="16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D17" s="13" t="s">
         <v>37</v>
@@ -8628,11 +8628,11 @@
     </row>
     <row r="21" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B21" s="9"/>
       <c r="C21" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E21" s="13">
         <v>0</v>
@@ -8648,7 +8648,7 @@
       </c>
       <c r="N21" s="16"/>
       <c r="O21" s="20" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="22" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
change input acetate copncentration
</commit_message>
<xml_diff>
--- a/KineticModel/data/gtoyall.xlsx
+++ b/KineticModel/data/gtoyall.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25590" windowHeight="7875" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25590" windowHeight="7875" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="gtoy1" sheetId="2" r:id="rId1"/>
@@ -5129,7 +5129,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:B6"/>
     </sheetView>
   </sheetViews>
@@ -5148,7 +5148,7 @@
         <v>94</v>
       </c>
       <c r="B2" s="13">
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -7797,7 +7797,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:U21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
new model file with h2oc and h2oe
</commit_message>
<xml_diff>
--- a/KineticModel/data/gtoyall.xlsx
+++ b/KineticModel/data/gtoyall.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25590" windowHeight="7875" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25590" windowHeight="7875" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="gtoy1" sheetId="2" r:id="rId1"/>
@@ -22,11 +22,13 @@
     <sheet name="gtoy4C" sheetId="9" r:id="rId8"/>
     <sheet name="gtoy5" sheetId="10" r:id="rId9"/>
     <sheet name="gtoy5C" sheetId="11" r:id="rId10"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId11"/>
+    <sheet name="gtoy6" sheetId="12" r:id="rId11"/>
+    <sheet name="gtoy6C" sheetId="13" r:id="rId12"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId13"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId12"/>
-    <externalReference r:id="rId13"/>
+    <externalReference r:id="rId14"/>
+    <externalReference r:id="rId15"/>
   </externalReferences>
   <calcPr calcId="171027"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="142">
   <si>
     <t>Enzymes</t>
   </si>
@@ -467,6 +469,24 @@
   </si>
   <si>
     <t>1e-5,1,1e-3,1</t>
+  </si>
+  <si>
+    <t>[c] : fdp + h2o --&gt; f6p</t>
+  </si>
+  <si>
+    <t>[c] : 2pg &lt;==&gt; pep + h2o</t>
+  </si>
+  <si>
+    <t>H2otr</t>
+  </si>
+  <si>
+    <t>H2Oex</t>
+  </si>
+  <si>
+    <t>h2o[c]</t>
+  </si>
+  <si>
+    <t>h2o[e]</t>
   </si>
 </sst>
 </file>
@@ -641,7 +661,6 @@
       <sheetName val="red_test"/>
       <sheetName val="red_testC"/>
       <sheetName val="red_test2"/>
-      <sheetName val="Sheet3"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
@@ -695,7 +714,6 @@
           <cell r="D3" t="str">
             <v>Transport, Extracellular</v>
           </cell>
-          <cell r="E3"/>
           <cell r="F3">
             <v>0</v>
           </cell>
@@ -809,7 +827,6 @@
           <cell r="D7" t="str">
             <v>Transport, Extracellular</v>
           </cell>
-          <cell r="E7"/>
           <cell r="F7">
             <v>0</v>
           </cell>
@@ -865,7 +882,6 @@
           <cell r="D9" t="str">
             <v>Citric Acid Cycle</v>
           </cell>
-          <cell r="E9"/>
           <cell r="F9">
             <v>-8.3000000000000007</v>
           </cell>
@@ -892,7 +908,6 @@
           <cell r="D10" t="str">
             <v>Transport, Extracellular</v>
           </cell>
-          <cell r="E10"/>
           <cell r="F10">
             <v>0</v>
           </cell>
@@ -948,7 +963,6 @@
           <cell r="D12" t="str">
             <v>Oxidative Phosphorylation</v>
           </cell>
-          <cell r="E12"/>
           <cell r="F12">
             <v>-6.6</v>
           </cell>
@@ -1001,10 +1015,6 @@
           <cell r="C14" t="str">
             <v>[c] : (1.496) 3pg + (3.7478) accoa + (59.8100) atp + (0.3610) e4p + (0.0709) f6p + (0.1290) g3p + (0.2050) g6p + (0.2557) gln-L + (4.9414) glu-L + (59.8100) h2o + (3.5470) nad + (13.0279) nadph + (1.7867) oaa + (0.5191) pep + (2.8328) pyr + (0.8977) r5p --&gt; (59.8100) adp + (4.1182) akg + (3.7478) coa + (59.8100) h + (3.5470) nadh + (13.0279) nadp + (59.8100) pi</v>
           </cell>
-          <cell r="D14"/>
-          <cell r="E14"/>
-          <cell r="F14"/>
-          <cell r="G14"/>
           <cell r="H14">
             <v>0.87390000000000001</v>
           </cell>
@@ -1025,7 +1035,6 @@
           <cell r="D15" t="str">
             <v>Transport, Extracellular</v>
           </cell>
-          <cell r="E15"/>
           <cell r="F15">
             <v>0</v>
           </cell>
@@ -1052,7 +1061,6 @@
           <cell r="D16" t="str">
             <v>Citric Acid Cycle</v>
           </cell>
-          <cell r="E16"/>
           <cell r="F16">
             <v>-8.6</v>
           </cell>
@@ -1079,7 +1087,6 @@
           <cell r="D17" t="str">
             <v>Oxidative Phosphorylation</v>
           </cell>
-          <cell r="E17"/>
           <cell r="F17">
             <v>-37.200000000000003</v>
           </cell>
@@ -1106,7 +1113,6 @@
           <cell r="D18" t="str">
             <v>Transport, Extracellular</v>
           </cell>
-          <cell r="E18"/>
           <cell r="F18">
             <v>0</v>
           </cell>
@@ -1162,7 +1168,6 @@
           <cell r="D20" t="str">
             <v>Transport, Extracellular</v>
           </cell>
-          <cell r="E20"/>
           <cell r="F20">
             <v>0</v>
           </cell>
@@ -1189,9 +1194,6 @@
           <cell r="D21" t="str">
             <v>Exchange</v>
           </cell>
-          <cell r="E21"/>
-          <cell r="F21"/>
-          <cell r="G21"/>
           <cell r="H21">
             <v>0</v>
           </cell>
@@ -1212,9 +1214,6 @@
           <cell r="D22" t="str">
             <v>Exchange</v>
           </cell>
-          <cell r="E22"/>
-          <cell r="F22"/>
-          <cell r="G22"/>
           <cell r="H22">
             <v>0</v>
           </cell>
@@ -1235,9 +1234,6 @@
           <cell r="D23" t="str">
             <v>Exchange</v>
           </cell>
-          <cell r="E23"/>
-          <cell r="F23"/>
-          <cell r="G23"/>
           <cell r="H23">
             <v>0</v>
           </cell>
@@ -1258,9 +1254,6 @@
           <cell r="D24" t="str">
             <v>Exchange</v>
           </cell>
-          <cell r="E24"/>
-          <cell r="F24"/>
-          <cell r="G24"/>
           <cell r="H24">
             <v>22.809799999999999</v>
           </cell>
@@ -1281,9 +1274,6 @@
           <cell r="D25" t="str">
             <v>Exchange</v>
           </cell>
-          <cell r="E25"/>
-          <cell r="F25"/>
-          <cell r="G25"/>
           <cell r="H25">
             <v>0</v>
           </cell>
@@ -1304,9 +1294,6 @@
           <cell r="D26" t="str">
             <v>Exchange</v>
           </cell>
-          <cell r="E26"/>
-          <cell r="F26"/>
-          <cell r="G26"/>
           <cell r="H26">
             <v>0</v>
           </cell>
@@ -1327,9 +1314,6 @@
           <cell r="D27" t="str">
             <v>Exchange</v>
           </cell>
-          <cell r="E27"/>
-          <cell r="F27"/>
-          <cell r="G27"/>
           <cell r="H27">
             <v>0</v>
           </cell>
@@ -1350,9 +1334,6 @@
           <cell r="D28" t="str">
             <v>Exchange</v>
           </cell>
-          <cell r="E28"/>
-          <cell r="F28"/>
-          <cell r="G28"/>
           <cell r="H28">
             <v>0</v>
           </cell>
@@ -1373,9 +1354,6 @@
           <cell r="D29" t="str">
             <v>Exchange</v>
           </cell>
-          <cell r="E29"/>
-          <cell r="F29"/>
-          <cell r="G29"/>
           <cell r="H29">
             <v>-10</v>
           </cell>
@@ -1396,9 +1374,6 @@
           <cell r="D30" t="str">
             <v>Exchange</v>
           </cell>
-          <cell r="E30"/>
-          <cell r="F30"/>
-          <cell r="G30"/>
           <cell r="H30">
             <v>0</v>
           </cell>
@@ -1419,9 +1394,6 @@
           <cell r="D31" t="str">
             <v>Exchange</v>
           </cell>
-          <cell r="E31"/>
-          <cell r="F31"/>
-          <cell r="G31"/>
           <cell r="H31">
             <v>0</v>
           </cell>
@@ -1442,9 +1414,6 @@
           <cell r="D32" t="str">
             <v>Exchange</v>
           </cell>
-          <cell r="E32"/>
-          <cell r="F32"/>
-          <cell r="G32"/>
           <cell r="H32">
             <v>17.530899999999999</v>
           </cell>
@@ -1465,9 +1434,6 @@
           <cell r="D33" t="str">
             <v>Exchange</v>
           </cell>
-          <cell r="E33"/>
-          <cell r="F33"/>
-          <cell r="G33"/>
           <cell r="H33">
             <v>29.175799999999999</v>
           </cell>
@@ -1488,9 +1454,6 @@
           <cell r="D34" t="str">
             <v>Exchange</v>
           </cell>
-          <cell r="E34"/>
-          <cell r="F34"/>
-          <cell r="G34"/>
           <cell r="H34">
             <v>0</v>
           </cell>
@@ -1511,9 +1474,6 @@
           <cell r="D35" t="str">
             <v>Exchange</v>
           </cell>
-          <cell r="E35"/>
-          <cell r="F35"/>
-          <cell r="G35"/>
           <cell r="H35">
             <v>0</v>
           </cell>
@@ -1534,9 +1494,6 @@
           <cell r="D36" t="str">
             <v>Exchange</v>
           </cell>
-          <cell r="E36"/>
-          <cell r="F36"/>
-          <cell r="G36"/>
           <cell r="H36">
             <v>-4.7652999999999999</v>
           </cell>
@@ -1557,9 +1514,6 @@
           <cell r="D37" t="str">
             <v>Exchange</v>
           </cell>
-          <cell r="E37"/>
-          <cell r="F37"/>
-          <cell r="G37"/>
           <cell r="H37">
             <v>-21.799499999999998</v>
           </cell>
@@ -1580,9 +1534,6 @@
           <cell r="D38" t="str">
             <v>Exchange</v>
           </cell>
-          <cell r="E38"/>
-          <cell r="F38"/>
-          <cell r="G38"/>
           <cell r="H38">
             <v>-3.2149000000000001</v>
           </cell>
@@ -1603,9 +1554,6 @@
           <cell r="D39" t="str">
             <v>Exchange</v>
           </cell>
-          <cell r="E39"/>
-          <cell r="F39"/>
-          <cell r="G39"/>
           <cell r="H39">
             <v>0</v>
           </cell>
@@ -1626,9 +1574,6 @@
           <cell r="D40" t="str">
             <v>Exchange</v>
           </cell>
-          <cell r="E40"/>
-          <cell r="F40"/>
-          <cell r="G40"/>
           <cell r="H40">
             <v>0</v>
           </cell>
@@ -1707,7 +1652,6 @@
           <cell r="D43" t="str">
             <v>Transport, Extracellular</v>
           </cell>
-          <cell r="E43"/>
           <cell r="F43">
             <v>0</v>
           </cell>
@@ -1734,7 +1678,6 @@
           <cell r="D44" t="str">
             <v>Transport, Extracellular</v>
           </cell>
-          <cell r="E44"/>
           <cell r="F44">
             <v>0</v>
           </cell>
@@ -1790,7 +1733,6 @@
           <cell r="D46" t="str">
             <v>Transport, Extracellular</v>
           </cell>
-          <cell r="E46"/>
           <cell r="F46">
             <v>-9.1</v>
           </cell>
@@ -1846,7 +1788,6 @@
           <cell r="D48" t="str">
             <v>Transport, Extracellular</v>
           </cell>
-          <cell r="E48"/>
           <cell r="F48">
             <v>0</v>
           </cell>
@@ -1931,7 +1872,6 @@
           <cell r="D51" t="str">
             <v>Transport, Extracellular</v>
           </cell>
-          <cell r="E51"/>
           <cell r="F51">
             <v>-9.1</v>
           </cell>
@@ -1987,7 +1927,6 @@
           <cell r="D53" t="str">
             <v>Transport, Extracellular</v>
           </cell>
-          <cell r="E53"/>
           <cell r="F53">
             <v>-6.6</v>
           </cell>
@@ -2101,7 +2040,6 @@
           <cell r="D57" t="str">
             <v>Transport, Extracellular</v>
           </cell>
-          <cell r="E57"/>
           <cell r="F57">
             <v>0</v>
           </cell>
@@ -2157,7 +2095,6 @@
           <cell r="D59" t="str">
             <v>Transport, Extracellular</v>
           </cell>
-          <cell r="E59"/>
           <cell r="F59">
             <v>0</v>
           </cell>
@@ -2300,7 +2237,6 @@
           <cell r="D64" t="str">
             <v>Transport, Extracellular</v>
           </cell>
-          <cell r="E64"/>
           <cell r="F64">
             <v>0</v>
           </cell>
@@ -2472,7 +2408,6 @@
           <cell r="D70" t="str">
             <v>Inorganic Ion Transport and Metabolism</v>
           </cell>
-          <cell r="E70"/>
           <cell r="F70">
             <v>0</v>
           </cell>
@@ -2499,7 +2434,6 @@
           <cell r="D71" t="str">
             <v>Transport, Extracellular</v>
           </cell>
-          <cell r="E71"/>
           <cell r="F71">
             <v>0</v>
           </cell>
@@ -2526,7 +2460,6 @@
           <cell r="D72" t="str">
             <v>Glycolysis/Gluconeogenesis</v>
           </cell>
-          <cell r="E72"/>
           <cell r="F72">
             <v>-8.3000000000000007</v>
           </cell>
@@ -2582,7 +2515,6 @@
           <cell r="D74" t="str">
             <v>Pyruvate Metabolism</v>
           </cell>
-          <cell r="E74"/>
           <cell r="F74">
             <v>-5.0999999999999996</v>
           </cell>
@@ -2725,7 +2657,6 @@
           <cell r="D79" t="str">
             <v>Inorganic Ion Transport and Metabolism</v>
           </cell>
-          <cell r="E79"/>
           <cell r="F79">
             <v>0</v>
           </cell>
@@ -2896,7 +2827,6 @@
       <sheetData sheetId="17"/>
       <sheetData sheetId="18"/>
       <sheetData sheetId="19"/>
-      <sheetData sheetId="20" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -5129,7 +5059,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B6"/>
     </sheetView>
   </sheetViews>
@@ -5189,6 +5119,1054 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="30.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="26"/>
+      <c r="C2" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="23">
+        <f>VLOOKUP(A2,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="17">
+        <v>1</v>
+      </c>
+      <c r="J2" s="23">
+        <v>1</v>
+      </c>
+      <c r="K2" s="23"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="18">
+        <v>-19.215657194822899</v>
+      </c>
+      <c r="N2" s="16"/>
+      <c r="O2" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23"/>
+      <c r="T2" s="23"/>
+      <c r="U2" s="23"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="23"/>
+      <c r="C3" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23">
+        <f>VLOOKUP(A3,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>4.2</v>
+      </c>
+      <c r="F3" s="23">
+        <v>-29.4</v>
+      </c>
+      <c r="G3" s="23">
+        <v>27.1</v>
+      </c>
+      <c r="H3" s="24"/>
+      <c r="I3" s="23">
+        <v>8.5</v>
+      </c>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="16" t="str">
+        <f>VLOOKUP(A3,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>4.1.2.13</v>
+      </c>
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="23"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="T3" s="23">
+        <v>0.218</v>
+      </c>
+      <c r="U3" s="23">
+        <v>0.218</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="23"/>
+      <c r="C4" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="23">
+        <f>VLOOKUP(A4,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>-2.8</v>
+      </c>
+      <c r="F4" s="23">
+        <v>-48.8</v>
+      </c>
+      <c r="G4" s="23">
+        <v>-9.6999999999999993</v>
+      </c>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23">
+        <v>22</v>
+      </c>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="18">
+        <v>0</v>
+      </c>
+      <c r="N4" s="16" t="str">
+        <f>VLOOKUP(A4,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>3.1.3.11</v>
+      </c>
+      <c r="O4" s="23"/>
+      <c r="P4" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q4" s="23"/>
+      <c r="R4" s="23">
+        <v>0.1</v>
+      </c>
+      <c r="S4" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="T4" s="23">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="U4" s="23">
+        <v>0.27200000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23">
+        <v>0</v>
+      </c>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23">
+        <v>1</v>
+      </c>
+      <c r="J5" s="23">
+        <v>1</v>
+      </c>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="23"/>
+      <c r="R5" s="23"/>
+      <c r="S5" s="23"/>
+      <c r="T5" s="23"/>
+      <c r="U5" s="23"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23">
+        <v>0</v>
+      </c>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23">
+        <v>1</v>
+      </c>
+      <c r="J6" s="23">
+        <v>0</v>
+      </c>
+      <c r="K6" s="23"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="23"/>
+      <c r="O6" s="23"/>
+      <c r="P6" s="23"/>
+      <c r="Q6" s="23"/>
+      <c r="R6" s="23"/>
+      <c r="S6" s="23"/>
+      <c r="T6" s="23"/>
+      <c r="U6" s="23"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="26"/>
+      <c r="C7" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" s="23">
+        <v>0</v>
+      </c>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="17">
+        <v>2540</v>
+      </c>
+      <c r="J7" s="23">
+        <v>2540</v>
+      </c>
+      <c r="K7" s="23"/>
+      <c r="L7" s="24">
+        <v>1E-3</v>
+      </c>
+      <c r="M7" s="18">
+        <v>-8.5077261088811902</v>
+      </c>
+      <c r="N7" s="16"/>
+      <c r="O7" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="P7" s="23"/>
+      <c r="Q7" s="23"/>
+      <c r="R7" s="23"/>
+      <c r="S7" s="23"/>
+      <c r="T7" s="23"/>
+      <c r="U7" s="23"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23">
+        <v>0</v>
+      </c>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23">
+        <v>1</v>
+      </c>
+      <c r="J8" s="23">
+        <v>1</v>
+      </c>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23"/>
+      <c r="O8" s="23"/>
+      <c r="P8" s="23"/>
+      <c r="Q8" s="23"/>
+      <c r="R8" s="23"/>
+      <c r="S8" s="23"/>
+      <c r="T8" s="23"/>
+      <c r="U8" s="23"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23">
+        <v>0</v>
+      </c>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23">
+        <v>1</v>
+      </c>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="23"/>
+      <c r="O9" s="23"/>
+      <c r="P9" s="23"/>
+      <c r="Q9" s="23"/>
+      <c r="R9" s="23"/>
+      <c r="S9" s="23"/>
+      <c r="T9" s="23"/>
+      <c r="U9" s="23"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="23"/>
+      <c r="C10" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23">
+        <f>VLOOKUP(A10,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>4.3</v>
+      </c>
+      <c r="F10" s="23">
+        <v>-24.3</v>
+      </c>
+      <c r="G10" s="23">
+        <v>52.1</v>
+      </c>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23">
+        <v>280</v>
+      </c>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="16" t="str">
+        <f>VLOOKUP(A10,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>2.7.2.1</v>
+      </c>
+      <c r="O10" s="23"/>
+      <c r="P10" s="23"/>
+      <c r="Q10" s="23"/>
+      <c r="R10" s="23"/>
+      <c r="S10" s="23"/>
+      <c r="T10" s="23"/>
+      <c r="U10" s="23"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="23"/>
+      <c r="C11" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="23">
+        <f>VLOOKUP(A11,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>3.8</v>
+      </c>
+      <c r="F11" s="23">
+        <v>-20.399999999999999</v>
+      </c>
+      <c r="G11" s="23">
+        <v>28.7</v>
+      </c>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23">
+        <v>120</v>
+      </c>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="16" t="str">
+        <f>VLOOKUP(A11,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>2.3.1.8</v>
+      </c>
+      <c r="O11" s="23"/>
+      <c r="P11" s="23"/>
+      <c r="Q11" s="23"/>
+      <c r="R11" s="23"/>
+      <c r="S11" s="23"/>
+      <c r="T11" s="23"/>
+      <c r="U11" s="23"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" s="23"/>
+      <c r="C12" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="23">
+        <v>-8.3000000000000007</v>
+      </c>
+      <c r="F12" s="23">
+        <v>-73</v>
+      </c>
+      <c r="G12" s="23">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23">
+        <v>6.32</v>
+      </c>
+      <c r="J12" s="23">
+        <v>0</v>
+      </c>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="O12" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="P12" s="23"/>
+      <c r="Q12" s="23"/>
+      <c r="R12" s="23"/>
+      <c r="S12" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="T12" s="23">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="U12" s="23">
+        <v>0.27600000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="23"/>
+      <c r="C13" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="23">
+        <v>-31.12</v>
+      </c>
+      <c r="F13" s="23">
+        <v>-10.8</v>
+      </c>
+      <c r="G13" s="23">
+        <v>65.3</v>
+      </c>
+      <c r="H13" s="24"/>
+      <c r="I13" s="23">
+        <v>2540</v>
+      </c>
+      <c r="J13" s="23"/>
+      <c r="K13" s="23"/>
+      <c r="L13" s="23"/>
+      <c r="M13" s="18"/>
+      <c r="N13" s="16" t="str">
+        <f>VLOOKUP(A13,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>2.7.1.40</v>
+      </c>
+      <c r="O13" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="P13" s="23"/>
+      <c r="Q13" s="23"/>
+      <c r="R13" s="23"/>
+      <c r="S13" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="T13" s="23">
+        <v>0.111</v>
+      </c>
+      <c r="U13" s="23">
+        <v>0.111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="23"/>
+      <c r="C14" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23">
+        <f>VLOOKUP(A14,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>-0.9</v>
+      </c>
+      <c r="F14" s="23">
+        <v>-22.9</v>
+      </c>
+      <c r="G14" s="23">
+        <v>14.7</v>
+      </c>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23">
+        <v>355.79</v>
+      </c>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="16" t="str">
+        <f>VLOOKUP(A14,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>4.2.1.11</v>
+      </c>
+      <c r="O14" s="23"/>
+      <c r="P14" s="23"/>
+      <c r="Q14" s="23"/>
+      <c r="R14" s="23"/>
+      <c r="S14" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="T14" s="23">
+        <v>2.67</v>
+      </c>
+      <c r="U14" s="23">
+        <v>2.67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="23"/>
+      <c r="C15" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23">
+        <v>6.2290000000000001</v>
+      </c>
+      <c r="F15" s="23">
+        <v>-23.1</v>
+      </c>
+      <c r="G15" s="23">
+        <v>14.6</v>
+      </c>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23">
+        <v>530</v>
+      </c>
+      <c r="K15" s="23"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="16" t="str">
+        <f>VLOOKUP(A15,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>5.4.2.1</v>
+      </c>
+      <c r="O15" s="23"/>
+      <c r="P15" s="23"/>
+      <c r="Q15" s="23"/>
+      <c r="R15" s="23"/>
+      <c r="S15" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="T15" s="23">
+        <v>2.67</v>
+      </c>
+      <c r="U15" s="23">
+        <v>2.67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="23"/>
+      <c r="C16" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23">
+        <v>-10.51</v>
+      </c>
+      <c r="F16" s="23">
+        <v>-19.2</v>
+      </c>
+      <c r="G16" s="23">
+        <v>56.1</v>
+      </c>
+      <c r="H16" s="24"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23">
+        <v>654</v>
+      </c>
+      <c r="K16" s="23"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="18"/>
+      <c r="N16" s="16" t="str">
+        <f>VLOOKUP(A16,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>2.7.2.3</v>
+      </c>
+      <c r="O16" s="23"/>
+      <c r="P16" s="23"/>
+      <c r="Q16" s="23"/>
+      <c r="R16" s="23"/>
+      <c r="S16" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="T16" s="23">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="U16" s="23">
+        <v>0.39900000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="23"/>
+      <c r="C17" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="23">
+        <f>VLOOKUP(A17,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>-0.1</v>
+      </c>
+      <c r="F17" s="23">
+        <v>-12.8</v>
+      </c>
+      <c r="G17" s="23">
+        <v>62.6</v>
+      </c>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23">
+        <v>268</v>
+      </c>
+      <c r="J17" s="23"/>
+      <c r="K17" s="23"/>
+      <c r="L17" s="23"/>
+      <c r="M17" s="18"/>
+      <c r="N17" s="16" t="str">
+        <f>VLOOKUP(A17,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>1.2.1.12</v>
+      </c>
+      <c r="O17" s="23"/>
+      <c r="P17" s="23"/>
+      <c r="Q17" s="23"/>
+      <c r="R17" s="23"/>
+      <c r="S17" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="T17" s="23">
+        <v>2.13</v>
+      </c>
+      <c r="U17" s="23">
+        <v>2.13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="23"/>
+      <c r="C18" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="23"/>
+      <c r="E18" s="17">
+        <v>7.5979999999999999</v>
+      </c>
+      <c r="F18" s="23">
+        <v>-24.3</v>
+      </c>
+      <c r="G18" s="23">
+        <v>13.4</v>
+      </c>
+      <c r="H18" s="23"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="23">
+        <v>9000</v>
+      </c>
+      <c r="K18" s="23"/>
+      <c r="L18" s="23"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="16" t="str">
+        <f>VLOOKUP(A18,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>5.3.1.1</v>
+      </c>
+      <c r="O18" s="23"/>
+      <c r="P18" s="23"/>
+      <c r="Q18" s="23"/>
+      <c r="R18" s="23"/>
+      <c r="S18" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="T18" s="23">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="U18" s="23">
+        <v>0.16700000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="23"/>
+      <c r="C19" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23">
+        <v>3.1320000000000001</v>
+      </c>
+      <c r="F19" s="23">
+        <v>-17.100000000000001</v>
+      </c>
+      <c r="G19" s="23">
+        <v>20.6</v>
+      </c>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23">
+        <v>120</v>
+      </c>
+      <c r="J19" s="23"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="23"/>
+      <c r="M19" s="18">
+        <v>11.639423575531699</v>
+      </c>
+      <c r="N19" s="16" t="str">
+        <f>VLOOKUP(A19,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>5.3.1.9</v>
+      </c>
+      <c r="O19" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="P19" s="23"/>
+      <c r="Q19" s="23"/>
+      <c r="R19" s="23"/>
+      <c r="S19" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="T19" s="23">
+        <v>3.48</v>
+      </c>
+      <c r="U19" s="23">
+        <v>3.48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" s="27"/>
+      <c r="C20" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23">
+        <v>0</v>
+      </c>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="18">
+        <v>63.607356573910501</v>
+      </c>
+      <c r="N20" s="16"/>
+      <c r="O20" s="23"/>
+      <c r="P20" s="23"/>
+      <c r="Q20" s="23"/>
+      <c r="R20" s="23"/>
+      <c r="S20" s="23"/>
+      <c r="T20" s="23"/>
+      <c r="U20" s="23"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A21" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="B21" s="26"/>
+      <c r="C21" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23">
+        <v>0</v>
+      </c>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="24">
+        <v>100</v>
+      </c>
+      <c r="J21" s="24">
+        <v>100</v>
+      </c>
+      <c r="K21" s="23"/>
+      <c r="L21" s="23"/>
+      <c r="M21" s="18">
+        <v>8.5514960440672301</v>
+      </c>
+      <c r="N21" s="16"/>
+      <c r="O21" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="P21" s="23"/>
+      <c r="Q21" s="23"/>
+      <c r="R21" s="23"/>
+      <c r="S21" s="23"/>
+      <c r="T21" s="23"/>
+      <c r="U21" s="23"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A22" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="E22" s="23">
+        <v>0</v>
+      </c>
+      <c r="F22" s="23"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="23"/>
+      <c r="K22" s="23"/>
+      <c r="L22" s="23"/>
+      <c r="M22" s="18"/>
+      <c r="N22" s="16"/>
+      <c r="O22" s="23"/>
+      <c r="P22" s="23"/>
+      <c r="Q22" s="23"/>
+      <c r="R22" s="23"/>
+      <c r="S22" s="23"/>
+      <c r="T22" s="23"/>
+      <c r="U22" s="23"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A23" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="E23" s="23">
+        <v>0</v>
+      </c>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="24">
+        <v>100</v>
+      </c>
+      <c r="J23" s="24">
+        <v>100</v>
+      </c>
+      <c r="K23" s="23"/>
+      <c r="L23" s="23"/>
+      <c r="M23" s="18"/>
+      <c r="N23" s="16"/>
+      <c r="O23" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="P23" s="23"/>
+      <c r="Q23" s="23"/>
+      <c r="R23" s="23"/>
+      <c r="S23" s="23"/>
+      <c r="T23" s="23"/>
+      <c r="U23" s="23"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="23">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5" s="24">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="24">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>140</v>
+      </c>
+      <c r="B7" s="24">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>141</v>
+      </c>
+      <c r="B8" s="24">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U25"/>
   <sheetViews>
@@ -7798,7 +8776,7 @@
   <dimension ref="A1:U22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:U21"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
new model with pic and pie
</commit_message>
<xml_diff>
--- a/KineticModel/data/gtoyall.xlsx
+++ b/KineticModel/data/gtoyall.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25590" windowHeight="7875" firstSheet="1" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25590" windowHeight="7875" firstSheet="1" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="gtoy1" sheetId="2" r:id="rId1"/>
@@ -23,15 +23,17 @@
     <sheet name="gtoy5" sheetId="10" r:id="rId9"/>
     <sheet name="gtoy5C" sheetId="11" r:id="rId10"/>
     <sheet name="gtoy6" sheetId="12" r:id="rId11"/>
-    <sheet name="Sheet3" sheetId="15" r:id="rId12"/>
-    <sheet name="gtoy6C" sheetId="13" r:id="rId13"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId14"/>
+    <sheet name="gtoy6C" sheetId="13" r:id="rId12"/>
+    <sheet name="gtoy7" sheetId="16" r:id="rId13"/>
+    <sheet name="gtoy7C" sheetId="17" r:id="rId14"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId15"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId15"/>
     <externalReference r:id="rId16"/>
+    <externalReference r:id="rId17"/>
   </externalReferences>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="229">
   <si>
     <t>Enzymes</t>
   </si>
@@ -712,30 +714,6 @@
     <t>[c] : mal --&gt; pyr</t>
   </si>
   <si>
-    <t>[c] : cit + coa &lt;==&gt; accoa + oaa</t>
-  </si>
-  <si>
-    <t>[c] : mal &lt;==&gt; fum</t>
-  </si>
-  <si>
-    <t>[c] : mal &lt;==&gt; oaa</t>
-  </si>
-  <si>
-    <t>succ[e] --&gt; succ[c]</t>
-  </si>
-  <si>
-    <t>akg[e] &lt;==&gt; akg[c]</t>
-  </si>
-  <si>
-    <t>fum[e] --&gt; fum[c]</t>
-  </si>
-  <si>
-    <t>mal[e] --&gt; mal[c]</t>
-  </si>
-  <si>
-    <t>pyr[e] &lt;==&gt; pyr[c]</t>
-  </si>
-  <si>
     <t>PPCK</t>
   </si>
   <si>
@@ -745,12 +723,6 @@
     <t>PPS</t>
   </si>
   <si>
-    <t>[c] : pyr --&gt; pep</t>
-  </si>
-  <si>
-    <t>[c] : coa + mal &lt;==&gt; accoa + glx</t>
-  </si>
-  <si>
     <t>[c] : cit + coa + h &lt;==&gt; accoa + oaa + h2o</t>
   </si>
   <si>
@@ -770,6 +742,15 @@
   </si>
   <si>
     <t>pyr[e] + h[e] &lt;==&gt; pyr[c] + h[c]</t>
+  </si>
+  <si>
+    <t>pi[c]</t>
+  </si>
+  <si>
+    <t>[c] : pyr + h2o --&gt; pep + 2 h + pi</t>
+  </si>
+  <si>
+    <t>[c] : succ + coa &lt;==&gt; succoa + pi</t>
   </si>
 </sst>
 </file>
@@ -947,14 +928,14 @@
       <sheetName val="red_test2"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
       <sheetData sheetId="8">
         <row r="2">
           <cell r="A2" t="str">
@@ -4658,16 +4639,16 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -4683,7 +4664,7 @@
       <sheetName val="metabolites"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="1">
           <cell r="A1" t="str">
@@ -6171,8 +6152,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -6929,13 +6910,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection sqref="A1:U42"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:U43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="42.5703125" customWidth="1"/>
+    <col min="15" max="15" width="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="18" x14ac:dyDescent="0.35">
@@ -7111,7 +7093,7 @@
         <v>142</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="E6" s="23">
         <v>8.6</v>
@@ -7231,7 +7213,7 @@
       </c>
       <c r="B9" s="23"/>
       <c r="C9" s="16" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="D9" s="23" t="s">
         <v>197</v>
@@ -7310,11 +7292,11 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="B11" s="16"/>
       <c r="C11" s="16" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="D11" s="23"/>
       <c r="E11" s="23">
@@ -7346,11 +7328,11 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="B12" s="16"/>
       <c r="C12" s="16" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="D12" s="23"/>
       <c r="E12" s="23">
@@ -7625,7 +7607,7 @@
       </c>
       <c r="B18" s="23"/>
       <c r="C18" s="16" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="D18" s="23" t="s">
         <v>169</v>
@@ -7669,7 +7651,7 @@
       </c>
       <c r="B19" s="26"/>
       <c r="C19" s="25" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="D19" s="23" t="s">
         <v>65</v>
@@ -7788,7 +7770,7 @@
       </c>
       <c r="B22" s="26"/>
       <c r="C22" s="28" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="D22" s="23" t="s">
         <v>65</v>
@@ -8355,7 +8337,7 @@
       </c>
       <c r="B36" s="26"/>
       <c r="C36" s="25" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="D36" s="23" t="s">
         <v>65</v>
@@ -8552,1220 +8534,32 @@
       </c>
       <c r="N42" s="16"/>
     </row>
-    <row r="43" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="23" t="s">
+        <v>214</v>
+      </c>
+      <c r="C43" s="23" t="s">
+        <v>215</v>
+      </c>
+      <c r="E43" s="23">
+        <f>VLOOKUP(A43,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>1.3</v>
+      </c>
+      <c r="I43" s="23">
+        <f>VLOOKUP($A43,[1]ecoliN1!$A$2:$J$84,9,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="J43" s="23">
+        <f>VLOOKUP($A43,[1]ecoliN1!$A$2:$J$84,10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U42"/>
-  <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection sqref="A1:U38"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="42.42578125" customWidth="1"/>
-    <col min="15" max="15" width="15" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:21" s="23" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="23" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="25" t="s">
-        <v>116</v>
-      </c>
-      <c r="D2" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="E2" s="23">
-        <f>VLOOKUP(A2,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="I2" s="17">
-        <v>1</v>
-      </c>
-      <c r="J2" s="23">
-        <v>1</v>
-      </c>
-      <c r="L2" s="24"/>
-      <c r="M2" s="18">
-        <v>-19.215657194822899</v>
-      </c>
-      <c r="N2" s="16"/>
-      <c r="O2" s="23" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
-        <v>119</v>
-      </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27" t="s">
-        <v>77</v>
-      </c>
-      <c r="E3" s="23">
-        <v>0</v>
-      </c>
-      <c r="I3" s="23">
-        <v>1</v>
-      </c>
-      <c r="J3" s="23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="E4" s="23">
-        <f>VLOOKUP(A4,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
-        <v>4.3</v>
-      </c>
-      <c r="F4" s="23">
-        <v>-24.3</v>
-      </c>
-      <c r="G4" s="23">
-        <v>52.1</v>
-      </c>
-      <c r="I4" s="23">
-        <v>280</v>
-      </c>
-      <c r="M4" s="18"/>
-      <c r="N4" s="16" t="str">
-        <f>VLOOKUP(A4,[2]reactions!$A$1:$E$96,5,FALSE)</f>
-        <v>2.7.2.1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="E5" s="23">
-        <f>VLOOKUP(A5,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
-        <v>3.8</v>
-      </c>
-      <c r="F5" s="23">
-        <v>-20.399999999999999</v>
-      </c>
-      <c r="G5" s="23">
-        <v>28.7</v>
-      </c>
-      <c r="I5" s="23">
-        <v>120</v>
-      </c>
-      <c r="M5" s="7"/>
-      <c r="N5" s="16" t="str">
-        <f>VLOOKUP(A5,[2]reactions!$A$1:$E$96,5,FALSE)</f>
-        <v>2.3.1.8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>216</v>
-      </c>
-      <c r="E6" s="23">
-        <v>8.6</v>
-      </c>
-      <c r="F6" s="23">
-        <v>-4</v>
-      </c>
-      <c r="G6" s="23">
-        <v>60.9</v>
-      </c>
-      <c r="J6" s="23">
-        <v>81</v>
-      </c>
-      <c r="M6" s="18">
-        <v>6.0051760006096302</v>
-      </c>
-      <c r="N6" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="S6" s="23" t="s">
-        <v>145</v>
-      </c>
-      <c r="T6" s="23">
-        <v>0.39800000000000002</v>
-      </c>
-      <c r="U6" s="23">
-        <v>0.39800000000000002</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="E7" s="23">
-        <f>VLOOKUP(A7,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
-        <v>1.5</v>
-      </c>
-      <c r="F7" s="23">
-        <v>-11.2</v>
-      </c>
-      <c r="G7" s="23">
-        <v>26.5</v>
-      </c>
-      <c r="I7" s="23">
-        <v>5.3</v>
-      </c>
-      <c r="M7" s="18">
-        <v>-6.0051760006096302</v>
-      </c>
-      <c r="N7" s="16" t="str">
-        <f>VLOOKUP(A7,[2]reactions!$A$1:$E$96,5,FALSE)</f>
-        <v>4.2.1.3</v>
-      </c>
-      <c r="S7" s="23" t="s">
-        <v>148</v>
-      </c>
-      <c r="T7" s="23">
-        <v>9.8000000000000004E-2</v>
-      </c>
-      <c r="U7" s="23">
-        <v>9.8000000000000004E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
-        <v>192</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>193</v>
-      </c>
-      <c r="E8" s="23">
-        <f>VLOOKUP(A8,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="F8" s="23">
-        <v>-38.700000000000003</v>
-      </c>
-      <c r="G8" s="23">
-        <v>17.8</v>
-      </c>
-      <c r="I8" s="23">
-        <v>5.2</v>
-      </c>
-      <c r="M8" s="18">
-        <v>0</v>
-      </c>
-      <c r="N8" s="16" t="str">
-        <f>VLOOKUP(A8,[2]reactions!$A$1:$E$96,5,FALSE)</f>
-        <v>4.1.3.1</v>
-      </c>
-      <c r="S8" s="23" t="s">
-        <v>194</v>
-      </c>
-      <c r="T8" s="23">
-        <v>0.59499999999999997</v>
-      </c>
-      <c r="U8" s="23">
-        <v>0.59499999999999997</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
-        <v>195</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>228</v>
-      </c>
-      <c r="D9" s="23" t="s">
-        <v>197</v>
-      </c>
-      <c r="E9" s="23">
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="F9" s="23">
-        <v>-9.1</v>
-      </c>
-      <c r="G9" s="23">
-        <v>63.1</v>
-      </c>
-      <c r="J9" s="23">
-        <v>48.1</v>
-      </c>
-      <c r="M9" s="18">
-        <v>0</v>
-      </c>
-      <c r="N9" s="16" t="s">
-        <v>198</v>
-      </c>
-      <c r="S9" s="23" t="s">
-        <v>199</v>
-      </c>
-      <c r="T9" s="23">
-        <v>4.2699999999999996</v>
-      </c>
-      <c r="U9" s="23">
-        <v>4.2699999999999996</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
-        <v>226</v>
-      </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16" t="s">
-        <v>227</v>
-      </c>
-      <c r="D10"/>
-      <c r="E10" s="23">
-        <f>VLOOKUP(A10,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
-        <v>-1.2</v>
-      </c>
-      <c r="F10"/>
-      <c r="G10"/>
-      <c r="H10"/>
-      <c r="I10" s="23">
-        <f>VLOOKUP($A10,[1]ecoliN1!$A$2:$J$84,9,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="J10" s="23">
-        <f>VLOOKUP($A10,[1]ecoliN1!$A$2:$J$84,10,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="K10"/>
-      <c r="L10"/>
-      <c r="M10"/>
-      <c r="N10"/>
-      <c r="O10"/>
-      <c r="P10"/>
-      <c r="Q10"/>
-      <c r="R10"/>
-      <c r="S10"/>
-      <c r="T10"/>
-      <c r="U10"/>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="s">
-        <v>224</v>
-      </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16" t="s">
-        <v>225</v>
-      </c>
-      <c r="E11" s="23">
-        <f>VLOOKUP(A11,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
-        <v>0.2</v>
-      </c>
-      <c r="I11" s="23">
-        <f>VLOOKUP($A11,[1]ecoliN1!$A$2:$J$84,9,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="J11" s="23">
-        <f>VLOOKUP($A11,[1]ecoliN1!$A$2:$J$84,10,FALSE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="D12" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="E12" s="23">
-        <f>VLOOKUP(A12,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
-        <v>3.4</v>
-      </c>
-      <c r="F12" s="23">
-        <v>-48.4</v>
-      </c>
-      <c r="G12" s="23">
-        <v>26.9</v>
-      </c>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23">
-        <v>106.4</v>
-      </c>
-      <c r="J12" s="23"/>
-      <c r="K12" s="23"/>
-      <c r="L12" s="23"/>
-      <c r="M12" s="18">
-        <v>-6.0051760006096302</v>
-      </c>
-      <c r="N12" s="16" t="str">
-        <f>VLOOKUP(A12,[2]reactions!$A$1:$E$96,5,FALSE)</f>
-        <v>1.1.1.42</v>
-      </c>
-      <c r="O12" s="23"/>
-      <c r="P12" s="23"/>
-      <c r="Q12" s="23"/>
-      <c r="R12" s="23"/>
-      <c r="S12" s="23" t="s">
-        <v>150</v>
-      </c>
-      <c r="T12" s="23">
-        <v>0.95499999999999996</v>
-      </c>
-      <c r="U12" s="23">
-        <v>0.95499999999999996</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="D13" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="E13" s="23">
-        <f>VLOOKUP(A13,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
-        <v>-8.3000000000000007</v>
-      </c>
-      <c r="F13" s="23">
-        <v>-72.3</v>
-      </c>
-      <c r="G13" s="23">
-        <v>20.3</v>
-      </c>
-      <c r="I13" s="23">
-        <v>49</v>
-      </c>
-      <c r="M13" s="18">
-        <v>3.5679805516174299</v>
-      </c>
-      <c r="N13" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="S13" s="23" t="s">
-        <v>154</v>
-      </c>
-      <c r="T13" s="23">
-        <v>0.19500000000000001</v>
-      </c>
-      <c r="U13" s="23">
-        <v>0.19500000000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="D14" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="E14" s="23">
-        <v>-1</v>
-      </c>
-      <c r="F14" s="23">
-        <v>-39.5</v>
-      </c>
-      <c r="G14" s="23">
-        <v>35.799999999999997</v>
-      </c>
-      <c r="H14" s="23">
-        <v>2.12</v>
-      </c>
-      <c r="I14" s="23">
-        <v>25.6</v>
-      </c>
-      <c r="M14" s="18">
-        <v>-3.5679805516174299</v>
-      </c>
-      <c r="N14" s="16" t="str">
-        <f>VLOOKUP(A14,[2]reactions!$A$1:$E$96,5,FALSE)</f>
-        <v>6.2.1.5</v>
-      </c>
-      <c r="S14" s="23" t="s">
-        <v>157</v>
-      </c>
-      <c r="T14" s="23">
-        <v>6.2E-2</v>
-      </c>
-      <c r="U14" s="23">
-        <v>6.2E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="E15" s="23">
-        <v>-2.1</v>
-      </c>
-      <c r="F15" s="23">
-        <v>-40.4</v>
-      </c>
-      <c r="G15" s="23">
-        <v>16.100000000000001</v>
-      </c>
-      <c r="I15" s="23">
-        <v>167</v>
-      </c>
-      <c r="M15" s="18">
-        <v>3.5679805516174299</v>
-      </c>
-      <c r="N15" s="16" t="str">
-        <f>VLOOKUP(A15,[2]reactions!$A$1:$E$96,5,FALSE)</f>
-        <v>1.3.99.1</v>
-      </c>
-      <c r="S15" s="23" t="s">
-        <v>160</v>
-      </c>
-      <c r="T15" s="23">
-        <v>1.47</v>
-      </c>
-      <c r="U15" s="23">
-        <v>1.47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
-        <v>165</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>217</v>
-      </c>
-      <c r="E16" s="23">
-        <v>0.6</v>
-      </c>
-      <c r="F16" s="23">
-        <v>-15.4</v>
-      </c>
-      <c r="G16" s="23">
-        <v>22.3</v>
-      </c>
-      <c r="I16" s="23">
-        <v>51.7</v>
-      </c>
-      <c r="M16" s="18">
-        <v>-3.5679805516174299</v>
-      </c>
-      <c r="N16" s="16" t="str">
-        <f>VLOOKUP(A16,[2]reactions!$A$1:$E$96,5,FALSE)</f>
-        <v>4.2.1.2</v>
-      </c>
-      <c r="S16" s="23" t="s">
-        <v>167</v>
-      </c>
-      <c r="T16" s="23">
-        <v>0.80800000000000005</v>
-      </c>
-      <c r="U16" s="23">
-        <v>0.80800000000000005</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="s">
-        <v>168</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>218</v>
-      </c>
-      <c r="D17" s="23" t="s">
-        <v>169</v>
-      </c>
-      <c r="E17" s="23">
-        <v>6.4</v>
-      </c>
-      <c r="F17" s="23">
-        <v>-7.3</v>
-      </c>
-      <c r="G17" s="23">
-        <v>68.599999999999994</v>
-      </c>
-      <c r="I17" s="23">
-        <v>931</v>
-      </c>
-      <c r="L17" s="23">
-        <v>50</v>
-      </c>
-      <c r="M17" s="18">
-        <v>3.5679805516174299</v>
-      </c>
-      <c r="N17" s="16" t="str">
-        <f>VLOOKUP(A17,[2]reactions!$A$1:$E$96,5,FALSE)</f>
-        <v>1.1.1.37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="23" t="s">
-        <v>214</v>
-      </c>
-      <c r="C18" s="23" t="s">
-        <v>215</v>
-      </c>
-      <c r="E18" s="23">
-        <f>VLOOKUP(A18,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
-        <v>1.3</v>
-      </c>
-      <c r="I18" s="23">
-        <f>VLOOKUP($A18,[1]ecoliN1!$A$2:$J$84,9,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="J18" s="23">
-        <f>VLOOKUP($A18,[1]ecoliN1!$A$2:$J$84,10,FALSE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="25" t="s">
-        <v>172</v>
-      </c>
-      <c r="B19" s="26"/>
-      <c r="C19" s="25" t="s">
-        <v>219</v>
-      </c>
-      <c r="D19" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="E19" s="23">
-        <v>0</v>
-      </c>
-      <c r="I19" s="17">
-        <v>1</v>
-      </c>
-      <c r="J19" s="23">
-        <v>0</v>
-      </c>
-      <c r="M19" s="18">
-        <v>0</v>
-      </c>
-      <c r="N19" s="16"/>
-      <c r="O19" s="23" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="B20" s="26"/>
-      <c r="C20" s="25" t="s">
-        <v>220</v>
-      </c>
-      <c r="D20" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="E20" s="23">
-        <f>VLOOKUP(A20,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="I20" s="17">
-        <v>1</v>
-      </c>
-      <c r="J20" s="23">
-        <v>1</v>
-      </c>
-      <c r="M20" s="18">
-        <v>0</v>
-      </c>
-      <c r="N20" s="16"/>
-      <c r="O20" s="23" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="s">
-        <v>180</v>
-      </c>
-      <c r="B21" s="26"/>
-      <c r="C21" s="25" t="s">
-        <v>221</v>
-      </c>
-      <c r="D21" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="E21" s="23">
-        <f>VLOOKUP(A21,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="I21" s="17">
-        <v>1</v>
-      </c>
-      <c r="J21" s="23">
-        <v>0</v>
-      </c>
-      <c r="M21" s="18">
-        <v>0</v>
-      </c>
-      <c r="N21" s="16"/>
-      <c r="O21" s="23" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="28" t="s">
-        <v>182</v>
-      </c>
-      <c r="B22" s="26"/>
-      <c r="C22" s="28" t="s">
-        <v>222</v>
-      </c>
-      <c r="D22" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="E22" s="23">
-        <f>VLOOKUP(A22,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="I22" s="17">
-        <v>1</v>
-      </c>
-      <c r="J22" s="23">
-        <v>0</v>
-      </c>
-      <c r="M22" s="18">
-        <v>0</v>
-      </c>
-      <c r="N22" s="16"/>
-      <c r="O22" s="23" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
-        <v>184</v>
-      </c>
-      <c r="B23" s="27"/>
-      <c r="C23" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="E23" s="23">
-        <v>0</v>
-      </c>
-      <c r="M23" s="18">
-        <v>0</v>
-      </c>
-      <c r="N23" s="16"/>
-    </row>
-    <row r="24" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="B24" s="27"/>
-      <c r="C24" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="E24" s="23">
-        <v>0</v>
-      </c>
-      <c r="M24" s="18">
-        <v>0</v>
-      </c>
-      <c r="N24" s="16"/>
-    </row>
-    <row r="25" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="B25" s="27"/>
-      <c r="C25" s="10" t="s">
-        <v>189</v>
-      </c>
-      <c r="E25" s="23">
-        <v>0</v>
-      </c>
-      <c r="M25" s="18">
-        <v>0</v>
-      </c>
-      <c r="N25" s="16"/>
-    </row>
-    <row r="26" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
-        <v>190</v>
-      </c>
-      <c r="B26" s="27"/>
-      <c r="C26" s="10" t="s">
-        <v>191</v>
-      </c>
-      <c r="E26" s="23">
-        <v>0</v>
-      </c>
-      <c r="M26" s="18">
-        <v>0</v>
-      </c>
-      <c r="N26" s="16"/>
-    </row>
-    <row r="27" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C27" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="E27" s="23">
-        <f>VLOOKUP(A27,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
-        <v>-0.9</v>
-      </c>
-      <c r="F27" s="23">
-        <v>-22.9</v>
-      </c>
-      <c r="G27" s="23">
-        <v>14.7</v>
-      </c>
-      <c r="I27" s="23">
-        <v>355.79</v>
-      </c>
-      <c r="M27" s="18"/>
-      <c r="N27" s="16" t="str">
-        <f>VLOOKUP(A27,[2]reactions!$A$1:$E$96,5,FALSE)</f>
-        <v>4.2.1.11</v>
-      </c>
-      <c r="S27" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="T27" s="23">
-        <v>2.67</v>
-      </c>
-      <c r="U27" s="23">
-        <v>2.67</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="C28" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="E28" s="23">
-        <v>6.2290000000000001</v>
-      </c>
-      <c r="F28" s="23">
-        <v>-23.1</v>
-      </c>
-      <c r="G28" s="23">
-        <v>14.6</v>
-      </c>
-      <c r="J28" s="23">
-        <v>530</v>
-      </c>
-      <c r="M28" s="18"/>
-      <c r="N28" s="16" t="str">
-        <f>VLOOKUP(A28,[2]reactions!$A$1:$E$96,5,FALSE)</f>
-        <v>5.4.2.1</v>
-      </c>
-      <c r="S28" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="T28" s="23">
-        <v>2.67</v>
-      </c>
-      <c r="U28" s="23">
-        <v>2.67</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="C29" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="E29" s="23">
-        <v>-10.51</v>
-      </c>
-      <c r="F29" s="23">
-        <v>-19.2</v>
-      </c>
-      <c r="G29" s="23">
-        <v>56.1</v>
-      </c>
-      <c r="H29" s="24"/>
-      <c r="J29" s="23">
-        <v>654</v>
-      </c>
-      <c r="M29" s="18"/>
-      <c r="N29" s="16" t="str">
-        <f>VLOOKUP(A29,[2]reactions!$A$1:$E$96,5,FALSE)</f>
-        <v>2.7.2.3</v>
-      </c>
-      <c r="S29" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="T29" s="23">
-        <v>0.39900000000000002</v>
-      </c>
-      <c r="U29" s="23">
-        <v>0.39900000000000002</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="D30" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="E30" s="23">
-        <f>VLOOKUP(A30,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
-        <v>-0.1</v>
-      </c>
-      <c r="F30" s="23">
-        <v>-12.8</v>
-      </c>
-      <c r="G30" s="23">
-        <v>62.6</v>
-      </c>
-      <c r="I30" s="23">
-        <v>268</v>
-      </c>
-      <c r="M30" s="18"/>
-      <c r="N30" s="16" t="str">
-        <f>VLOOKUP(A30,[2]reactions!$A$1:$E$96,5,FALSE)</f>
-        <v>1.2.1.12</v>
-      </c>
-      <c r="S30" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="T30" s="23">
-        <v>2.13</v>
-      </c>
-      <c r="U30" s="23">
-        <v>2.13</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="C31" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E31" s="17">
-        <v>7.5979999999999999</v>
-      </c>
-      <c r="F31" s="23">
-        <v>-24.3</v>
-      </c>
-      <c r="G31" s="23">
-        <v>13.4</v>
-      </c>
-      <c r="J31" s="23">
-        <v>9000</v>
-      </c>
-      <c r="M31" s="7"/>
-      <c r="N31" s="16" t="str">
-        <f>VLOOKUP(A31,[2]reactions!$A$1:$E$96,5,FALSE)</f>
-        <v>5.3.1.1</v>
-      </c>
-      <c r="S31" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="T31" s="23">
-        <v>0.16700000000000001</v>
-      </c>
-      <c r="U31" s="23">
-        <v>0.16700000000000001</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C32" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="E32" s="23">
-        <f>VLOOKUP(A32,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
-        <v>4.2</v>
-      </c>
-      <c r="F32" s="23">
-        <v>-29.4</v>
-      </c>
-      <c r="G32" s="23">
-        <v>27.1</v>
-      </c>
-      <c r="H32" s="24"/>
-      <c r="I32" s="23">
-        <v>8.5</v>
-      </c>
-      <c r="M32" s="18"/>
-      <c r="N32" s="16" t="str">
-        <f>VLOOKUP(A32,[2]reactions!$A$1:$E$96,5,FALSE)</f>
-        <v>4.1.2.13</v>
-      </c>
-      <c r="S32" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="T32" s="23">
-        <v>0.218</v>
-      </c>
-      <c r="U32" s="23">
-        <v>0.218</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="C33" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="D33" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="E33" s="23">
-        <f>VLOOKUP(A33,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
-        <v>-2.8</v>
-      </c>
-      <c r="F33" s="23">
-        <v>-48.8</v>
-      </c>
-      <c r="G33" s="23">
-        <v>-9.6999999999999993</v>
-      </c>
-      <c r="I33" s="23">
-        <v>22</v>
-      </c>
-      <c r="M33" s="18">
-        <v>0</v>
-      </c>
-      <c r="N33" s="16" t="str">
-        <f>VLOOKUP(A33,[2]reactions!$A$1:$E$96,5,FALSE)</f>
-        <v>3.1.3.11</v>
-      </c>
-      <c r="P33" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="R33" s="23">
-        <v>0.1</v>
-      </c>
-      <c r="S33" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="T33" s="23">
-        <v>0.27200000000000002</v>
-      </c>
-      <c r="U33" s="23">
-        <v>0.27200000000000002</v>
-      </c>
-    </row>
-    <row r="34" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C34" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="E34" s="23">
-        <v>3.1320000000000001</v>
-      </c>
-      <c r="F34" s="23">
-        <v>-17.100000000000001</v>
-      </c>
-      <c r="G34" s="23">
-        <v>20.6</v>
-      </c>
-      <c r="I34" s="23">
-        <v>120</v>
-      </c>
-      <c r="M34" s="18">
-        <v>11.639423575531699</v>
-      </c>
-      <c r="N34" s="16" t="str">
-        <f>VLOOKUP(A34,[2]reactions!$A$1:$E$96,5,FALSE)</f>
-        <v>5.3.1.9</v>
-      </c>
-      <c r="O34" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="S34" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="T34" s="23">
-        <v>3.48</v>
-      </c>
-      <c r="U34" s="23">
-        <v>3.48</v>
-      </c>
-    </row>
-    <row r="35" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="26" t="s">
-        <v>125</v>
-      </c>
-      <c r="B35" s="26"/>
-      <c r="C35" s="26" t="s">
-        <v>127</v>
-      </c>
-      <c r="E35" s="23">
-        <v>0</v>
-      </c>
-      <c r="I35" s="23">
-        <v>1</v>
-      </c>
-      <c r="J35" s="23">
-        <v>0</v>
-      </c>
-      <c r="L35" s="24"/>
-    </row>
-    <row r="36" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="B36" s="26"/>
-      <c r="C36" s="25" t="s">
-        <v>223</v>
-      </c>
-      <c r="D36" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="E36" s="23">
-        <v>0</v>
-      </c>
-      <c r="I36" s="17">
-        <v>2540</v>
-      </c>
-      <c r="J36" s="23">
-        <v>2540</v>
-      </c>
-      <c r="L36" s="24">
-        <v>1E-3</v>
-      </c>
-      <c r="M36" s="18">
-        <v>-8.5077261088811902</v>
-      </c>
-      <c r="N36" s="16"/>
-      <c r="O36" s="23" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="37" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="27" t="s">
-        <v>122</v>
-      </c>
-      <c r="B37" s="27"/>
-      <c r="C37" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="E37" s="23">
-        <v>0</v>
-      </c>
-      <c r="I37" s="23">
-        <v>1</v>
-      </c>
-      <c r="J37" s="23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="27" t="s">
-        <v>126</v>
-      </c>
-      <c r="B38" s="27"/>
-      <c r="C38" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="E38" s="23">
-        <v>0</v>
-      </c>
-      <c r="J38" s="23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
@@ -9884,12 +8678,1895 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U43"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:XFD28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="44.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="26"/>
+      <c r="C2" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="23">
+        <f>VLOOKUP(A2,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="17">
+        <v>1</v>
+      </c>
+      <c r="J2" s="23">
+        <v>1</v>
+      </c>
+      <c r="K2" s="23"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="18">
+        <v>-19.215657194822899</v>
+      </c>
+      <c r="N2" s="16"/>
+      <c r="O2" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23"/>
+      <c r="T2" s="23"/>
+      <c r="U2" s="23"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23">
+        <v>0</v>
+      </c>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23">
+        <v>1</v>
+      </c>
+      <c r="J3" s="23">
+        <v>1</v>
+      </c>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="23"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="23"/>
+      <c r="T3" s="23"/>
+      <c r="U3" s="23"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="23"/>
+      <c r="C4" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23">
+        <f>VLOOKUP(A4,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>4.3</v>
+      </c>
+      <c r="F4" s="23">
+        <v>-24.3</v>
+      </c>
+      <c r="G4" s="23">
+        <v>52.1</v>
+      </c>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23">
+        <v>280</v>
+      </c>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="16" t="str">
+        <f>VLOOKUP(A4,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>2.7.2.1</v>
+      </c>
+      <c r="O4" s="23"/>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="23"/>
+      <c r="R4" s="23"/>
+      <c r="S4" s="23"/>
+      <c r="T4" s="23"/>
+      <c r="U4" s="23"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="23"/>
+      <c r="C5" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="23">
+        <f>VLOOKUP(A5,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>3.8</v>
+      </c>
+      <c r="F5" s="23">
+        <v>-20.399999999999999</v>
+      </c>
+      <c r="G5" s="23">
+        <v>28.7</v>
+      </c>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23">
+        <v>120</v>
+      </c>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="16" t="str">
+        <f>VLOOKUP(A5,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>2.3.1.8</v>
+      </c>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="23"/>
+      <c r="R5" s="23"/>
+      <c r="S5" s="23"/>
+      <c r="T5" s="23"/>
+      <c r="U5" s="23"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="B6" s="23"/>
+      <c r="C6" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23">
+        <v>8.6</v>
+      </c>
+      <c r="F6" s="23">
+        <v>-4</v>
+      </c>
+      <c r="G6" s="23">
+        <v>60.9</v>
+      </c>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23">
+        <v>81</v>
+      </c>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="18">
+        <v>6.0051760006096302</v>
+      </c>
+      <c r="N6" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="O6" s="23"/>
+      <c r="P6" s="23"/>
+      <c r="Q6" s="23"/>
+      <c r="R6" s="23"/>
+      <c r="S6" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="T6" s="23">
+        <v>0.39800000000000002</v>
+      </c>
+      <c r="U6" s="23">
+        <v>0.39800000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="B7" s="23"/>
+      <c r="C7" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23">
+        <f>VLOOKUP(A7,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>1.5</v>
+      </c>
+      <c r="F7" s="23">
+        <v>-11.2</v>
+      </c>
+      <c r="G7" s="23">
+        <v>26.5</v>
+      </c>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23">
+        <v>5.3</v>
+      </c>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="18">
+        <v>-6.0051760006096302</v>
+      </c>
+      <c r="N7" s="16" t="str">
+        <f>VLOOKUP(A7,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>4.2.1.3</v>
+      </c>
+      <c r="O7" s="23"/>
+      <c r="P7" s="23"/>
+      <c r="Q7" s="23"/>
+      <c r="R7" s="23"/>
+      <c r="S7" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="T7" s="23">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="U7" s="23">
+        <v>9.8000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="B8" s="23"/>
+      <c r="C8" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23">
+        <f>VLOOKUP(A8,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="F8" s="23">
+        <v>-38.700000000000003</v>
+      </c>
+      <c r="G8" s="23">
+        <v>17.8</v>
+      </c>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23">
+        <v>5.2</v>
+      </c>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="18">
+        <v>0</v>
+      </c>
+      <c r="N8" s="16" t="str">
+        <f>VLOOKUP(A8,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>4.1.3.1</v>
+      </c>
+      <c r="O8" s="23"/>
+      <c r="P8" s="23"/>
+      <c r="Q8" s="23"/>
+      <c r="R8" s="23"/>
+      <c r="S8" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="T8" s="23">
+        <v>0.59499999999999997</v>
+      </c>
+      <c r="U8" s="23">
+        <v>0.59499999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="B9" s="23"/>
+      <c r="C9" s="16" t="s">
+        <v>220</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>197</v>
+      </c>
+      <c r="E9" s="23">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="F9" s="23">
+        <v>-9.1</v>
+      </c>
+      <c r="G9" s="23">
+        <v>63.1</v>
+      </c>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23">
+        <v>48.1</v>
+      </c>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="18">
+        <v>0</v>
+      </c>
+      <c r="N9" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="O9" s="23"/>
+      <c r="P9" s="23"/>
+      <c r="Q9" s="23"/>
+      <c r="R9" s="23"/>
+      <c r="S9" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="T9" s="23">
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="U9" s="23">
+        <v>4.2699999999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="23" t="s">
+        <v>214</v>
+      </c>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23" t="s">
+        <v>215</v>
+      </c>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23">
+        <f>VLOOKUP(A10,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>1.3</v>
+      </c>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23">
+        <f>VLOOKUP($A10,[1]ecoliN1!$A$2:$J$84,9,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="J10" s="23">
+        <f>VLOOKUP($A10,[1]ecoliN1!$A$2:$J$84,10,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="23"/>
+      <c r="O10" s="23"/>
+      <c r="P10" s="23"/>
+      <c r="Q10" s="23"/>
+      <c r="R10" s="23"/>
+      <c r="S10" s="23"/>
+      <c r="T10" s="23"/>
+      <c r="U10" s="23"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16" t="s">
+        <v>227</v>
+      </c>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23">
+        <f>VLOOKUP(A11,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>-1.2</v>
+      </c>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23">
+        <f>VLOOKUP($A11,[1]ecoliN1!$A$2:$J$84,9,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="J11" s="23">
+        <f>VLOOKUP($A11,[1]ecoliN1!$A$2:$J$84,10,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="23"/>
+      <c r="O11" s="23"/>
+      <c r="P11" s="23"/>
+      <c r="Q11" s="23"/>
+      <c r="R11" s="23"/>
+      <c r="S11" s="23"/>
+      <c r="T11" s="23"/>
+      <c r="U11" s="23"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
+        <v>216</v>
+      </c>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23">
+        <f>VLOOKUP(A12,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>0.2</v>
+      </c>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23">
+        <f>VLOOKUP($A12,[1]ecoliN1!$A$2:$J$84,9,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="J12" s="23">
+        <f>VLOOKUP($A12,[1]ecoliN1!$A$2:$J$84,10,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="23"/>
+      <c r="O12" s="23"/>
+      <c r="P12" s="23"/>
+      <c r="Q12" s="23"/>
+      <c r="R12" s="23"/>
+      <c r="S12" s="23"/>
+      <c r="T12" s="23"/>
+      <c r="U12" s="23"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="B13" s="23"/>
+      <c r="C13" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="23">
+        <f>VLOOKUP(A13,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>3.4</v>
+      </c>
+      <c r="F13" s="23">
+        <v>-48.4</v>
+      </c>
+      <c r="G13" s="23">
+        <v>26.9</v>
+      </c>
+      <c r="H13" s="23"/>
+      <c r="I13" s="23">
+        <v>106.4</v>
+      </c>
+      <c r="J13" s="23"/>
+      <c r="K13" s="23"/>
+      <c r="L13" s="23"/>
+      <c r="M13" s="18">
+        <v>-6.0051760006096302</v>
+      </c>
+      <c r="N13" s="16" t="str">
+        <f>VLOOKUP(A13,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>1.1.1.42</v>
+      </c>
+      <c r="O13" s="23"/>
+      <c r="P13" s="23"/>
+      <c r="Q13" s="23"/>
+      <c r="R13" s="23"/>
+      <c r="S13" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="T13" s="23">
+        <v>0.95499999999999996</v>
+      </c>
+      <c r="U13" s="23">
+        <v>0.95499999999999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="B14" s="23"/>
+      <c r="C14" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="23">
+        <f>VLOOKUP(A14,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>-8.3000000000000007</v>
+      </c>
+      <c r="F14" s="23">
+        <v>-72.3</v>
+      </c>
+      <c r="G14" s="23">
+        <v>20.3</v>
+      </c>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23">
+        <v>49</v>
+      </c>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="18">
+        <v>3.5679805516174299</v>
+      </c>
+      <c r="N14" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="O14" s="23"/>
+      <c r="P14" s="23"/>
+      <c r="Q14" s="23"/>
+      <c r="R14" s="23"/>
+      <c r="S14" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="T14" s="23">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="U14" s="23">
+        <v>0.19500000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="B15" s="23"/>
+      <c r="C15" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="23">
+        <v>-1</v>
+      </c>
+      <c r="F15" s="23">
+        <v>-39.5</v>
+      </c>
+      <c r="G15" s="23">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="H15" s="23">
+        <v>2.12</v>
+      </c>
+      <c r="I15" s="23">
+        <v>25.6</v>
+      </c>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="18">
+        <v>-3.5679805516174299</v>
+      </c>
+      <c r="N15" s="16" t="str">
+        <f>VLOOKUP(A15,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>6.2.1.5</v>
+      </c>
+      <c r="O15" s="23"/>
+      <c r="P15" s="23"/>
+      <c r="Q15" s="23"/>
+      <c r="R15" s="23"/>
+      <c r="S15" s="23" t="s">
+        <v>157</v>
+      </c>
+      <c r="T15" s="23">
+        <v>6.2E-2</v>
+      </c>
+      <c r="U15" s="23">
+        <v>6.2E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="B16" s="23"/>
+      <c r="C16" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23">
+        <v>-2.1</v>
+      </c>
+      <c r="F16" s="23">
+        <v>-40.4</v>
+      </c>
+      <c r="G16" s="23">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23">
+        <v>167</v>
+      </c>
+      <c r="J16" s="23"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="18">
+        <v>3.5679805516174299</v>
+      </c>
+      <c r="N16" s="16" t="str">
+        <f>VLOOKUP(A16,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>1.3.99.1</v>
+      </c>
+      <c r="O16" s="23"/>
+      <c r="P16" s="23"/>
+      <c r="Q16" s="23"/>
+      <c r="R16" s="23"/>
+      <c r="S16" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="T16" s="23">
+        <v>1.47</v>
+      </c>
+      <c r="U16" s="23">
+        <v>1.47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="B17" s="23"/>
+      <c r="C17" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23">
+        <v>0.6</v>
+      </c>
+      <c r="F17" s="23">
+        <v>-15.4</v>
+      </c>
+      <c r="G17" s="23">
+        <v>22.3</v>
+      </c>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23">
+        <v>51.7</v>
+      </c>
+      <c r="J17" s="23"/>
+      <c r="K17" s="23"/>
+      <c r="L17" s="23"/>
+      <c r="M17" s="18">
+        <v>-3.5679805516174299</v>
+      </c>
+      <c r="N17" s="16" t="str">
+        <f>VLOOKUP(A17,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>4.2.1.2</v>
+      </c>
+      <c r="O17" s="23"/>
+      <c r="P17" s="23"/>
+      <c r="Q17" s="23"/>
+      <c r="R17" s="23"/>
+      <c r="S17" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="T17" s="23">
+        <v>0.80800000000000005</v>
+      </c>
+      <c r="U17" s="23">
+        <v>0.80800000000000005</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="B18" s="23"/>
+      <c r="C18" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="E18" s="23">
+        <v>6.4</v>
+      </c>
+      <c r="F18" s="23">
+        <v>-7.3</v>
+      </c>
+      <c r="G18" s="23">
+        <v>68.599999999999994</v>
+      </c>
+      <c r="H18" s="23"/>
+      <c r="I18" s="23">
+        <v>931</v>
+      </c>
+      <c r="J18" s="23"/>
+      <c r="K18" s="23"/>
+      <c r="L18" s="23">
+        <v>50</v>
+      </c>
+      <c r="M18" s="18">
+        <v>3.5679805516174299</v>
+      </c>
+      <c r="N18" s="16" t="str">
+        <f>VLOOKUP(A18,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>1.1.1.37</v>
+      </c>
+      <c r="O18" s="23"/>
+      <c r="P18" s="23"/>
+      <c r="Q18" s="23"/>
+      <c r="R18" s="23"/>
+      <c r="S18" s="23"/>
+      <c r="T18" s="23"/>
+      <c r="U18" s="23"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="B19" s="26"/>
+      <c r="C19" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19" s="23">
+        <v>0</v>
+      </c>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="17">
+        <v>1</v>
+      </c>
+      <c r="J19" s="23">
+        <v>0</v>
+      </c>
+      <c r="K19" s="23"/>
+      <c r="L19" s="23"/>
+      <c r="M19" s="18">
+        <v>0</v>
+      </c>
+      <c r="N19" s="16"/>
+      <c r="O19" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="P19" s="23"/>
+      <c r="Q19" s="23"/>
+      <c r="R19" s="23"/>
+      <c r="S19" s="23"/>
+      <c r="T19" s="23"/>
+      <c r="U19" s="23"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20" s="25" t="s">
+        <v>178</v>
+      </c>
+      <c r="B20" s="26"/>
+      <c r="C20" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20" s="23">
+        <f>VLOOKUP(A20,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="17">
+        <v>1</v>
+      </c>
+      <c r="J20" s="23">
+        <v>1</v>
+      </c>
+      <c r="K20" s="23"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="18">
+        <v>0</v>
+      </c>
+      <c r="N20" s="16"/>
+      <c r="O20" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="P20" s="23"/>
+      <c r="Q20" s="23"/>
+      <c r="R20" s="23"/>
+      <c r="S20" s="23"/>
+      <c r="T20" s="23"/>
+      <c r="U20" s="23"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A21" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="B21" s="26"/>
+      <c r="C21" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="D21" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="E21" s="23">
+        <f>VLOOKUP(A21,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="17">
+        <v>1</v>
+      </c>
+      <c r="J21" s="23">
+        <v>0</v>
+      </c>
+      <c r="K21" s="23"/>
+      <c r="L21" s="23"/>
+      <c r="M21" s="18">
+        <v>0</v>
+      </c>
+      <c r="N21" s="16"/>
+      <c r="O21" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="P21" s="23"/>
+      <c r="Q21" s="23"/>
+      <c r="R21" s="23"/>
+      <c r="S21" s="23"/>
+      <c r="T21" s="23"/>
+      <c r="U21" s="23"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="B22" s="27"/>
+      <c r="C22" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23">
+        <v>0</v>
+      </c>
+      <c r="F22" s="23"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="23"/>
+      <c r="K22" s="23"/>
+      <c r="L22" s="23"/>
+      <c r="M22" s="18">
+        <v>0</v>
+      </c>
+      <c r="N22" s="16"/>
+      <c r="O22" s="23"/>
+      <c r="P22" s="23"/>
+      <c r="Q22" s="23"/>
+      <c r="R22" s="23"/>
+      <c r="S22" s="23"/>
+      <c r="T22" s="23"/>
+      <c r="U22" s="23"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="B23" s="27"/>
+      <c r="C23" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23">
+        <v>0</v>
+      </c>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="23"/>
+      <c r="K23" s="23"/>
+      <c r="L23" s="23"/>
+      <c r="M23" s="18">
+        <v>0</v>
+      </c>
+      <c r="N23" s="16"/>
+      <c r="O23" s="23"/>
+      <c r="P23" s="23"/>
+      <c r="Q23" s="23"/>
+      <c r="R23" s="23"/>
+      <c r="S23" s="23"/>
+      <c r="T23" s="23"/>
+      <c r="U23" s="23"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="B24" s="27"/>
+      <c r="C24" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23">
+        <v>0</v>
+      </c>
+      <c r="F24" s="23"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="23"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="23"/>
+      <c r="K24" s="23"/>
+      <c r="L24" s="23"/>
+      <c r="M24" s="18">
+        <v>0</v>
+      </c>
+      <c r="N24" s="16"/>
+      <c r="O24" s="23"/>
+      <c r="P24" s="23"/>
+      <c r="Q24" s="23"/>
+      <c r="R24" s="23"/>
+      <c r="S24" s="23"/>
+      <c r="T24" s="23"/>
+      <c r="U24" s="23"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A25" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="23"/>
+      <c r="C25" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23">
+        <f>VLOOKUP(A25,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>-0.9</v>
+      </c>
+      <c r="F25" s="23">
+        <v>-22.9</v>
+      </c>
+      <c r="G25" s="23">
+        <v>14.7</v>
+      </c>
+      <c r="H25" s="23"/>
+      <c r="I25" s="23">
+        <v>355.79</v>
+      </c>
+      <c r="J25" s="23"/>
+      <c r="K25" s="23"/>
+      <c r="L25" s="23"/>
+      <c r="M25" s="18"/>
+      <c r="N25" s="16" t="str">
+        <f>VLOOKUP(A25,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>4.2.1.11</v>
+      </c>
+      <c r="O25" s="23"/>
+      <c r="P25" s="23"/>
+      <c r="Q25" s="23"/>
+      <c r="R25" s="23"/>
+      <c r="S25" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="T25" s="23">
+        <v>2.67</v>
+      </c>
+      <c r="U25" s="23">
+        <v>2.67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A26" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="23"/>
+      <c r="C26" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="23"/>
+      <c r="E26" s="23">
+        <v>6.2290000000000001</v>
+      </c>
+      <c r="F26" s="23">
+        <v>-23.1</v>
+      </c>
+      <c r="G26" s="23">
+        <v>14.6</v>
+      </c>
+      <c r="H26" s="23"/>
+      <c r="I26" s="23"/>
+      <c r="J26" s="23">
+        <v>530</v>
+      </c>
+      <c r="K26" s="23"/>
+      <c r="L26" s="23"/>
+      <c r="M26" s="18"/>
+      <c r="N26" s="16" t="str">
+        <f>VLOOKUP(A26,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>5.4.2.1</v>
+      </c>
+      <c r="O26" s="23"/>
+      <c r="P26" s="23"/>
+      <c r="Q26" s="23"/>
+      <c r="R26" s="23"/>
+      <c r="S26" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="T26" s="23">
+        <v>2.67</v>
+      </c>
+      <c r="U26" s="23">
+        <v>2.67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A27" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="23"/>
+      <c r="C27" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23">
+        <v>-10.51</v>
+      </c>
+      <c r="F27" s="23">
+        <v>-19.2</v>
+      </c>
+      <c r="G27" s="23">
+        <v>56.1</v>
+      </c>
+      <c r="H27" s="24"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="23">
+        <v>654</v>
+      </c>
+      <c r="K27" s="23"/>
+      <c r="L27" s="23"/>
+      <c r="M27" s="18"/>
+      <c r="N27" s="16" t="str">
+        <f>VLOOKUP(A27,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>2.7.2.3</v>
+      </c>
+      <c r="O27" s="23"/>
+      <c r="P27" s="23"/>
+      <c r="Q27" s="23"/>
+      <c r="R27" s="23"/>
+      <c r="S27" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="T27" s="23">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="U27" s="23">
+        <v>0.39900000000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A28" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="23"/>
+      <c r="C28" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="D28" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E28" s="23">
+        <f>VLOOKUP(A28,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>-0.1</v>
+      </c>
+      <c r="F28" s="23">
+        <v>-12.8</v>
+      </c>
+      <c r="G28" s="23">
+        <v>62.6</v>
+      </c>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23">
+        <v>268</v>
+      </c>
+      <c r="J28" s="23"/>
+      <c r="K28" s="23"/>
+      <c r="L28" s="23"/>
+      <c r="M28" s="18"/>
+      <c r="N28" s="16" t="str">
+        <f>VLOOKUP(A28,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>1.2.1.12</v>
+      </c>
+      <c r="O28" s="23"/>
+      <c r="P28" s="23"/>
+      <c r="Q28" s="23"/>
+      <c r="R28" s="23"/>
+      <c r="S28" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="T28" s="23">
+        <v>2.13</v>
+      </c>
+      <c r="U28" s="23">
+        <v>2.13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A29" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" s="23"/>
+      <c r="C29" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29" s="23"/>
+      <c r="E29" s="17">
+        <v>7.5979999999999999</v>
+      </c>
+      <c r="F29" s="23">
+        <v>-24.3</v>
+      </c>
+      <c r="G29" s="23">
+        <v>13.4</v>
+      </c>
+      <c r="H29" s="23"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="23">
+        <v>9000</v>
+      </c>
+      <c r="K29" s="23"/>
+      <c r="L29" s="23"/>
+      <c r="M29" s="7"/>
+      <c r="N29" s="16" t="str">
+        <f>VLOOKUP(A29,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>5.3.1.1</v>
+      </c>
+      <c r="O29" s="23"/>
+      <c r="P29" s="23"/>
+      <c r="Q29" s="23"/>
+      <c r="R29" s="23"/>
+      <c r="S29" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="T29" s="23">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="U29" s="23">
+        <v>0.16700000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A30" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="23"/>
+      <c r="C30" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D30" s="23"/>
+      <c r="E30" s="23">
+        <f>VLOOKUP(A30,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>4.2</v>
+      </c>
+      <c r="F30" s="23">
+        <v>-29.4</v>
+      </c>
+      <c r="G30" s="23">
+        <v>27.1</v>
+      </c>
+      <c r="H30" s="24"/>
+      <c r="I30" s="23">
+        <v>8.5</v>
+      </c>
+      <c r="J30" s="23"/>
+      <c r="K30" s="23"/>
+      <c r="L30" s="23"/>
+      <c r="M30" s="18"/>
+      <c r="N30" s="16" t="str">
+        <f>VLOOKUP(A30,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>4.1.2.13</v>
+      </c>
+      <c r="O30" s="23"/>
+      <c r="P30" s="23"/>
+      <c r="Q30" s="23"/>
+      <c r="R30" s="23"/>
+      <c r="S30" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="T30" s="23">
+        <v>0.218</v>
+      </c>
+      <c r="U30" s="23">
+        <v>0.218</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A31" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="23"/>
+      <c r="C31" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" s="23">
+        <f>VLOOKUP(A31,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>-2.8</v>
+      </c>
+      <c r="F31" s="23">
+        <v>-48.8</v>
+      </c>
+      <c r="G31" s="23">
+        <v>-9.6999999999999993</v>
+      </c>
+      <c r="H31" s="23"/>
+      <c r="I31" s="23">
+        <v>22</v>
+      </c>
+      <c r="J31" s="23"/>
+      <c r="K31" s="23"/>
+      <c r="L31" s="23"/>
+      <c r="M31" s="18">
+        <v>0</v>
+      </c>
+      <c r="N31" s="16" t="str">
+        <f>VLOOKUP(A31,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>3.1.3.11</v>
+      </c>
+      <c r="O31" s="23"/>
+      <c r="P31" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q31" s="23"/>
+      <c r="R31" s="23">
+        <v>0.1</v>
+      </c>
+      <c r="S31" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="T31" s="23">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="U31" s="23">
+        <v>0.27200000000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A32" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B32" s="23"/>
+      <c r="C32" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" s="23"/>
+      <c r="E32" s="23">
+        <v>3.1320000000000001</v>
+      </c>
+      <c r="F32" s="23">
+        <v>-17.100000000000001</v>
+      </c>
+      <c r="G32" s="23">
+        <v>20.6</v>
+      </c>
+      <c r="H32" s="23"/>
+      <c r="I32" s="23">
+        <v>120</v>
+      </c>
+      <c r="J32" s="23"/>
+      <c r="K32" s="23"/>
+      <c r="L32" s="23"/>
+      <c r="M32" s="18">
+        <v>11.639423575531699</v>
+      </c>
+      <c r="N32" s="16" t="str">
+        <f>VLOOKUP(A32,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>5.3.1.9</v>
+      </c>
+      <c r="O32" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="P32" s="23"/>
+      <c r="Q32" s="23"/>
+      <c r="R32" s="23"/>
+      <c r="S32" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="T32" s="23">
+        <v>3.48</v>
+      </c>
+      <c r="U32" s="23">
+        <v>3.48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A33" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="B33" s="26"/>
+      <c r="C33" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="D33" s="23"/>
+      <c r="E33" s="23">
+        <v>0</v>
+      </c>
+      <c r="F33" s="23"/>
+      <c r="G33" s="23"/>
+      <c r="H33" s="23"/>
+      <c r="I33" s="23">
+        <v>1</v>
+      </c>
+      <c r="J33" s="23">
+        <v>0</v>
+      </c>
+      <c r="K33" s="23"/>
+      <c r="L33" s="24"/>
+      <c r="M33" s="23"/>
+      <c r="N33" s="23"/>
+      <c r="O33" s="23"/>
+      <c r="P33" s="23"/>
+      <c r="Q33" s="23"/>
+      <c r="R33" s="23"/>
+      <c r="S33" s="23"/>
+      <c r="T33" s="23"/>
+      <c r="U33" s="23"/>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A34" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" s="26"/>
+      <c r="C34" s="25" t="s">
+        <v>225</v>
+      </c>
+      <c r="D34" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="E34" s="23">
+        <v>0</v>
+      </c>
+      <c r="F34" s="23"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="23"/>
+      <c r="I34" s="17">
+        <v>2540</v>
+      </c>
+      <c r="J34" s="23">
+        <v>2540</v>
+      </c>
+      <c r="K34" s="23"/>
+      <c r="L34" s="24">
+        <v>1E-3</v>
+      </c>
+      <c r="M34" s="18">
+        <v>-8.5077261088811902</v>
+      </c>
+      <c r="N34" s="16"/>
+      <c r="O34" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="P34" s="23"/>
+      <c r="Q34" s="23"/>
+      <c r="R34" s="23"/>
+      <c r="S34" s="23"/>
+      <c r="T34" s="23"/>
+      <c r="U34" s="23"/>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A35" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="B35" s="27"/>
+      <c r="C35" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="D35" s="23"/>
+      <c r="E35" s="23">
+        <v>0</v>
+      </c>
+      <c r="F35" s="23"/>
+      <c r="G35" s="23"/>
+      <c r="H35" s="23"/>
+      <c r="I35" s="23">
+        <v>1</v>
+      </c>
+      <c r="J35" s="23">
+        <v>1</v>
+      </c>
+      <c r="K35" s="23"/>
+      <c r="L35" s="23"/>
+      <c r="M35" s="23"/>
+      <c r="N35" s="23"/>
+      <c r="O35" s="23"/>
+      <c r="P35" s="23"/>
+      <c r="Q35" s="23"/>
+      <c r="R35" s="23"/>
+      <c r="S35" s="23"/>
+      <c r="T35" s="23"/>
+      <c r="U35" s="23"/>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A36" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="B36" s="27"/>
+      <c r="C36" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="D36" s="23"/>
+      <c r="E36" s="23">
+        <v>0</v>
+      </c>
+      <c r="F36" s="23"/>
+      <c r="G36" s="23"/>
+      <c r="H36" s="23"/>
+      <c r="I36" s="23"/>
+      <c r="J36" s="23">
+        <v>1</v>
+      </c>
+      <c r="K36" s="23"/>
+      <c r="L36" s="23"/>
+      <c r="M36" s="23"/>
+      <c r="N36" s="23"/>
+      <c r="O36" s="23"/>
+      <c r="P36" s="23"/>
+      <c r="Q36" s="23"/>
+      <c r="R36" s="23"/>
+      <c r="S36" s="23"/>
+      <c r="T36" s="23"/>
+      <c r="U36" s="23"/>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B37" s="27"/>
+      <c r="C37" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D37" s="23"/>
+      <c r="E37" s="23">
+        <v>0</v>
+      </c>
+      <c r="F37" s="23"/>
+      <c r="G37" s="23"/>
+      <c r="H37" s="23"/>
+      <c r="I37" s="23"/>
+      <c r="J37" s="23"/>
+      <c r="K37" s="23"/>
+      <c r="L37" s="23"/>
+      <c r="M37" s="18">
+        <v>63.607356573910501</v>
+      </c>
+      <c r="N37" s="16"/>
+      <c r="O37" s="23"/>
+      <c r="P37" s="23"/>
+      <c r="Q37" s="23"/>
+      <c r="R37" s="23"/>
+      <c r="S37" s="23"/>
+      <c r="T37" s="23"/>
+      <c r="U37" s="23"/>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A38" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="B38" s="26"/>
+      <c r="C38" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="D38" s="23"/>
+      <c r="E38" s="23">
+        <v>0</v>
+      </c>
+      <c r="F38" s="23"/>
+      <c r="G38" s="23"/>
+      <c r="H38" s="23"/>
+      <c r="I38" s="24">
+        <v>100</v>
+      </c>
+      <c r="J38" s="24">
+        <v>100</v>
+      </c>
+      <c r="K38" s="23"/>
+      <c r="L38" s="23"/>
+      <c r="M38" s="18">
+        <v>8.5514960440672301</v>
+      </c>
+      <c r="N38" s="16"/>
+      <c r="O38" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="P38" s="23"/>
+      <c r="Q38" s="23"/>
+      <c r="R38" s="23"/>
+      <c r="S38" s="23"/>
+      <c r="T38" s="23"/>
+      <c r="U38" s="23"/>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A39" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="B39" s="26"/>
+      <c r="C39" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="D39" s="23"/>
+      <c r="E39" s="23">
+        <f>VLOOKUP(A39,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="F39" s="23"/>
+      <c r="G39" s="23"/>
+      <c r="H39" s="23"/>
+      <c r="I39" s="23">
+        <v>1</v>
+      </c>
+      <c r="J39" s="23">
+        <v>2</v>
+      </c>
+      <c r="K39" s="23"/>
+      <c r="L39" s="23"/>
+      <c r="M39" s="18">
+        <v>-13.3040694607334</v>
+      </c>
+      <c r="N39" s="16"/>
+      <c r="O39" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="P39" s="23"/>
+      <c r="Q39" s="23"/>
+      <c r="R39" s="23"/>
+      <c r="S39" s="23"/>
+      <c r="T39" s="23"/>
+      <c r="U39" s="23"/>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A40" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B40" s="27"/>
+      <c r="C40" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D40" s="23"/>
+      <c r="E40" s="23">
+        <v>0</v>
+      </c>
+      <c r="F40" s="23"/>
+      <c r="G40" s="23"/>
+      <c r="H40" s="23"/>
+      <c r="I40" s="23"/>
+      <c r="J40" s="23"/>
+      <c r="K40" s="23"/>
+      <c r="L40" s="23"/>
+      <c r="M40" s="18">
+        <v>13.304069460733899</v>
+      </c>
+      <c r="N40" s="16"/>
+      <c r="O40" s="23"/>
+      <c r="P40" s="23"/>
+      <c r="Q40" s="23"/>
+      <c r="R40" s="23"/>
+      <c r="S40" s="23"/>
+      <c r="T40" s="23"/>
+      <c r="U40" s="23"/>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A41" s="23" t="s">
+        <v>214</v>
+      </c>
+      <c r="B41" s="23"/>
+      <c r="C41" s="23" t="s">
+        <v>215</v>
+      </c>
+      <c r="D41" s="23"/>
+      <c r="E41" s="23">
+        <f>VLOOKUP(A41,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>1.3</v>
+      </c>
+      <c r="F41" s="23"/>
+      <c r="G41" s="23"/>
+      <c r="H41" s="23"/>
+      <c r="I41" s="23">
+        <f>VLOOKUP($A41,[1]ecoliN1!$A$2:$J$84,9,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="J41" s="23">
+        <f>VLOOKUP($A41,[1]ecoliN1!$A$2:$J$84,10,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="K41" s="23"/>
+      <c r="L41" s="23"/>
+      <c r="M41" s="23"/>
+      <c r="N41" s="23"/>
+      <c r="O41" s="23"/>
+      <c r="P41" s="23"/>
+      <c r="Q41" s="23"/>
+      <c r="R41" s="23"/>
+      <c r="S41" s="23"/>
+      <c r="T41" s="23"/>
+      <c r="U41" s="23"/>
+    </row>
+    <row r="42" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="B42" s="26"/>
+      <c r="C42" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="E42" s="23">
+        <f>VLOOKUP(A42,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="I42" s="24">
+        <v>100</v>
+      </c>
+      <c r="J42" s="24">
+        <v>100</v>
+      </c>
+      <c r="M42" s="18">
+        <v>8.5514960440672301</v>
+      </c>
+      <c r="N42" s="16"/>
+      <c r="O42" s="24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B43" s="27"/>
+      <c r="C43" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E43" s="23">
+        <v>0</v>
+      </c>
+      <c r="M43" s="18">
+        <v>-8.5514960440672301</v>
+      </c>
+      <c r="N43" s="16"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="23">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5" s="24">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="24">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="B7" s="24">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="B8" s="24">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="B9" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="23" t="s">
+        <v>208</v>
+      </c>
+      <c r="B10" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="23" t="s">
+        <v>209</v>
+      </c>
+      <c r="B11" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="23" t="s">
+        <v>210</v>
+      </c>
+      <c r="B12" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="23" t="s">
+        <v>211</v>
+      </c>
+      <c r="B13" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>93</v>
+      </c>
+      <c r="B14" s="24">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>226</v>
+      </c>
+      <c r="B15" s="24">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:XFD67"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
new model with pp and ed pathway
</commit_message>
<xml_diff>
--- a/KineticModel/data/gtoyall.xlsx
+++ b/KineticModel/data/gtoyall.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17127"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shyam\Documents\Courses\CHE1125Project\IntegratedModels\KineticModel\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shyam\Documents\Courses\CHE1125Project\IntegratedModels\KineticModel\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25590" windowHeight="7875" firstSheet="1" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25590" windowHeight="7875" firstSheet="3" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="gtoy1" sheetId="2" r:id="rId1"/>
@@ -24,16 +24,17 @@
     <sheet name="gtoy5C" sheetId="11" r:id="rId10"/>
     <sheet name="gtoy6" sheetId="12" r:id="rId11"/>
     <sheet name="gtoy6C" sheetId="13" r:id="rId12"/>
-    <sheet name="gtoy7" sheetId="16" r:id="rId13"/>
-    <sheet name="gtoy7C" sheetId="17" r:id="rId14"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId15"/>
+    <sheet name="gtoy8" sheetId="18" r:id="rId13"/>
+    <sheet name="gtoy8C" sheetId="19" r:id="rId14"/>
+    <sheet name="gtoy7" sheetId="16" r:id="rId15"/>
+    <sheet name="gtoy7C" sheetId="17" r:id="rId16"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId17"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId16"/>
-    <externalReference r:id="rId17"/>
+    <externalReference r:id="rId18"/>
+    <externalReference r:id="rId19"/>
   </externalReferences>
-  <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="256">
   <si>
     <t>Enzymes</t>
   </si>
@@ -751,6 +752,87 @@
   </si>
   <si>
     <t>[c] : succ + coa &lt;==&gt; succoa + pi</t>
+  </si>
+  <si>
+    <t>G6PDH2r</t>
+  </si>
+  <si>
+    <t>1.1.1.49</t>
+  </si>
+  <si>
+    <t>0.174,0.0075,1,1,1</t>
+  </si>
+  <si>
+    <t>PGL</t>
+  </si>
+  <si>
+    <t>[c] : 6pgl + h2o --&gt; 6pgc + h</t>
+  </si>
+  <si>
+    <t>h2o,h</t>
+  </si>
+  <si>
+    <t>3.1.1.31</t>
+  </si>
+  <si>
+    <t>GND</t>
+  </si>
+  <si>
+    <t>1.1.1.44</t>
+  </si>
+  <si>
+    <t>RPE</t>
+  </si>
+  <si>
+    <t>[c] : ru5p-D &lt;==&gt; xu5p-D</t>
+  </si>
+  <si>
+    <t>5.1.3.1</t>
+  </si>
+  <si>
+    <t>RPI</t>
+  </si>
+  <si>
+    <t>[c] : r5p &lt;==&gt; ru5p-D</t>
+  </si>
+  <si>
+    <t>5.3.1.6</t>
+  </si>
+  <si>
+    <t>TKT1</t>
+  </si>
+  <si>
+    <t>[c] : g3p + s7p &lt;==&gt; r5p + xu5p-D</t>
+  </si>
+  <si>
+    <t>2.2.1.1</t>
+  </si>
+  <si>
+    <t>TALA</t>
+  </si>
+  <si>
+    <t>[c] : g3p + s7p &lt;==&gt; e4p + f6p</t>
+  </si>
+  <si>
+    <t>2.2.1.2</t>
+  </si>
+  <si>
+    <t>TKT2</t>
+  </si>
+  <si>
+    <t>[c] : f6p + g3p &lt;==&gt; e4p + xu5p-D</t>
+  </si>
+  <si>
+    <t>[c] : g6p ---&gt; 6pgl + h</t>
+  </si>
+  <si>
+    <t>[c] : 6pgc ---&gt; ru5p-D</t>
+  </si>
+  <si>
+    <t>[c] : 1.496 3pg + 3.7478 accoa + 0.3610 e4p + 0.0709 f6p + 0.1290 g3p + 0.2050 g6p + 59.8100 h2o + 1.7867 oaa + 0.5191 pep + 2.8328 pyr + 0.8977 r5p --&gt; 4.1182 akg + 3.7478 coa + 59.8100 h</t>
+  </si>
+  <si>
+    <t>biomass</t>
   </si>
 </sst>
 </file>
@@ -816,7 +898,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -840,6 +922,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -854,7 +942,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -884,6 +972,25 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -928,14 +1035,14 @@
       <sheetName val="red_test2"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
       <sheetData sheetId="8">
         <row r="2">
           <cell r="A2" t="str">
@@ -979,6 +1086,7 @@
           <cell r="D3" t="str">
             <v>Transport, Extracellular</v>
           </cell>
+          <cell r="E3"/>
           <cell r="F3">
             <v>0</v>
           </cell>
@@ -1092,6 +1200,7 @@
           <cell r="D7" t="str">
             <v>Transport, Extracellular</v>
           </cell>
+          <cell r="E7"/>
           <cell r="F7">
             <v>0</v>
           </cell>
@@ -1147,6 +1256,7 @@
           <cell r="D9" t="str">
             <v>Citric Acid Cycle</v>
           </cell>
+          <cell r="E9"/>
           <cell r="F9">
             <v>-8.3000000000000007</v>
           </cell>
@@ -1173,6 +1283,7 @@
           <cell r="D10" t="str">
             <v>Transport, Extracellular</v>
           </cell>
+          <cell r="E10"/>
           <cell r="F10">
             <v>0</v>
           </cell>
@@ -1228,6 +1339,7 @@
           <cell r="D12" t="str">
             <v>Oxidative Phosphorylation</v>
           </cell>
+          <cell r="E12"/>
           <cell r="F12">
             <v>-6.6</v>
           </cell>
@@ -1280,6 +1392,10 @@
           <cell r="C14" t="str">
             <v>[c] : (1.496) 3pg + (3.7478) accoa + (59.8100) atp + (0.3610) e4p + (0.0709) f6p + (0.1290) g3p + (0.2050) g6p + (0.2557) gln-L + (4.9414) glu-L + (59.8100) h2o + (3.5470) nad + (13.0279) nadph + (1.7867) oaa + (0.5191) pep + (2.8328) pyr + (0.8977) r5p --&gt; (59.8100) adp + (4.1182) akg + (3.7478) coa + (59.8100) h + (3.5470) nadh + (13.0279) nadp + (59.8100) pi</v>
           </cell>
+          <cell r="D14"/>
+          <cell r="E14"/>
+          <cell r="F14"/>
+          <cell r="G14"/>
           <cell r="H14">
             <v>0.87390000000000001</v>
           </cell>
@@ -1300,6 +1416,7 @@
           <cell r="D15" t="str">
             <v>Transport, Extracellular</v>
           </cell>
+          <cell r="E15"/>
           <cell r="F15">
             <v>0</v>
           </cell>
@@ -1326,6 +1443,7 @@
           <cell r="D16" t="str">
             <v>Citric Acid Cycle</v>
           </cell>
+          <cell r="E16"/>
           <cell r="F16">
             <v>-8.6</v>
           </cell>
@@ -1352,6 +1470,7 @@
           <cell r="D17" t="str">
             <v>Oxidative Phosphorylation</v>
           </cell>
+          <cell r="E17"/>
           <cell r="F17">
             <v>-37.200000000000003</v>
           </cell>
@@ -1378,6 +1497,7 @@
           <cell r="D18" t="str">
             <v>Transport, Extracellular</v>
           </cell>
+          <cell r="E18"/>
           <cell r="F18">
             <v>0</v>
           </cell>
@@ -1433,6 +1553,7 @@
           <cell r="D20" t="str">
             <v>Transport, Extracellular</v>
           </cell>
+          <cell r="E20"/>
           <cell r="F20">
             <v>0</v>
           </cell>
@@ -1459,6 +1580,9 @@
           <cell r="D21" t="str">
             <v>Exchange</v>
           </cell>
+          <cell r="E21"/>
+          <cell r="F21"/>
+          <cell r="G21"/>
           <cell r="H21">
             <v>0</v>
           </cell>
@@ -1479,6 +1603,9 @@
           <cell r="D22" t="str">
             <v>Exchange</v>
           </cell>
+          <cell r="E22"/>
+          <cell r="F22"/>
+          <cell r="G22"/>
           <cell r="H22">
             <v>0</v>
           </cell>
@@ -1499,6 +1626,9 @@
           <cell r="D23" t="str">
             <v>Exchange</v>
           </cell>
+          <cell r="E23"/>
+          <cell r="F23"/>
+          <cell r="G23"/>
           <cell r="H23">
             <v>0</v>
           </cell>
@@ -1519,6 +1649,9 @@
           <cell r="D24" t="str">
             <v>Exchange</v>
           </cell>
+          <cell r="E24"/>
+          <cell r="F24"/>
+          <cell r="G24"/>
           <cell r="H24">
             <v>22.809799999999999</v>
           </cell>
@@ -1539,6 +1672,9 @@
           <cell r="D25" t="str">
             <v>Exchange</v>
           </cell>
+          <cell r="E25"/>
+          <cell r="F25"/>
+          <cell r="G25"/>
           <cell r="H25">
             <v>0</v>
           </cell>
@@ -1559,6 +1695,9 @@
           <cell r="D26" t="str">
             <v>Exchange</v>
           </cell>
+          <cell r="E26"/>
+          <cell r="F26"/>
+          <cell r="G26"/>
           <cell r="H26">
             <v>0</v>
           </cell>
@@ -1579,6 +1718,9 @@
           <cell r="D27" t="str">
             <v>Exchange</v>
           </cell>
+          <cell r="E27"/>
+          <cell r="F27"/>
+          <cell r="G27"/>
           <cell r="H27">
             <v>0</v>
           </cell>
@@ -1599,6 +1741,9 @@
           <cell r="D28" t="str">
             <v>Exchange</v>
           </cell>
+          <cell r="E28"/>
+          <cell r="F28"/>
+          <cell r="G28"/>
           <cell r="H28">
             <v>0</v>
           </cell>
@@ -1619,6 +1764,9 @@
           <cell r="D29" t="str">
             <v>Exchange</v>
           </cell>
+          <cell r="E29"/>
+          <cell r="F29"/>
+          <cell r="G29"/>
           <cell r="H29">
             <v>-10</v>
           </cell>
@@ -1639,6 +1787,9 @@
           <cell r="D30" t="str">
             <v>Exchange</v>
           </cell>
+          <cell r="E30"/>
+          <cell r="F30"/>
+          <cell r="G30"/>
           <cell r="H30">
             <v>0</v>
           </cell>
@@ -1659,6 +1810,9 @@
           <cell r="D31" t="str">
             <v>Exchange</v>
           </cell>
+          <cell r="E31"/>
+          <cell r="F31"/>
+          <cell r="G31"/>
           <cell r="H31">
             <v>0</v>
           </cell>
@@ -1679,6 +1833,9 @@
           <cell r="D32" t="str">
             <v>Exchange</v>
           </cell>
+          <cell r="E32"/>
+          <cell r="F32"/>
+          <cell r="G32"/>
           <cell r="H32">
             <v>17.530899999999999</v>
           </cell>
@@ -1699,6 +1856,9 @@
           <cell r="D33" t="str">
             <v>Exchange</v>
           </cell>
+          <cell r="E33"/>
+          <cell r="F33"/>
+          <cell r="G33"/>
           <cell r="H33">
             <v>29.175799999999999</v>
           </cell>
@@ -1719,6 +1879,9 @@
           <cell r="D34" t="str">
             <v>Exchange</v>
           </cell>
+          <cell r="E34"/>
+          <cell r="F34"/>
+          <cell r="G34"/>
           <cell r="H34">
             <v>0</v>
           </cell>
@@ -1739,6 +1902,9 @@
           <cell r="D35" t="str">
             <v>Exchange</v>
           </cell>
+          <cell r="E35"/>
+          <cell r="F35"/>
+          <cell r="G35"/>
           <cell r="H35">
             <v>0</v>
           </cell>
@@ -1759,6 +1925,9 @@
           <cell r="D36" t="str">
             <v>Exchange</v>
           </cell>
+          <cell r="E36"/>
+          <cell r="F36"/>
+          <cell r="G36"/>
           <cell r="H36">
             <v>-4.7652999999999999</v>
           </cell>
@@ -1779,6 +1948,9 @@
           <cell r="D37" t="str">
             <v>Exchange</v>
           </cell>
+          <cell r="E37"/>
+          <cell r="F37"/>
+          <cell r="G37"/>
           <cell r="H37">
             <v>-21.799499999999998</v>
           </cell>
@@ -1799,6 +1971,9 @@
           <cell r="D38" t="str">
             <v>Exchange</v>
           </cell>
+          <cell r="E38"/>
+          <cell r="F38"/>
+          <cell r="G38"/>
           <cell r="H38">
             <v>-3.2149000000000001</v>
           </cell>
@@ -1819,6 +1994,9 @@
           <cell r="D39" t="str">
             <v>Exchange</v>
           </cell>
+          <cell r="E39"/>
+          <cell r="F39"/>
+          <cell r="G39"/>
           <cell r="H39">
             <v>0</v>
           </cell>
@@ -1839,6 +2017,9 @@
           <cell r="D40" t="str">
             <v>Exchange</v>
           </cell>
+          <cell r="E40"/>
+          <cell r="F40"/>
+          <cell r="G40"/>
           <cell r="H40">
             <v>0</v>
           </cell>
@@ -1917,6 +2098,7 @@
           <cell r="D43" t="str">
             <v>Transport, Extracellular</v>
           </cell>
+          <cell r="E43"/>
           <cell r="F43">
             <v>0</v>
           </cell>
@@ -1943,6 +2125,7 @@
           <cell r="D44" t="str">
             <v>Transport, Extracellular</v>
           </cell>
+          <cell r="E44"/>
           <cell r="F44">
             <v>0</v>
           </cell>
@@ -1998,6 +2181,7 @@
           <cell r="D46" t="str">
             <v>Transport, Extracellular</v>
           </cell>
+          <cell r="E46"/>
           <cell r="F46">
             <v>-9.1</v>
           </cell>
@@ -2053,6 +2237,7 @@
           <cell r="D48" t="str">
             <v>Transport, Extracellular</v>
           </cell>
+          <cell r="E48"/>
           <cell r="F48">
             <v>0</v>
           </cell>
@@ -2137,6 +2322,7 @@
           <cell r="D51" t="str">
             <v>Transport, Extracellular</v>
           </cell>
+          <cell r="E51"/>
           <cell r="F51">
             <v>-9.1</v>
           </cell>
@@ -2192,6 +2378,7 @@
           <cell r="D53" t="str">
             <v>Transport, Extracellular</v>
           </cell>
+          <cell r="E53"/>
           <cell r="F53">
             <v>-6.6</v>
           </cell>
@@ -2305,6 +2492,7 @@
           <cell r="D57" t="str">
             <v>Transport, Extracellular</v>
           </cell>
+          <cell r="E57"/>
           <cell r="F57">
             <v>0</v>
           </cell>
@@ -2360,6 +2548,7 @@
           <cell r="D59" t="str">
             <v>Transport, Extracellular</v>
           </cell>
+          <cell r="E59"/>
           <cell r="F59">
             <v>0</v>
           </cell>
@@ -2502,6 +2691,7 @@
           <cell r="D64" t="str">
             <v>Transport, Extracellular</v>
           </cell>
+          <cell r="E64"/>
           <cell r="F64">
             <v>0</v>
           </cell>
@@ -2673,6 +2863,7 @@
           <cell r="D70" t="str">
             <v>Inorganic Ion Transport and Metabolism</v>
           </cell>
+          <cell r="E70"/>
           <cell r="F70">
             <v>0</v>
           </cell>
@@ -2699,6 +2890,7 @@
           <cell r="D71" t="str">
             <v>Transport, Extracellular</v>
           </cell>
+          <cell r="E71"/>
           <cell r="F71">
             <v>0</v>
           </cell>
@@ -2725,6 +2917,7 @@
           <cell r="D72" t="str">
             <v>Glycolysis/Gluconeogenesis</v>
           </cell>
+          <cell r="E72"/>
           <cell r="F72">
             <v>-8.3000000000000007</v>
           </cell>
@@ -2780,6 +2973,7 @@
           <cell r="D74" t="str">
             <v>Pyruvate Metabolism</v>
           </cell>
+          <cell r="E74"/>
           <cell r="F74">
             <v>-5.0999999999999996</v>
           </cell>
@@ -2922,6 +3116,7 @@
           <cell r="D79" t="str">
             <v>Inorganic Ion Transport and Metabolism</v>
           </cell>
+          <cell r="E79"/>
           <cell r="F79">
             <v>0</v>
           </cell>
@@ -3155,6 +3350,7 @@
           <cell r="A5" t="str">
             <v>FBP</v>
           </cell>
+          <cell r="B5"/>
           <cell r="C5" t="str">
             <v>[c] : fdp + h2o --&gt; f6p + pi</v>
           </cell>
@@ -3170,17 +3366,21 @@
           <cell r="G5">
             <v>-9.6999999999999993</v>
           </cell>
+          <cell r="H5"/>
           <cell r="I5">
             <v>22</v>
           </cell>
+          <cell r="J5"/>
         </row>
         <row r="6">
           <cell r="A6" t="str">
             <v>FBA</v>
           </cell>
+          <cell r="B6"/>
           <cell r="C6" t="str">
             <v>[c] : fdp &lt;==&gt; dhap + g3p</v>
           </cell>
+          <cell r="D6"/>
           <cell r="E6">
             <v>4.2</v>
           </cell>
@@ -3190,17 +3390,21 @@
           <cell r="G6">
             <v>27.1</v>
           </cell>
+          <cell r="H6"/>
           <cell r="I6">
             <v>8.5</v>
           </cell>
+          <cell r="J6"/>
         </row>
         <row r="7">
           <cell r="A7" t="str">
             <v>TPI</v>
           </cell>
+          <cell r="B7"/>
           <cell r="C7" t="str">
             <v>[c] : g3p &lt;==&gt; dhap</v>
           </cell>
+          <cell r="D7"/>
           <cell r="E7">
             <v>7.5979999999999999</v>
           </cell>
@@ -3210,6 +3414,8 @@
           <cell r="G7">
             <v>13.4</v>
           </cell>
+          <cell r="H7"/>
+          <cell r="I7"/>
           <cell r="J7">
             <v>9000</v>
           </cell>
@@ -3218,6 +3424,7 @@
           <cell r="A8" t="str">
             <v>GAPD</v>
           </cell>
+          <cell r="B8"/>
           <cell r="C8" t="str">
             <v>[c] : g3p + nad + pi &lt;==&gt; 13dpg + h + nadh</v>
           </cell>
@@ -3233,17 +3440,21 @@
           <cell r="G8">
             <v>62.6</v>
           </cell>
+          <cell r="H8"/>
           <cell r="I8">
             <v>268</v>
           </cell>
+          <cell r="J8"/>
         </row>
         <row r="9">
           <cell r="A9" t="str">
             <v>PGK</v>
           </cell>
+          <cell r="B9"/>
           <cell r="C9" t="str">
             <v>[c] : 3pg + atp &lt;==&gt; 13dpg + adp</v>
           </cell>
+          <cell r="D9"/>
           <cell r="E9">
             <v>-10.51</v>
           </cell>
@@ -3253,6 +3464,8 @@
           <cell r="G9">
             <v>56.1</v>
           </cell>
+          <cell r="H9"/>
+          <cell r="I9"/>
           <cell r="J9">
             <v>654</v>
           </cell>
@@ -3261,9 +3474,11 @@
           <cell r="A10" t="str">
             <v>PGM</v>
           </cell>
+          <cell r="B10"/>
           <cell r="C10" t="str">
             <v>[c] : 2pg &lt;==&gt; 3pg</v>
           </cell>
+          <cell r="D10"/>
           <cell r="E10">
             <v>6.2290000000000001</v>
           </cell>
@@ -3273,6 +3488,8 @@
           <cell r="G10">
             <v>14.6</v>
           </cell>
+          <cell r="H10"/>
+          <cell r="I10"/>
           <cell r="J10">
             <v>530</v>
           </cell>
@@ -3281,9 +3498,11 @@
           <cell r="A11" t="str">
             <v>ENO</v>
           </cell>
+          <cell r="B11"/>
           <cell r="C11" t="str">
             <v>[c] : 2pg &lt;==&gt; h2o + pep</v>
           </cell>
+          <cell r="D11"/>
           <cell r="E11">
             <v>-0.9</v>
           </cell>
@@ -3293,9 +3512,11 @@
           <cell r="G11">
             <v>14.7</v>
           </cell>
+          <cell r="H11"/>
           <cell r="I11">
             <v>355.79</v>
           </cell>
+          <cell r="J11"/>
         </row>
         <row r="12">
           <cell r="A12" t="str">
@@ -3316,6 +3537,7 @@
           <cell r="G12">
             <v>65.3</v>
           </cell>
+          <cell r="H12"/>
           <cell r="I12">
             <v>2540</v>
           </cell>
@@ -3324,6 +3546,7 @@
           <cell r="A13" t="str">
             <v>PPS</v>
           </cell>
+          <cell r="B13"/>
           <cell r="C13" t="str">
             <v>[c] : atp + h2o + pyr --&gt; amp + 2 h + pep + pi</v>
           </cell>
@@ -3339,14 +3562,17 @@
           <cell r="G13">
             <v>24.4</v>
           </cell>
+          <cell r="H13"/>
           <cell r="I13">
             <v>1</v>
           </cell>
+          <cell r="J13"/>
         </row>
         <row r="14">
           <cell r="A14" t="str">
             <v>PDH</v>
           </cell>
+          <cell r="B14"/>
           <cell r="C14" t="str">
             <v>[c] : coa + nad + pyr --&gt; accoa + co2 + nadh</v>
           </cell>
@@ -3362,17 +3588,21 @@
           <cell r="G14">
             <v>2.2999999999999998</v>
           </cell>
+          <cell r="H14"/>
           <cell r="I14">
             <v>6.32</v>
           </cell>
+          <cell r="J14"/>
         </row>
         <row r="15">
           <cell r="A15" t="str">
             <v>CS</v>
           </cell>
+          <cell r="B15"/>
           <cell r="C15" t="str">
             <v>[c] : cit + coa + h &lt;==&gt; accoa + h2o + oaa</v>
           </cell>
+          <cell r="D15"/>
           <cell r="E15">
             <v>8.6</v>
           </cell>
@@ -3382,6 +3612,8 @@
           <cell r="G15">
             <v>60.9</v>
           </cell>
+          <cell r="H15"/>
+          <cell r="I15"/>
           <cell r="J15">
             <v>81</v>
           </cell>
@@ -3390,9 +3622,11 @@
           <cell r="A16" t="str">
             <v>ACONTa</v>
           </cell>
+          <cell r="B16"/>
           <cell r="C16" t="str">
             <v>[c] : cit &lt;==&gt; icit</v>
           </cell>
+          <cell r="D16"/>
           <cell r="E16">
             <v>1.5</v>
           </cell>
@@ -3402,14 +3636,17 @@
           <cell r="G16">
             <v>26.5</v>
           </cell>
+          <cell r="H16"/>
           <cell r="I16">
             <v>5.3</v>
           </cell>
+          <cell r="J16"/>
         </row>
         <row r="17">
           <cell r="A17" t="str">
             <v>ICDHyr</v>
           </cell>
+          <cell r="B17"/>
           <cell r="C17" t="str">
             <v>[c] : icit + nadp &lt;==&gt; akg + co2 + nadph</v>
           </cell>
@@ -3425,17 +3662,21 @@
           <cell r="G17">
             <v>26.9</v>
           </cell>
+          <cell r="H17"/>
           <cell r="I17">
             <v>106.4</v>
           </cell>
+          <cell r="J17"/>
         </row>
         <row r="18">
           <cell r="A18" t="str">
             <v>ICL</v>
           </cell>
+          <cell r="B18"/>
           <cell r="C18" t="str">
             <v>[c] : icit --&gt; glx + succ</v>
           </cell>
+          <cell r="D18"/>
           <cell r="E18">
             <v>4.9000000000000004</v>
           </cell>
@@ -3445,14 +3686,17 @@
           <cell r="G18">
             <v>17.8</v>
           </cell>
+          <cell r="H18"/>
           <cell r="I18">
             <v>5.2</v>
           </cell>
+          <cell r="J18"/>
         </row>
         <row r="19">
           <cell r="A19" t="str">
             <v>MALS</v>
           </cell>
+          <cell r="B19"/>
           <cell r="C19" t="str">
             <v>[c] : coa + h + mal &lt;==&gt; accoa + glx + h2o</v>
           </cell>
@@ -3468,6 +3712,8 @@
           <cell r="G19">
             <v>63.1</v>
           </cell>
+          <cell r="H19"/>
+          <cell r="I19"/>
           <cell r="J19">
             <v>48.1</v>
           </cell>
@@ -3476,6 +3722,7 @@
           <cell r="A20" t="str">
             <v>AKGDH</v>
           </cell>
+          <cell r="B20"/>
           <cell r="C20" t="str">
             <v>[c] : akg + coa + nad --&gt; co2 + nadh + succoa</v>
           </cell>
@@ -3491,20 +3738,24 @@
           <cell r="G20">
             <v>20.3</v>
           </cell>
+          <cell r="H20"/>
           <cell r="I20">
             <v>49</v>
           </cell>
+          <cell r="J20"/>
         </row>
         <row r="21">
           <cell r="A21" t="str">
             <v>SUCOAS</v>
           </cell>
+          <cell r="B21"/>
           <cell r="C21" t="str">
             <v>[c] : atp + coa + succ &lt;==&gt; adp + pi + succoa</v>
           </cell>
           <cell r="D21" t="str">
             <v>pi</v>
           </cell>
+          <cell r="E21"/>
           <cell r="F21">
             <v>-39.5</v>
           </cell>
@@ -3517,14 +3768,17 @@
           <cell r="I21">
             <v>44.73</v>
           </cell>
+          <cell r="J21"/>
         </row>
         <row r="22">
           <cell r="A22" t="str">
             <v>SUCDi</v>
           </cell>
+          <cell r="B22"/>
           <cell r="C22" t="str">
             <v>[c] : q8 + succ --&gt; fum + q8h2</v>
           </cell>
+          <cell r="D22"/>
           <cell r="E22">
             <v>-2.1</v>
           </cell>
@@ -3534,17 +3788,21 @@
           <cell r="G22">
             <v>16.100000000000001</v>
           </cell>
+          <cell r="H22"/>
           <cell r="I22">
             <v>24</v>
           </cell>
+          <cell r="J22"/>
         </row>
         <row r="23">
           <cell r="A23" t="str">
             <v>FRD7</v>
           </cell>
+          <cell r="B23"/>
           <cell r="C23" t="str">
             <v>[c] : q8 + succ &lt;==&gt; fum + q8h2</v>
           </cell>
+          <cell r="D23"/>
           <cell r="E23">
             <v>-5.9</v>
           </cell>
@@ -3554,17 +3812,21 @@
           <cell r="G23">
             <v>16.100000000000001</v>
           </cell>
+          <cell r="H23"/>
           <cell r="I23">
             <v>250</v>
           </cell>
+          <cell r="J23"/>
         </row>
         <row r="24">
           <cell r="A24" t="str">
             <v>FUM</v>
           </cell>
+          <cell r="B24"/>
           <cell r="C24" t="str">
             <v>[c] : mal &lt;==&gt; fum + h2o</v>
           </cell>
+          <cell r="D24"/>
           <cell r="E24">
             <v>0.6</v>
           </cell>
@@ -3574,14 +3836,17 @@
           <cell r="G24">
             <v>22.3</v>
           </cell>
+          <cell r="H24"/>
           <cell r="I24">
             <v>51.7</v>
           </cell>
+          <cell r="J24"/>
         </row>
         <row r="25">
           <cell r="A25" t="str">
             <v>MDH</v>
           </cell>
+          <cell r="B25"/>
           <cell r="C25" t="str">
             <v>[c] : mal + nad &lt;==&gt; h + nadh + oaa</v>
           </cell>
@@ -3597,17 +3862,21 @@
           <cell r="G25">
             <v>68.599999999999994</v>
           </cell>
+          <cell r="H25"/>
           <cell r="I25">
             <v>931</v>
           </cell>
+          <cell r="J25"/>
         </row>
         <row r="26">
           <cell r="A26" t="str">
             <v>PFL</v>
           </cell>
+          <cell r="B26"/>
           <cell r="C26" t="str">
             <v>[c] : accoa + for &lt;==&gt; coa + pyr</v>
           </cell>
+          <cell r="D26"/>
           <cell r="E26">
             <v>5.0999999999999996</v>
           </cell>
@@ -3617,14 +3886,17 @@
           <cell r="G26">
             <v>51.5</v>
           </cell>
+          <cell r="H26"/>
           <cell r="I26">
             <v>12.8</v>
           </cell>
+          <cell r="J26"/>
         </row>
         <row r="27">
           <cell r="A27" t="str">
             <v>LDH_D</v>
           </cell>
+          <cell r="B27"/>
           <cell r="C27" t="str">
             <v>[c] : lac + nad &lt;==&gt; h + nadh + pyr</v>
           </cell>
@@ -3640,14 +3912,17 @@
           <cell r="G27">
             <v>62.1</v>
           </cell>
+          <cell r="H27"/>
           <cell r="I27">
             <v>320</v>
           </cell>
+          <cell r="J27"/>
         </row>
         <row r="28">
           <cell r="A28" t="str">
             <v>PTAr</v>
           </cell>
+          <cell r="B28"/>
           <cell r="C28" t="str">
             <v>[c] : accoa + pi &lt;==&gt; actp + coa</v>
           </cell>
@@ -3663,6 +3938,7 @@
           <cell r="G28">
             <v>28.7</v>
           </cell>
+          <cell r="H28"/>
           <cell r="I28">
             <v>120</v>
           </cell>
@@ -3674,9 +3950,11 @@
           <cell r="A29" t="str">
             <v>ACKr</v>
           </cell>
+          <cell r="B29"/>
           <cell r="C29" t="str">
             <v>[c] : ac + atp &lt;==&gt; actp + adp</v>
           </cell>
+          <cell r="D29"/>
           <cell r="E29">
             <v>4.3</v>
           </cell>
@@ -3686,14 +3964,17 @@
           <cell r="G29">
             <v>52.1</v>
           </cell>
+          <cell r="H29"/>
           <cell r="I29">
             <v>280</v>
           </cell>
+          <cell r="J29"/>
         </row>
         <row r="30">
           <cell r="A30" t="str">
             <v>ACALD</v>
           </cell>
+          <cell r="B30"/>
           <cell r="C30" t="str">
             <v>[c] : acald + coa + nad &lt;==&gt; accoa + h + nadh</v>
           </cell>
@@ -3709,20 +3990,24 @@
           <cell r="G30">
             <v>49.2</v>
           </cell>
+          <cell r="H30"/>
           <cell r="I30">
             <v>15.7</v>
           </cell>
+          <cell r="J30"/>
         </row>
         <row r="31">
           <cell r="A31" t="str">
             <v>ALCD2x</v>
           </cell>
+          <cell r="B31"/>
           <cell r="C31" t="str">
             <v>[c] : etoh + nad &lt;==&gt; acald + h + nadh</v>
           </cell>
           <cell r="D31" t="str">
             <v>h</v>
           </cell>
+          <cell r="E31"/>
           <cell r="F31">
             <v>-16.600000000000001</v>
           </cell>
@@ -3735,11 +4020,13 @@
           <cell r="I31">
             <v>150.19999999999999</v>
           </cell>
+          <cell r="J31"/>
         </row>
         <row r="32">
           <cell r="A32" t="str">
             <v>G6PDH2r</v>
           </cell>
+          <cell r="B32"/>
           <cell r="C32" t="str">
             <v>[c] : g6p + nadp --&gt; 6pgl + h + nadph</v>
           </cell>
@@ -3755,14 +4042,17 @@
           <cell r="G32">
             <v>35.299999999999997</v>
           </cell>
+          <cell r="H32"/>
           <cell r="I32">
             <v>174</v>
           </cell>
+          <cell r="J32"/>
         </row>
         <row r="33">
           <cell r="A33" t="str">
             <v>PGL</v>
           </cell>
+          <cell r="B33"/>
           <cell r="C33" t="str">
             <v>[c] : 6pgl + h2o --&gt; 6pgc + h</v>
           </cell>
@@ -3778,14 +4068,17 @@
           <cell r="G33">
             <v>-2.1</v>
           </cell>
+          <cell r="H33"/>
           <cell r="I33">
             <v>25</v>
           </cell>
+          <cell r="J33"/>
         </row>
         <row r="34">
           <cell r="A34" t="str">
             <v>GND</v>
           </cell>
+          <cell r="B34"/>
           <cell r="C34" t="str">
             <v>[c] : 6pgc + nadp --&gt; co2 + nadph + ru5p-D</v>
           </cell>
@@ -3801,17 +4094,22 @@
           <cell r="G34">
             <v>31.7</v>
           </cell>
+          <cell r="H34"/>
           <cell r="I34">
             <v>75.650000000000006</v>
           </cell>
+          <cell r="J34"/>
         </row>
         <row r="35">
           <cell r="A35" t="str">
             <v>RPE</v>
           </cell>
+          <cell r="B35"/>
           <cell r="C35" t="str">
             <v>[c] : ru5p-D &lt;==&gt; xu5p-D</v>
           </cell>
+          <cell r="D35"/>
+          <cell r="E35"/>
           <cell r="F35">
             <v>-22.2</v>
           </cell>
@@ -3824,14 +4122,17 @@
           <cell r="I35">
             <v>21.05</v>
           </cell>
+          <cell r="J35"/>
         </row>
         <row r="36">
           <cell r="A36" t="str">
             <v>RPI</v>
           </cell>
+          <cell r="B36"/>
           <cell r="C36" t="str">
             <v>[c] : r5p &lt;==&gt; ru5p-D</v>
           </cell>
+          <cell r="D36"/>
           <cell r="E36">
             <v>0.5</v>
           </cell>
@@ -3841,17 +4142,22 @@
           <cell r="G36">
             <v>20.8</v>
           </cell>
+          <cell r="H36"/>
           <cell r="I36">
             <v>2100</v>
           </cell>
+          <cell r="J36"/>
         </row>
         <row r="37">
           <cell r="A37" t="str">
             <v>TKT1</v>
           </cell>
+          <cell r="B37"/>
           <cell r="C37" t="str">
             <v>[c] : g3p + s7p &lt;==&gt; r5p + xu5p-D</v>
           </cell>
+          <cell r="D37"/>
+          <cell r="E37"/>
           <cell r="F37">
             <v>-33.9</v>
           </cell>
@@ -3861,6 +4167,7 @@
           <cell r="H37">
             <v>0.216</v>
           </cell>
+          <cell r="I37"/>
           <cell r="J37">
             <v>55.57</v>
           </cell>
@@ -3869,9 +4176,11 @@
           <cell r="A38" t="str">
             <v>TALA</v>
           </cell>
+          <cell r="B38"/>
           <cell r="C38" t="str">
             <v>[c] : g3p + s7p &lt;==&gt; e4p + f6p</v>
           </cell>
+          <cell r="D38"/>
           <cell r="E38">
             <v>-1.7</v>
           </cell>
@@ -3881,17 +4190,21 @@
           <cell r="G38">
             <v>36.9</v>
           </cell>
+          <cell r="H38"/>
           <cell r="I38">
             <v>16.57</v>
           </cell>
+          <cell r="J38"/>
         </row>
         <row r="39">
           <cell r="A39" t="str">
             <v>TKT2</v>
           </cell>
+          <cell r="B39"/>
           <cell r="C39" t="str">
             <v>[c] : f6p + g3p &lt;==&gt; e4p + xu5p-D</v>
           </cell>
+          <cell r="D39"/>
           <cell r="E39">
             <v>1.7</v>
           </cell>
@@ -3904,6 +4217,7 @@
           <cell r="H39">
             <v>1.77E-2</v>
           </cell>
+          <cell r="I39"/>
           <cell r="J39">
             <v>15.45</v>
           </cell>
@@ -3912,6 +4226,7 @@
           <cell r="A40" t="str">
             <v>NADH16</v>
           </cell>
+          <cell r="B40"/>
           <cell r="C40" t="str">
             <v>4 h[e] + nad[c] + q8h2[c] &lt;==&gt; 5 h[c] + nadh[c] + q8[c]</v>
           </cell>
@@ -3935,9 +4250,12 @@
           <cell r="A41" t="str">
             <v>NADTRHD</v>
           </cell>
+          <cell r="B41"/>
           <cell r="C41" t="str">
             <v>[c] : nad + nadph &lt;==&gt; nadh + nadp</v>
           </cell>
+          <cell r="D41"/>
+          <cell r="E41"/>
           <cell r="F41">
             <v>-38.6</v>
           </cell>
@@ -3947,6 +4265,7 @@
           <cell r="H41">
             <v>1.48</v>
           </cell>
+          <cell r="I41"/>
           <cell r="J41">
             <v>6.6699999999999995E-2</v>
           </cell>
@@ -3955,12 +4274,14 @@
           <cell r="A42" t="str">
             <v>THD2</v>
           </cell>
+          <cell r="B42"/>
           <cell r="C42" t="str">
             <v>2 h[c] + nad[c] + nadph[c] &lt;==&gt; 2 h[e] + nadh[c] + nadp[c]</v>
           </cell>
           <cell r="D42" t="str">
             <v>h[c],h[e]</v>
           </cell>
+          <cell r="E42"/>
           <cell r="F42">
             <v>-38.6</v>
           </cell>
@@ -3981,9 +4302,12 @@
           <cell r="A43" t="str">
             <v>ADK1</v>
           </cell>
+          <cell r="B43"/>
           <cell r="C43" t="str">
             <v>[c] : amp + atp &lt;==&gt; 2 adp</v>
           </cell>
+          <cell r="D43"/>
+          <cell r="E43"/>
           <cell r="F43">
             <v>-40.200000000000003</v>
           </cell>
@@ -3996,11 +4320,13 @@
           <cell r="I43">
             <v>5.2999999999999999E-2</v>
           </cell>
+          <cell r="J43"/>
         </row>
         <row r="44">
           <cell r="A44" t="str">
             <v>ATPM</v>
           </cell>
+          <cell r="B44"/>
           <cell r="C44" t="str">
             <v>[c] : atp + h2o --&gt; adp + h + pi</v>
           </cell>
@@ -4010,6 +4336,9 @@
           <cell r="E44">
             <v>-6.6</v>
           </cell>
+          <cell r="F44"/>
+          <cell r="G44"/>
+          <cell r="H44"/>
           <cell r="I44">
             <v>1</v>
           </cell>
@@ -4021,6 +4350,7 @@
           <cell r="A45" t="str">
             <v>ATPS4r</v>
           </cell>
+          <cell r="B45"/>
           <cell r="C45" t="str">
             <v>atp[c] + 3 h[c] &lt;==&gt; adp[c] + 4 h[e] + pi[c]</v>
           </cell>
@@ -4044,6 +4374,7 @@
           <cell r="A46" t="str">
             <v>CYTBD</v>
           </cell>
+          <cell r="B46"/>
           <cell r="C46" t="str">
             <v>6 h[c] + 0.5 o2[c] + q8h2[c] --&gt; 6 h[e] + h2o[c] + q8[c]</v>
           </cell>
@@ -4064,6 +4395,7 @@
           <cell r="A47" t="str">
             <v>PPC</v>
           </cell>
+          <cell r="B47"/>
           <cell r="C47" t="str">
             <v>[c] : h + oaa + pi &lt;==&gt; co2 + h2o + pep</v>
           </cell>
@@ -4079,6 +4411,8 @@
           <cell r="G47">
             <v>55.6</v>
           </cell>
+          <cell r="H47"/>
+          <cell r="I47"/>
           <cell r="J47">
             <v>540</v>
           </cell>
@@ -4087,6 +4421,7 @@
           <cell r="A48" t="str">
             <v>PPCK</v>
           </cell>
+          <cell r="B48"/>
           <cell r="C48" t="str">
             <v>[c] : atp + oaa --&gt; adp + co2 + pep</v>
           </cell>
@@ -4102,14 +4437,17 @@
           <cell r="G48">
             <v>30.9</v>
           </cell>
+          <cell r="H48"/>
           <cell r="I48">
             <v>1</v>
           </cell>
+          <cell r="J48"/>
         </row>
         <row r="49">
           <cell r="A49" t="str">
             <v>ME1</v>
           </cell>
+          <cell r="B49"/>
           <cell r="C49" t="str">
             <v>[c] : mal + nad --&gt; co2 + nadh + pyr</v>
           </cell>
@@ -4125,14 +4463,17 @@
           <cell r="G49">
             <v>33.6</v>
           </cell>
+          <cell r="H49"/>
           <cell r="I49">
             <v>1</v>
           </cell>
+          <cell r="J49"/>
         </row>
         <row r="50">
           <cell r="A50" t="str">
             <v>ME2</v>
           </cell>
+          <cell r="B50"/>
           <cell r="C50" t="str">
             <v>[c] : mal + nadp --&gt; co2 + nadph + pyr</v>
           </cell>
@@ -4148,20 +4489,27 @@
           <cell r="G50">
             <v>34.5</v>
           </cell>
+          <cell r="H50"/>
           <cell r="I50">
             <v>1</v>
           </cell>
+          <cell r="J50"/>
         </row>
         <row r="51">
           <cell r="A51" t="str">
             <v>H2Ot</v>
           </cell>
+          <cell r="B51"/>
           <cell r="C51" t="str">
             <v>h2o[e] &lt;==&gt; h2o[c]</v>
           </cell>
+          <cell r="D51"/>
           <cell r="E51">
             <v>0</v>
           </cell>
+          <cell r="F51"/>
+          <cell r="G51"/>
+          <cell r="H51"/>
           <cell r="I51">
             <v>1</v>
           </cell>
@@ -4173,12 +4521,17 @@
           <cell r="A52" t="str">
             <v>O2t</v>
           </cell>
+          <cell r="B52"/>
           <cell r="C52" t="str">
             <v>o2[e] &lt;==&gt; o2[c]</v>
           </cell>
+          <cell r="D52"/>
           <cell r="E52">
             <v>0</v>
           </cell>
+          <cell r="F52"/>
+          <cell r="G52"/>
+          <cell r="H52"/>
           <cell r="I52">
             <v>1</v>
           </cell>
@@ -4190,6 +4543,7 @@
           <cell r="A53" t="str">
             <v>PIt2r</v>
           </cell>
+          <cell r="B53"/>
           <cell r="C53" t="str">
             <v>h[e] + pi[e] &lt;==&gt; h[c] + pi[c]</v>
           </cell>
@@ -4207,12 +4561,17 @@
           <cell r="A54" t="str">
             <v>CO2t</v>
           </cell>
+          <cell r="B54"/>
           <cell r="C54" t="str">
             <v>co2[e] &lt;==&gt; co2[c]</v>
           </cell>
+          <cell r="D54"/>
           <cell r="E54">
             <v>0</v>
           </cell>
+          <cell r="F54"/>
+          <cell r="G54"/>
+          <cell r="H54"/>
           <cell r="I54">
             <v>0</v>
           </cell>
@@ -4224,6 +4583,7 @@
           <cell r="A55" t="str">
             <v>PYRt2r</v>
           </cell>
+          <cell r="B55"/>
           <cell r="C55" t="str">
             <v>h[e] + pyr[e] &lt;==&gt; h[c] + pyr[c]</v>
           </cell>
@@ -4244,6 +4604,7 @@
           <cell r="A56" t="str">
             <v>SUCCt2_2</v>
           </cell>
+          <cell r="B56"/>
           <cell r="C56" t="str">
             <v>2 h[e] + succ[e] --&gt; 2 h[c] + succ[c]</v>
           </cell>
@@ -4253,6 +4614,9 @@
           <cell r="E56">
             <v>0</v>
           </cell>
+          <cell r="F56"/>
+          <cell r="G56"/>
+          <cell r="H56"/>
           <cell r="I56">
             <v>1</v>
           </cell>
@@ -4264,6 +4628,7 @@
           <cell r="A57" t="str">
             <v>SUCCt3</v>
           </cell>
+          <cell r="B57"/>
           <cell r="C57" t="str">
             <v>h[e] + succ[c] --&gt; h[c] + succ[e]</v>
           </cell>
@@ -4273,6 +4638,9 @@
           <cell r="E57">
             <v>0</v>
           </cell>
+          <cell r="F57"/>
+          <cell r="G57"/>
+          <cell r="H57"/>
           <cell r="I57">
             <v>1</v>
           </cell>
@@ -4284,6 +4652,7 @@
           <cell r="A58" t="str">
             <v>AKGt2r</v>
           </cell>
+          <cell r="B58"/>
           <cell r="C58" t="str">
             <v>akg[e] + h[e] &lt;==&gt; akg[c] + h[c]</v>
           </cell>
@@ -4293,6 +4662,9 @@
           <cell r="E58">
             <v>0</v>
           </cell>
+          <cell r="F58"/>
+          <cell r="G58"/>
+          <cell r="H58"/>
           <cell r="I58">
             <v>1</v>
           </cell>
@@ -4304,6 +4676,7 @@
           <cell r="A59" t="str">
             <v>FUMt2_2</v>
           </cell>
+          <cell r="B59"/>
           <cell r="C59" t="str">
             <v>fum[e] + 2 h[e] --&gt; fum[c] + 2 h[c]</v>
           </cell>
@@ -4313,6 +4686,9 @@
           <cell r="E59">
             <v>0</v>
           </cell>
+          <cell r="F59"/>
+          <cell r="G59"/>
+          <cell r="H59"/>
           <cell r="I59">
             <v>1</v>
           </cell>
@@ -4324,6 +4700,7 @@
           <cell r="A60" t="str">
             <v>MALt2_2</v>
           </cell>
+          <cell r="B60"/>
           <cell r="C60" t="str">
             <v>2 h[e] + mal[e] --&gt; 2 h[c] + mal[c]</v>
           </cell>
@@ -4333,6 +4710,9 @@
           <cell r="E60">
             <v>0</v>
           </cell>
+          <cell r="F60"/>
+          <cell r="G60"/>
+          <cell r="H60"/>
           <cell r="I60">
             <v>1</v>
           </cell>
@@ -4344,6 +4724,7 @@
           <cell r="A61" t="str">
             <v>D_LACt2</v>
           </cell>
+          <cell r="B61"/>
           <cell r="C61" t="str">
             <v>h[e] + lac[e] &lt;==&gt; h[c] + lac[c]</v>
           </cell>
@@ -4353,6 +4734,9 @@
           <cell r="E61">
             <v>0</v>
           </cell>
+          <cell r="F61"/>
+          <cell r="G61"/>
+          <cell r="H61"/>
           <cell r="I61">
             <v>1</v>
           </cell>
@@ -4364,6 +4748,7 @@
           <cell r="A62" t="str">
             <v>FORt2</v>
           </cell>
+          <cell r="B62"/>
           <cell r="C62" t="str">
             <v>for[e] + h[e] --&gt; for[c] + h[c]</v>
           </cell>
@@ -4373,6 +4758,9 @@
           <cell r="E62">
             <v>0</v>
           </cell>
+          <cell r="F62"/>
+          <cell r="G62"/>
+          <cell r="H62"/>
           <cell r="I62">
             <v>1</v>
           </cell>
@@ -4384,12 +4772,17 @@
           <cell r="A63" t="str">
             <v>FORti</v>
           </cell>
+          <cell r="B63"/>
           <cell r="C63" t="str">
             <v>for[c] --&gt; for[e]</v>
           </cell>
+          <cell r="D63"/>
           <cell r="E63">
             <v>0</v>
           </cell>
+          <cell r="F63"/>
+          <cell r="G63"/>
+          <cell r="H63"/>
           <cell r="I63">
             <v>1</v>
           </cell>
@@ -4401,12 +4794,17 @@
           <cell r="A64" t="str">
             <v>ETOHt2r</v>
           </cell>
+          <cell r="B64"/>
           <cell r="C64" t="str">
             <v>etoh[e] + h[e] &lt;==&gt; etoh[c] + h[c]</v>
           </cell>
+          <cell r="D64"/>
           <cell r="E64">
             <v>0</v>
           </cell>
+          <cell r="F64"/>
+          <cell r="G64"/>
+          <cell r="H64"/>
           <cell r="I64">
             <v>1</v>
           </cell>
@@ -4418,6 +4816,7 @@
           <cell r="A65" t="str">
             <v>ACt2r</v>
           </cell>
+          <cell r="B65"/>
           <cell r="C65" t="str">
             <v>ac[e] + h[e] &lt;==&gt; ac[c] + h[c]</v>
           </cell>
@@ -4427,6 +4826,9 @@
           <cell r="E65">
             <v>0</v>
           </cell>
+          <cell r="F65"/>
+          <cell r="G65"/>
+          <cell r="H65"/>
           <cell r="I65">
             <v>1</v>
           </cell>
@@ -4438,12 +4840,17 @@
           <cell r="A66" t="str">
             <v>ACALDt</v>
           </cell>
+          <cell r="B66"/>
           <cell r="C66" t="str">
             <v>acald[e] &lt;==&gt; acald[c]</v>
           </cell>
+          <cell r="D66"/>
           <cell r="E66">
             <v>0</v>
           </cell>
+          <cell r="F66"/>
+          <cell r="G66"/>
+          <cell r="H66"/>
           <cell r="I66">
             <v>1</v>
           </cell>
@@ -4455,200 +4862,319 @@
           <cell r="A67" t="str">
             <v>exPYR</v>
           </cell>
+          <cell r="B67"/>
           <cell r="C67" t="str">
             <v>pyr[e] &lt;==&gt;</v>
           </cell>
+          <cell r="D67"/>
           <cell r="E67">
             <v>0</v>
           </cell>
+          <cell r="F67"/>
+          <cell r="G67"/>
+          <cell r="H67"/>
+          <cell r="I67"/>
+          <cell r="J67"/>
         </row>
         <row r="68">
           <cell r="A68" t="str">
             <v>exSUCC</v>
           </cell>
+          <cell r="B68"/>
           <cell r="C68" t="str">
             <v>succ[e] &lt;==&gt;</v>
           </cell>
+          <cell r="D68"/>
           <cell r="E68">
             <v>0</v>
           </cell>
+          <cell r="F68"/>
+          <cell r="G68"/>
+          <cell r="H68"/>
+          <cell r="I68"/>
+          <cell r="J68"/>
         </row>
         <row r="69">
           <cell r="A69" t="str">
             <v>exAKG</v>
           </cell>
+          <cell r="B69"/>
           <cell r="C69" t="str">
             <v>akg[e] &lt;==&gt;</v>
           </cell>
+          <cell r="D69"/>
           <cell r="E69">
             <v>0</v>
           </cell>
+          <cell r="F69"/>
+          <cell r="G69"/>
+          <cell r="H69"/>
+          <cell r="I69"/>
+          <cell r="J69"/>
         </row>
         <row r="70">
           <cell r="A70" t="str">
             <v>exFUM</v>
           </cell>
+          <cell r="B70"/>
           <cell r="C70" t="str">
             <v>fum[e] &lt;==&gt;</v>
           </cell>
+          <cell r="D70"/>
           <cell r="E70">
             <v>0</v>
           </cell>
+          <cell r="F70"/>
+          <cell r="G70"/>
+          <cell r="H70"/>
+          <cell r="I70"/>
+          <cell r="J70"/>
         </row>
         <row r="71">
           <cell r="A71" t="str">
             <v>exMAL</v>
           </cell>
+          <cell r="B71"/>
           <cell r="C71" t="str">
             <v>mal[e] &lt;==&gt;</v>
           </cell>
+          <cell r="D71"/>
           <cell r="E71">
             <v>0</v>
           </cell>
+          <cell r="F71"/>
+          <cell r="G71"/>
+          <cell r="H71"/>
+          <cell r="I71"/>
+          <cell r="J71"/>
         </row>
         <row r="72">
           <cell r="A72" t="str">
             <v>exLAC</v>
           </cell>
+          <cell r="B72"/>
           <cell r="C72" t="str">
             <v>lac[e] &lt;==&gt;</v>
           </cell>
+          <cell r="D72"/>
           <cell r="E72">
             <v>0</v>
           </cell>
+          <cell r="F72"/>
+          <cell r="G72"/>
+          <cell r="H72"/>
+          <cell r="I72"/>
+          <cell r="J72"/>
         </row>
         <row r="73">
           <cell r="A73" t="str">
             <v>exFOR</v>
           </cell>
+          <cell r="B73"/>
           <cell r="C73" t="str">
             <v>for[e] &lt;==&gt;</v>
           </cell>
+          <cell r="D73"/>
           <cell r="E73">
             <v>0</v>
           </cell>
+          <cell r="F73"/>
+          <cell r="G73"/>
+          <cell r="H73"/>
+          <cell r="I73"/>
+          <cell r="J73"/>
         </row>
         <row r="74">
           <cell r="A74" t="str">
             <v>exETOH</v>
           </cell>
+          <cell r="B74"/>
           <cell r="C74" t="str">
             <v>etoh[e] &lt;==&gt;</v>
           </cell>
+          <cell r="D74"/>
           <cell r="E74">
             <v>0</v>
           </cell>
+          <cell r="F74"/>
+          <cell r="G74"/>
+          <cell r="H74"/>
+          <cell r="I74"/>
+          <cell r="J74"/>
         </row>
         <row r="75">
           <cell r="A75" t="str">
             <v>exAC</v>
           </cell>
+          <cell r="B75"/>
           <cell r="C75" t="str">
             <v>ac[e] &lt;==&gt;</v>
           </cell>
+          <cell r="D75"/>
           <cell r="E75">
             <v>0</v>
           </cell>
+          <cell r="F75"/>
+          <cell r="G75"/>
+          <cell r="H75"/>
+          <cell r="I75"/>
+          <cell r="J75"/>
         </row>
         <row r="76">
           <cell r="A76" t="str">
             <v>exACALD</v>
           </cell>
+          <cell r="B76"/>
           <cell r="C76" t="str">
             <v>acald[e] &lt;==&gt;</v>
           </cell>
+          <cell r="D76"/>
           <cell r="E76">
             <v>0</v>
           </cell>
+          <cell r="F76"/>
+          <cell r="G76"/>
+          <cell r="H76"/>
+          <cell r="I76"/>
+          <cell r="J76"/>
         </row>
         <row r="77">
           <cell r="A77" t="str">
             <v>exGLC</v>
           </cell>
+          <cell r="B77"/>
           <cell r="C77" t="str">
             <v>glc[e] &lt;==&gt;</v>
           </cell>
+          <cell r="D77"/>
           <cell r="E77">
             <v>0</v>
           </cell>
+          <cell r="F77"/>
+          <cell r="G77"/>
+          <cell r="H77"/>
+          <cell r="I77"/>
+          <cell r="J77"/>
         </row>
         <row r="78">
           <cell r="A78" t="str">
             <v>exCO2</v>
           </cell>
+          <cell r="B78"/>
           <cell r="C78" t="str">
             <v>co2[e]&lt;==&gt;</v>
           </cell>
+          <cell r="D78"/>
           <cell r="E78">
             <v>0</v>
           </cell>
+          <cell r="F78"/>
+          <cell r="G78"/>
+          <cell r="H78"/>
+          <cell r="I78"/>
+          <cell r="J78"/>
         </row>
         <row r="79">
           <cell r="A79" t="str">
             <v>exH</v>
           </cell>
+          <cell r="B79"/>
           <cell r="C79" t="str">
             <v>h[e] &lt;==&gt;</v>
           </cell>
+          <cell r="D79"/>
           <cell r="E79">
             <v>0</v>
           </cell>
+          <cell r="F79"/>
+          <cell r="G79"/>
+          <cell r="H79"/>
+          <cell r="I79"/>
+          <cell r="J79"/>
         </row>
         <row r="80">
           <cell r="A80" t="str">
             <v>exH2O</v>
           </cell>
+          <cell r="B80"/>
           <cell r="C80" t="str">
             <v>h2o[e] &lt;==&gt;</v>
           </cell>
+          <cell r="D80"/>
           <cell r="E80">
             <v>0</v>
           </cell>
+          <cell r="F80"/>
+          <cell r="G80"/>
+          <cell r="H80"/>
+          <cell r="I80"/>
+          <cell r="J80"/>
         </row>
         <row r="81">
           <cell r="A81" t="str">
             <v>exPI</v>
           </cell>
+          <cell r="B81"/>
           <cell r="C81" t="str">
             <v>pi[e] &lt;==&gt;</v>
           </cell>
+          <cell r="D81"/>
           <cell r="E81">
             <v>0</v>
           </cell>
+          <cell r="F81"/>
+          <cell r="G81"/>
+          <cell r="H81"/>
+          <cell r="I81"/>
+          <cell r="J81"/>
         </row>
         <row r="82">
           <cell r="A82" t="str">
             <v>exO2</v>
           </cell>
+          <cell r="B82"/>
           <cell r="C82" t="str">
             <v>o2[e] &lt;==&gt;</v>
           </cell>
+          <cell r="D82"/>
           <cell r="E82">
             <v>0</v>
           </cell>
+          <cell r="F82"/>
+          <cell r="G82"/>
+          <cell r="H82"/>
+          <cell r="I82"/>
+          <cell r="J82"/>
         </row>
         <row r="83">
           <cell r="A83" t="str">
             <v>EC_biomass</v>
           </cell>
+          <cell r="B83"/>
           <cell r="C83" t="str">
             <v>[c] : 1.496 3pg + 3.7478 accoa + 59.8100 atp + 0.3610 e4p + 0.0709 f6p + 0.1290 g3p + 0.2050 g6p + 59.8100 h2o + 3.5470 nad + 13.0279 nadph + 1.7867 oaa + 0.5191 pep + 2.8328 pyr + 0.8977 r5p --&gt; 59.8100 adp + 4.1182 akg + 3.7478 coa + 59.8100 h + 3.5470 nadh + 13.0279 nadp + 59.8100 pi</v>
           </cell>
+          <cell r="D83"/>
           <cell r="E83">
             <v>0</v>
           </cell>
+          <cell r="F83"/>
+          <cell r="G83"/>
+          <cell r="H83"/>
+          <cell r="I83"/>
+          <cell r="J83"/>
         </row>
       </sheetData>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -6235,6 +6761,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -6270,6 +6813,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -6910,7 +7470,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection sqref="A1:U43"/>
     </sheetView>
   </sheetViews>
@@ -8680,6 +9240,2243 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection sqref="A1:U51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="41.140625" customWidth="1"/>
+    <col min="15" max="15" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="26"/>
+      <c r="C2" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="23">
+        <f>VLOOKUP(A2,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="17">
+        <v>1</v>
+      </c>
+      <c r="J2" s="23">
+        <v>1</v>
+      </c>
+      <c r="K2" s="23"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="18">
+        <v>-19.215657194822899</v>
+      </c>
+      <c r="N2" s="16"/>
+      <c r="O2" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23"/>
+      <c r="T2" s="23"/>
+      <c r="U2" s="23"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23">
+        <v>0</v>
+      </c>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23">
+        <v>1</v>
+      </c>
+      <c r="J3" s="23">
+        <v>1</v>
+      </c>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="23"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="23"/>
+      <c r="T3" s="23"/>
+      <c r="U3" s="23"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="23"/>
+      <c r="C4" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23">
+        <f>VLOOKUP(A4,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>4.3</v>
+      </c>
+      <c r="F4" s="23">
+        <v>-24.3</v>
+      </c>
+      <c r="G4" s="23">
+        <v>52.1</v>
+      </c>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23">
+        <v>280</v>
+      </c>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="16" t="str">
+        <f>VLOOKUP(A4,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>2.7.2.1</v>
+      </c>
+      <c r="O4" s="23"/>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="23"/>
+      <c r="R4" s="23"/>
+      <c r="S4" s="23"/>
+      <c r="T4" s="23"/>
+      <c r="U4" s="23"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="23"/>
+      <c r="C5" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="23">
+        <f>VLOOKUP(A5,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>3.8</v>
+      </c>
+      <c r="F5" s="23">
+        <v>-20.399999999999999</v>
+      </c>
+      <c r="G5" s="23">
+        <v>28.7</v>
+      </c>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23">
+        <v>120</v>
+      </c>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="16" t="str">
+        <f>VLOOKUP(A5,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>2.3.1.8</v>
+      </c>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="23"/>
+      <c r="R5" s="23"/>
+      <c r="S5" s="23"/>
+      <c r="T5" s="23"/>
+      <c r="U5" s="23"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="B6" s="23"/>
+      <c r="C6" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23">
+        <v>8.6</v>
+      </c>
+      <c r="F6" s="23">
+        <v>-4</v>
+      </c>
+      <c r="G6" s="23">
+        <v>60.9</v>
+      </c>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23">
+        <v>81</v>
+      </c>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="18">
+        <v>6.0051760006096302</v>
+      </c>
+      <c r="N6" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="O6" s="23"/>
+      <c r="P6" s="23"/>
+      <c r="Q6" s="23"/>
+      <c r="R6" s="23"/>
+      <c r="S6" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="T6" s="23">
+        <v>0.39800000000000002</v>
+      </c>
+      <c r="U6" s="23">
+        <v>0.39800000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="B7" s="23"/>
+      <c r="C7" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23">
+        <f>VLOOKUP(A7,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>1.5</v>
+      </c>
+      <c r="F7" s="23">
+        <v>-11.2</v>
+      </c>
+      <c r="G7" s="23">
+        <v>26.5</v>
+      </c>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23">
+        <v>5.3</v>
+      </c>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="18">
+        <v>-6.0051760006096302</v>
+      </c>
+      <c r="N7" s="16" t="str">
+        <f>VLOOKUP(A7,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>4.2.1.3</v>
+      </c>
+      <c r="O7" s="23"/>
+      <c r="P7" s="23"/>
+      <c r="Q7" s="23"/>
+      <c r="R7" s="23"/>
+      <c r="S7" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="T7" s="23">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="U7" s="23">
+        <v>9.8000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="B8" s="23"/>
+      <c r="C8" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23">
+        <f>VLOOKUP(A8,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="F8" s="23">
+        <v>-38.700000000000003</v>
+      </c>
+      <c r="G8" s="23">
+        <v>17.8</v>
+      </c>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23">
+        <v>5.2</v>
+      </c>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="18">
+        <v>0</v>
+      </c>
+      <c r="N8" s="16" t="str">
+        <f>VLOOKUP(A8,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>4.1.3.1</v>
+      </c>
+      <c r="O8" s="23"/>
+      <c r="P8" s="23"/>
+      <c r="Q8" s="23"/>
+      <c r="R8" s="23"/>
+      <c r="S8" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="T8" s="23">
+        <v>0.59499999999999997</v>
+      </c>
+      <c r="U8" s="23">
+        <v>0.59499999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="B9" s="23"/>
+      <c r="C9" s="16" t="s">
+        <v>220</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>197</v>
+      </c>
+      <c r="E9" s="23">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="F9" s="23">
+        <v>-9.1</v>
+      </c>
+      <c r="G9" s="23">
+        <v>63.1</v>
+      </c>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23">
+        <v>48.1</v>
+      </c>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="18">
+        <v>0</v>
+      </c>
+      <c r="N9" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="O9" s="23"/>
+      <c r="P9" s="23"/>
+      <c r="Q9" s="23"/>
+      <c r="R9" s="23"/>
+      <c r="S9" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="T9" s="23">
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="U9" s="23">
+        <v>4.2699999999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="23" t="s">
+        <v>214</v>
+      </c>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23" t="s">
+        <v>215</v>
+      </c>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23">
+        <f>VLOOKUP(A10,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>1.3</v>
+      </c>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23">
+        <f>VLOOKUP($A10,[1]ecoliN1!$A$2:$J$84,9,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="J10" s="23">
+        <f>VLOOKUP($A10,[1]ecoliN1!$A$2:$J$84,10,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="23"/>
+      <c r="O10" s="23"/>
+      <c r="P10" s="23"/>
+      <c r="Q10" s="23"/>
+      <c r="R10" s="23"/>
+      <c r="S10" s="23"/>
+      <c r="T10" s="23"/>
+      <c r="U10" s="23"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16" t="s">
+        <v>221</v>
+      </c>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23">
+        <f>VLOOKUP(A11,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>-1.2</v>
+      </c>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23">
+        <f>VLOOKUP($A11,[1]ecoliN1!$A$2:$J$84,9,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="J11" s="23">
+        <f>VLOOKUP($A11,[1]ecoliN1!$A$2:$J$84,10,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="23"/>
+      <c r="O11" s="23"/>
+      <c r="P11" s="23"/>
+      <c r="Q11" s="23"/>
+      <c r="R11" s="23"/>
+      <c r="S11" s="23"/>
+      <c r="T11" s="23"/>
+      <c r="U11" s="23"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
+        <v>216</v>
+      </c>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23">
+        <f>VLOOKUP(A12,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>0.2</v>
+      </c>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23">
+        <f>VLOOKUP($A12,[1]ecoliN1!$A$2:$J$84,9,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="J12" s="23">
+        <f>VLOOKUP($A12,[1]ecoliN1!$A$2:$J$84,10,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="23"/>
+      <c r="O12" s="23"/>
+      <c r="P12" s="23"/>
+      <c r="Q12" s="23"/>
+      <c r="R12" s="23"/>
+      <c r="S12" s="23"/>
+      <c r="T12" s="23"/>
+      <c r="U12" s="23"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="B13" s="23"/>
+      <c r="C13" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="23">
+        <f>VLOOKUP(A13,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>3.4</v>
+      </c>
+      <c r="F13" s="23">
+        <v>-48.4</v>
+      </c>
+      <c r="G13" s="23">
+        <v>26.9</v>
+      </c>
+      <c r="H13" s="23"/>
+      <c r="I13" s="23">
+        <v>106.4</v>
+      </c>
+      <c r="J13" s="23"/>
+      <c r="K13" s="23"/>
+      <c r="L13" s="23"/>
+      <c r="M13" s="18">
+        <v>-6.0051760006096302</v>
+      </c>
+      <c r="N13" s="16" t="str">
+        <f>VLOOKUP(A13,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>1.1.1.42</v>
+      </c>
+      <c r="O13" s="23"/>
+      <c r="P13" s="23"/>
+      <c r="Q13" s="23"/>
+      <c r="R13" s="23"/>
+      <c r="S13" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="T13" s="23">
+        <v>0.95499999999999996</v>
+      </c>
+      <c r="U13" s="23">
+        <v>0.95499999999999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="B14" s="23"/>
+      <c r="C14" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="23">
+        <f>VLOOKUP(A14,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>-8.3000000000000007</v>
+      </c>
+      <c r="F14" s="23">
+        <v>-72.3</v>
+      </c>
+      <c r="G14" s="23">
+        <v>20.3</v>
+      </c>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23">
+        <v>49</v>
+      </c>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="18">
+        <v>3.5679805516174299</v>
+      </c>
+      <c r="N14" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="O14" s="23"/>
+      <c r="P14" s="23"/>
+      <c r="Q14" s="23"/>
+      <c r="R14" s="23"/>
+      <c r="S14" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="T14" s="23">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="U14" s="23">
+        <v>0.19500000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="B15" s="23"/>
+      <c r="C15" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="23">
+        <v>-1</v>
+      </c>
+      <c r="F15" s="23">
+        <v>-39.5</v>
+      </c>
+      <c r="G15" s="23">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="H15" s="23">
+        <v>2.12</v>
+      </c>
+      <c r="I15" s="23">
+        <v>25.6</v>
+      </c>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="18">
+        <v>-3.5679805516174299</v>
+      </c>
+      <c r="N15" s="16" t="str">
+        <f>VLOOKUP(A15,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>6.2.1.5</v>
+      </c>
+      <c r="O15" s="23"/>
+      <c r="P15" s="23"/>
+      <c r="Q15" s="23"/>
+      <c r="R15" s="23"/>
+      <c r="S15" s="23" t="s">
+        <v>157</v>
+      </c>
+      <c r="T15" s="23">
+        <v>6.2E-2</v>
+      </c>
+      <c r="U15" s="23">
+        <v>6.2E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="B16" s="23"/>
+      <c r="C16" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23">
+        <v>-2.1</v>
+      </c>
+      <c r="F16" s="23">
+        <v>-40.4</v>
+      </c>
+      <c r="G16" s="23">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23">
+        <v>167</v>
+      </c>
+      <c r="J16" s="23"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="18">
+        <v>3.5679805516174299</v>
+      </c>
+      <c r="N16" s="16" t="str">
+        <f>VLOOKUP(A16,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>1.3.99.1</v>
+      </c>
+      <c r="O16" s="23"/>
+      <c r="P16" s="23"/>
+      <c r="Q16" s="23"/>
+      <c r="R16" s="23"/>
+      <c r="S16" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="T16" s="23">
+        <v>1.47</v>
+      </c>
+      <c r="U16" s="23">
+        <v>1.47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="B17" s="23"/>
+      <c r="C17" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23">
+        <v>0.6</v>
+      </c>
+      <c r="F17" s="23">
+        <v>-15.4</v>
+      </c>
+      <c r="G17" s="23">
+        <v>22.3</v>
+      </c>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23">
+        <v>51.7</v>
+      </c>
+      <c r="J17" s="23"/>
+      <c r="K17" s="23"/>
+      <c r="L17" s="23"/>
+      <c r="M17" s="18">
+        <v>-3.5679805516174299</v>
+      </c>
+      <c r="N17" s="16" t="str">
+        <f>VLOOKUP(A17,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>4.2.1.2</v>
+      </c>
+      <c r="O17" s="23"/>
+      <c r="P17" s="23"/>
+      <c r="Q17" s="23"/>
+      <c r="R17" s="23"/>
+      <c r="S17" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="T17" s="23">
+        <v>0.80800000000000005</v>
+      </c>
+      <c r="U17" s="23">
+        <v>0.80800000000000005</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="B18" s="23"/>
+      <c r="C18" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="E18" s="23">
+        <v>6.4</v>
+      </c>
+      <c r="F18" s="23">
+        <v>-7.3</v>
+      </c>
+      <c r="G18" s="23">
+        <v>68.599999999999994</v>
+      </c>
+      <c r="H18" s="23"/>
+      <c r="I18" s="23">
+        <v>931</v>
+      </c>
+      <c r="J18" s="23"/>
+      <c r="K18" s="23"/>
+      <c r="L18" s="23">
+        <v>50</v>
+      </c>
+      <c r="M18" s="18">
+        <v>3.5679805516174299</v>
+      </c>
+      <c r="N18" s="16" t="str">
+        <f>VLOOKUP(A18,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>1.1.1.37</v>
+      </c>
+      <c r="O18" s="23"/>
+      <c r="P18" s="23"/>
+      <c r="Q18" s="23"/>
+      <c r="R18" s="23"/>
+      <c r="S18" s="23"/>
+      <c r="T18" s="23"/>
+      <c r="U18" s="23"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="B19" s="26"/>
+      <c r="C19" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19" s="23">
+        <v>0</v>
+      </c>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="17">
+        <v>1</v>
+      </c>
+      <c r="J19" s="23">
+        <v>0</v>
+      </c>
+      <c r="K19" s="23"/>
+      <c r="L19" s="23"/>
+      <c r="M19" s="18">
+        <v>0</v>
+      </c>
+      <c r="N19" s="16"/>
+      <c r="O19" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="P19" s="23"/>
+      <c r="Q19" s="23"/>
+      <c r="R19" s="23"/>
+      <c r="S19" s="23"/>
+      <c r="T19" s="23"/>
+      <c r="U19" s="23"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20" s="25" t="s">
+        <v>178</v>
+      </c>
+      <c r="B20" s="26"/>
+      <c r="C20" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20" s="23">
+        <f>VLOOKUP(A20,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="17">
+        <v>1</v>
+      </c>
+      <c r="J20" s="23">
+        <v>1</v>
+      </c>
+      <c r="K20" s="23"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="18">
+        <v>0</v>
+      </c>
+      <c r="N20" s="16"/>
+      <c r="O20" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="P20" s="23"/>
+      <c r="Q20" s="23"/>
+      <c r="R20" s="23"/>
+      <c r="S20" s="23"/>
+      <c r="T20" s="23"/>
+      <c r="U20" s="23"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A21" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="B21" s="26"/>
+      <c r="C21" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="D21" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="E21" s="23">
+        <f>VLOOKUP(A21,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="17">
+        <v>1</v>
+      </c>
+      <c r="J21" s="23">
+        <v>0</v>
+      </c>
+      <c r="K21" s="23"/>
+      <c r="L21" s="23"/>
+      <c r="M21" s="18">
+        <v>0</v>
+      </c>
+      <c r="N21" s="16"/>
+      <c r="O21" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="P21" s="23"/>
+      <c r="Q21" s="23"/>
+      <c r="R21" s="23"/>
+      <c r="S21" s="23"/>
+      <c r="T21" s="23"/>
+      <c r="U21" s="23"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A22" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="B22" s="26"/>
+      <c r="C22" s="28" t="s">
+        <v>224</v>
+      </c>
+      <c r="D22" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="E22" s="23">
+        <f>VLOOKUP(A22,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="23"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="17">
+        <v>1</v>
+      </c>
+      <c r="J22" s="23">
+        <v>0</v>
+      </c>
+      <c r="K22" s="23"/>
+      <c r="L22" s="23"/>
+      <c r="M22" s="18">
+        <v>0</v>
+      </c>
+      <c r="N22" s="16"/>
+      <c r="O22" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="P22" s="23"/>
+      <c r="Q22" s="23"/>
+      <c r="R22" s="23"/>
+      <c r="S22" s="23"/>
+      <c r="T22" s="23"/>
+      <c r="U22" s="23"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="B23" s="27"/>
+      <c r="C23" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23">
+        <v>0</v>
+      </c>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="23"/>
+      <c r="K23" s="23"/>
+      <c r="L23" s="23"/>
+      <c r="M23" s="18">
+        <v>0</v>
+      </c>
+      <c r="N23" s="16"/>
+      <c r="O23" s="23"/>
+      <c r="P23" s="23"/>
+      <c r="Q23" s="23"/>
+      <c r="R23" s="23"/>
+      <c r="S23" s="23"/>
+      <c r="T23" s="23"/>
+      <c r="U23" s="23"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="B24" s="27"/>
+      <c r="C24" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23">
+        <v>0</v>
+      </c>
+      <c r="F24" s="23"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="23"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="23"/>
+      <c r="K24" s="23"/>
+      <c r="L24" s="23"/>
+      <c r="M24" s="18">
+        <v>0</v>
+      </c>
+      <c r="N24" s="16"/>
+      <c r="O24" s="23"/>
+      <c r="P24" s="23"/>
+      <c r="Q24" s="23"/>
+      <c r="R24" s="23"/>
+      <c r="S24" s="23"/>
+      <c r="T24" s="23"/>
+      <c r="U24" s="23"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="B25" s="27"/>
+      <c r="C25" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23">
+        <v>0</v>
+      </c>
+      <c r="F25" s="23"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="23"/>
+      <c r="I25" s="23"/>
+      <c r="J25" s="23"/>
+      <c r="K25" s="23"/>
+      <c r="L25" s="23"/>
+      <c r="M25" s="18">
+        <v>0</v>
+      </c>
+      <c r="N25" s="16"/>
+      <c r="O25" s="23"/>
+      <c r="P25" s="23"/>
+      <c r="Q25" s="23"/>
+      <c r="R25" s="23"/>
+      <c r="S25" s="23"/>
+      <c r="T25" s="23"/>
+      <c r="U25" s="23"/>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="B26" s="27"/>
+      <c r="C26" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="D26" s="23"/>
+      <c r="E26" s="23">
+        <v>0</v>
+      </c>
+      <c r="F26" s="23"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="23"/>
+      <c r="I26" s="23"/>
+      <c r="J26" s="23"/>
+      <c r="K26" s="23"/>
+      <c r="L26" s="23"/>
+      <c r="M26" s="18">
+        <v>0</v>
+      </c>
+      <c r="N26" s="16"/>
+      <c r="O26" s="23"/>
+      <c r="P26" s="23"/>
+      <c r="Q26" s="23"/>
+      <c r="R26" s="23"/>
+      <c r="S26" s="23"/>
+      <c r="T26" s="23"/>
+      <c r="U26" s="23"/>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A27" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="23"/>
+      <c r="C27" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23">
+        <f>VLOOKUP(A27,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>-0.9</v>
+      </c>
+      <c r="F27" s="23">
+        <v>-22.9</v>
+      </c>
+      <c r="G27" s="23">
+        <v>14.7</v>
+      </c>
+      <c r="H27" s="23"/>
+      <c r="I27" s="23">
+        <v>355.79</v>
+      </c>
+      <c r="J27" s="23"/>
+      <c r="K27" s="23"/>
+      <c r="L27" s="23"/>
+      <c r="M27" s="18"/>
+      <c r="N27" s="16" t="str">
+        <f>VLOOKUP(A27,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>4.2.1.11</v>
+      </c>
+      <c r="O27" s="23"/>
+      <c r="P27" s="23"/>
+      <c r="Q27" s="23"/>
+      <c r="R27" s="23"/>
+      <c r="S27" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="T27" s="23">
+        <v>2.67</v>
+      </c>
+      <c r="U27" s="23">
+        <v>2.67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A28" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="23"/>
+      <c r="C28" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23">
+        <v>6.2290000000000001</v>
+      </c>
+      <c r="F28" s="23">
+        <v>-23.1</v>
+      </c>
+      <c r="G28" s="23">
+        <v>14.6</v>
+      </c>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23">
+        <v>530</v>
+      </c>
+      <c r="K28" s="23"/>
+      <c r="L28" s="23"/>
+      <c r="M28" s="18"/>
+      <c r="N28" s="16" t="str">
+        <f>VLOOKUP(A28,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>5.4.2.1</v>
+      </c>
+      <c r="O28" s="23"/>
+      <c r="P28" s="23"/>
+      <c r="Q28" s="23"/>
+      <c r="R28" s="23"/>
+      <c r="S28" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="T28" s="23">
+        <v>2.67</v>
+      </c>
+      <c r="U28" s="23">
+        <v>2.67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A29" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" s="23"/>
+      <c r="C29" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23">
+        <v>-10.51</v>
+      </c>
+      <c r="F29" s="23">
+        <v>-19.2</v>
+      </c>
+      <c r="G29" s="23">
+        <v>56.1</v>
+      </c>
+      <c r="H29" s="24"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="23">
+        <v>654</v>
+      </c>
+      <c r="K29" s="23"/>
+      <c r="L29" s="23"/>
+      <c r="M29" s="18"/>
+      <c r="N29" s="16" t="str">
+        <f>VLOOKUP(A29,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>2.7.2.3</v>
+      </c>
+      <c r="O29" s="23"/>
+      <c r="P29" s="23"/>
+      <c r="Q29" s="23"/>
+      <c r="R29" s="23"/>
+      <c r="S29" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="T29" s="23">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="U29" s="23">
+        <v>0.39900000000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A30" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" s="23"/>
+      <c r="C30" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="D30" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E30" s="23">
+        <f>VLOOKUP(A30,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>-0.1</v>
+      </c>
+      <c r="F30" s="23">
+        <v>-12.8</v>
+      </c>
+      <c r="G30" s="23">
+        <v>62.6</v>
+      </c>
+      <c r="H30" s="23"/>
+      <c r="I30" s="23">
+        <v>268</v>
+      </c>
+      <c r="J30" s="23"/>
+      <c r="K30" s="23"/>
+      <c r="L30" s="23"/>
+      <c r="M30" s="18"/>
+      <c r="N30" s="16" t="str">
+        <f>VLOOKUP(A30,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>1.2.1.12</v>
+      </c>
+      <c r="O30" s="23"/>
+      <c r="P30" s="23"/>
+      <c r="Q30" s="23"/>
+      <c r="R30" s="23"/>
+      <c r="S30" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="T30" s="23">
+        <v>2.13</v>
+      </c>
+      <c r="U30" s="23">
+        <v>2.13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A31" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="23"/>
+      <c r="C31" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D31" s="23"/>
+      <c r="E31" s="17">
+        <v>7.5979999999999999</v>
+      </c>
+      <c r="F31" s="23">
+        <v>-24.3</v>
+      </c>
+      <c r="G31" s="23">
+        <v>13.4</v>
+      </c>
+      <c r="H31" s="23"/>
+      <c r="I31" s="23"/>
+      <c r="J31" s="23">
+        <v>9000</v>
+      </c>
+      <c r="K31" s="23"/>
+      <c r="L31" s="23"/>
+      <c r="M31" s="7"/>
+      <c r="N31" s="16" t="str">
+        <f>VLOOKUP(A31,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>5.3.1.1</v>
+      </c>
+      <c r="O31" s="23"/>
+      <c r="P31" s="23"/>
+      <c r="Q31" s="23"/>
+      <c r="R31" s="23"/>
+      <c r="S31" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="T31" s="23">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="U31" s="23">
+        <v>0.16700000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A32" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" s="23"/>
+      <c r="C32" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D32" s="23"/>
+      <c r="E32" s="23">
+        <f>VLOOKUP(A32,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>4.2</v>
+      </c>
+      <c r="F32" s="23">
+        <v>-29.4</v>
+      </c>
+      <c r="G32" s="23">
+        <v>27.1</v>
+      </c>
+      <c r="H32" s="24"/>
+      <c r="I32" s="23">
+        <v>8.5</v>
+      </c>
+      <c r="J32" s="23"/>
+      <c r="K32" s="23"/>
+      <c r="L32" s="23"/>
+      <c r="M32" s="18"/>
+      <c r="N32" s="16" t="str">
+        <f>VLOOKUP(A32,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>4.1.2.13</v>
+      </c>
+      <c r="O32" s="23"/>
+      <c r="P32" s="23"/>
+      <c r="Q32" s="23"/>
+      <c r="R32" s="23"/>
+      <c r="S32" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="T32" s="23">
+        <v>0.218</v>
+      </c>
+      <c r="U32" s="23">
+        <v>0.218</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A33" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33" s="23"/>
+      <c r="C33" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="D33" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="E33" s="23">
+        <f>VLOOKUP(A33,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>-2.8</v>
+      </c>
+      <c r="F33" s="23">
+        <v>-48.8</v>
+      </c>
+      <c r="G33" s="23">
+        <v>-9.6999999999999993</v>
+      </c>
+      <c r="H33" s="23"/>
+      <c r="I33" s="23">
+        <v>22</v>
+      </c>
+      <c r="J33" s="23"/>
+      <c r="K33" s="23"/>
+      <c r="L33" s="23"/>
+      <c r="M33" s="18">
+        <v>0</v>
+      </c>
+      <c r="N33" s="16" t="str">
+        <f>VLOOKUP(A33,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>3.1.3.11</v>
+      </c>
+      <c r="O33" s="23"/>
+      <c r="P33" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q33" s="23"/>
+      <c r="R33" s="23">
+        <v>0.1</v>
+      </c>
+      <c r="S33" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="T33" s="23">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="U33" s="23">
+        <v>0.27200000000000002</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A34" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" s="23"/>
+      <c r="C34" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" s="23"/>
+      <c r="E34" s="23">
+        <v>3.1320000000000001</v>
+      </c>
+      <c r="F34" s="23">
+        <v>-17.100000000000001</v>
+      </c>
+      <c r="G34" s="23">
+        <v>20.6</v>
+      </c>
+      <c r="H34" s="23"/>
+      <c r="I34" s="23">
+        <v>120</v>
+      </c>
+      <c r="J34" s="23"/>
+      <c r="K34" s="23"/>
+      <c r="L34" s="23"/>
+      <c r="M34" s="18">
+        <v>11.639423575531699</v>
+      </c>
+      <c r="N34" s="16" t="str">
+        <f>VLOOKUP(A34,[2]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>5.3.1.9</v>
+      </c>
+      <c r="O34" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="P34" s="23"/>
+      <c r="Q34" s="23"/>
+      <c r="R34" s="23"/>
+      <c r="S34" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="T34" s="23">
+        <v>3.48</v>
+      </c>
+      <c r="U34" s="23">
+        <v>3.48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" ht="75" x14ac:dyDescent="0.25">
+      <c r="A35" s="44" t="s">
+        <v>255</v>
+      </c>
+      <c r="B35" s="44"/>
+      <c r="C35" s="45" t="s">
+        <v>254</v>
+      </c>
+      <c r="D35" s="23"/>
+      <c r="E35" s="23">
+        <v>0</v>
+      </c>
+      <c r="F35" s="23"/>
+      <c r="G35" s="23"/>
+      <c r="H35" s="23"/>
+      <c r="I35" s="23">
+        <v>1</v>
+      </c>
+      <c r="J35" s="23">
+        <v>0</v>
+      </c>
+      <c r="K35" s="23"/>
+      <c r="L35" s="24"/>
+      <c r="M35" s="23"/>
+      <c r="N35" s="23"/>
+      <c r="O35" s="23"/>
+      <c r="P35" s="23"/>
+      <c r="Q35" s="23"/>
+      <c r="R35" s="23"/>
+      <c r="S35" s="23"/>
+      <c r="T35" s="23"/>
+      <c r="U35" s="23"/>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A36" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="B36" s="26"/>
+      <c r="C36" s="25" t="s">
+        <v>225</v>
+      </c>
+      <c r="D36" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="E36" s="23">
+        <v>0</v>
+      </c>
+      <c r="F36" s="23"/>
+      <c r="G36" s="23"/>
+      <c r="H36" s="23"/>
+      <c r="I36" s="17">
+        <v>2540</v>
+      </c>
+      <c r="J36" s="23">
+        <v>2540</v>
+      </c>
+      <c r="K36" s="23"/>
+      <c r="L36" s="24">
+        <v>1E-3</v>
+      </c>
+      <c r="M36" s="18">
+        <v>-8.5077261088811902</v>
+      </c>
+      <c r="N36" s="16"/>
+      <c r="O36" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="P36" s="23"/>
+      <c r="Q36" s="23"/>
+      <c r="R36" s="23"/>
+      <c r="S36" s="23"/>
+      <c r="T36" s="23"/>
+      <c r="U36" s="23"/>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A37" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="B37" s="27"/>
+      <c r="C37" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="D37" s="23"/>
+      <c r="E37" s="23">
+        <v>0</v>
+      </c>
+      <c r="F37" s="23"/>
+      <c r="G37" s="23"/>
+      <c r="H37" s="23"/>
+      <c r="I37" s="23">
+        <v>1</v>
+      </c>
+      <c r="J37" s="23">
+        <v>1</v>
+      </c>
+      <c r="K37" s="23"/>
+      <c r="L37" s="23"/>
+      <c r="M37" s="23"/>
+      <c r="N37" s="23"/>
+      <c r="O37" s="23"/>
+      <c r="P37" s="23"/>
+      <c r="Q37" s="23"/>
+      <c r="R37" s="23"/>
+      <c r="S37" s="23"/>
+      <c r="T37" s="23"/>
+      <c r="U37" s="23"/>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A38" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="B38" s="27"/>
+      <c r="C38" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="D38" s="23"/>
+      <c r="E38" s="23">
+        <v>0</v>
+      </c>
+      <c r="F38" s="23"/>
+      <c r="G38" s="23"/>
+      <c r="H38" s="23"/>
+      <c r="I38" s="23"/>
+      <c r="J38" s="23">
+        <v>1</v>
+      </c>
+      <c r="K38" s="23"/>
+      <c r="L38" s="23"/>
+      <c r="M38" s="23"/>
+      <c r="N38" s="23"/>
+      <c r="O38" s="23"/>
+      <c r="P38" s="23"/>
+      <c r="Q38" s="23"/>
+      <c r="R38" s="23"/>
+      <c r="S38" s="23"/>
+      <c r="T38" s="23"/>
+      <c r="U38" s="23"/>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A39" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B39" s="27"/>
+      <c r="C39" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D39" s="23"/>
+      <c r="E39" s="23">
+        <v>0</v>
+      </c>
+      <c r="F39" s="23"/>
+      <c r="G39" s="23"/>
+      <c r="H39" s="23"/>
+      <c r="I39" s="23"/>
+      <c r="J39" s="23"/>
+      <c r="K39" s="23"/>
+      <c r="L39" s="23"/>
+      <c r="M39" s="18">
+        <v>63.607356573910501</v>
+      </c>
+      <c r="N39" s="16"/>
+      <c r="O39" s="23"/>
+      <c r="P39" s="23"/>
+      <c r="Q39" s="23"/>
+      <c r="R39" s="23"/>
+      <c r="S39" s="23"/>
+      <c r="T39" s="23"/>
+      <c r="U39" s="23"/>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A40" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="B40" s="26"/>
+      <c r="C40" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="D40" s="23"/>
+      <c r="E40" s="23">
+        <v>0</v>
+      </c>
+      <c r="F40" s="23"/>
+      <c r="G40" s="23"/>
+      <c r="H40" s="23"/>
+      <c r="I40" s="24">
+        <v>100</v>
+      </c>
+      <c r="J40" s="24">
+        <v>100</v>
+      </c>
+      <c r="K40" s="23"/>
+      <c r="L40" s="23"/>
+      <c r="M40" s="18">
+        <v>8.5514960440672301</v>
+      </c>
+      <c r="N40" s="16"/>
+      <c r="O40" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="P40" s="23"/>
+      <c r="Q40" s="23"/>
+      <c r="R40" s="23"/>
+      <c r="S40" s="23"/>
+      <c r="T40" s="23"/>
+      <c r="U40" s="23"/>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A41" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="B41" s="26"/>
+      <c r="C41" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="D41" s="23"/>
+      <c r="E41" s="23">
+        <f>VLOOKUP(A41,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="F41" s="23"/>
+      <c r="G41" s="23"/>
+      <c r="H41" s="23"/>
+      <c r="I41" s="23">
+        <v>1</v>
+      </c>
+      <c r="J41" s="23">
+        <v>2</v>
+      </c>
+      <c r="K41" s="23"/>
+      <c r="L41" s="23"/>
+      <c r="M41" s="18">
+        <v>-13.3040694607334</v>
+      </c>
+      <c r="N41" s="16"/>
+      <c r="O41" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="P41" s="23"/>
+      <c r="Q41" s="23"/>
+      <c r="R41" s="23"/>
+      <c r="S41" s="23"/>
+      <c r="T41" s="23"/>
+      <c r="U41" s="23"/>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A42" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B42" s="27"/>
+      <c r="C42" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D42" s="23"/>
+      <c r="E42" s="23">
+        <v>0</v>
+      </c>
+      <c r="F42" s="23"/>
+      <c r="G42" s="23"/>
+      <c r="H42" s="23"/>
+      <c r="I42" s="23"/>
+      <c r="J42" s="23"/>
+      <c r="K42" s="23"/>
+      <c r="L42" s="23"/>
+      <c r="M42" s="18">
+        <v>13.304069460733899</v>
+      </c>
+      <c r="N42" s="16"/>
+      <c r="O42" s="23"/>
+      <c r="P42" s="23"/>
+      <c r="Q42" s="23"/>
+      <c r="R42" s="23"/>
+      <c r="S42" s="23"/>
+      <c r="T42" s="23"/>
+      <c r="U42" s="23"/>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A43" s="23" t="s">
+        <v>214</v>
+      </c>
+      <c r="B43" s="23"/>
+      <c r="C43" s="23" t="s">
+        <v>215</v>
+      </c>
+      <c r="D43" s="23"/>
+      <c r="E43" s="23">
+        <f>VLOOKUP(A43,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>1.3</v>
+      </c>
+      <c r="F43" s="23"/>
+      <c r="G43" s="23"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23">
+        <f>VLOOKUP($A43,[1]ecoliN1!$A$2:$J$84,9,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="J43" s="23">
+        <f>VLOOKUP($A43,[1]ecoliN1!$A$2:$J$84,10,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="K43" s="23"/>
+      <c r="L43" s="23"/>
+      <c r="M43" s="23"/>
+      <c r="N43" s="23"/>
+      <c r="O43" s="23"/>
+      <c r="P43" s="23"/>
+      <c r="Q43" s="23"/>
+      <c r="R43" s="23"/>
+      <c r="S43" s="23"/>
+      <c r="T43" s="23"/>
+      <c r="U43" s="23"/>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A44" s="30" t="s">
+        <v>229</v>
+      </c>
+      <c r="B44" s="29"/>
+      <c r="C44" s="30" t="s">
+        <v>252</v>
+      </c>
+      <c r="D44" s="29" t="s">
+        <v>169</v>
+      </c>
+      <c r="E44" s="29">
+        <v>-1.6</v>
+      </c>
+      <c r="F44" s="29">
+        <v>-42.6</v>
+      </c>
+      <c r="G44" s="29">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="H44" s="29"/>
+      <c r="I44" s="29">
+        <v>174</v>
+      </c>
+      <c r="J44" s="29"/>
+      <c r="K44" s="29"/>
+      <c r="L44" s="29">
+        <v>0.63</v>
+      </c>
+      <c r="M44" s="31">
+        <v>18.144898505714799</v>
+      </c>
+      <c r="N44" s="30" t="s">
+        <v>230</v>
+      </c>
+      <c r="O44" s="29" t="s">
+        <v>231</v>
+      </c>
+      <c r="P44" s="29"/>
+      <c r="Q44" s="29"/>
+      <c r="R44" s="29"/>
+      <c r="S44" s="29"/>
+      <c r="T44" s="29"/>
+      <c r="U44" s="29"/>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A45" s="33" t="s">
+        <v>232</v>
+      </c>
+      <c r="B45" s="32"/>
+      <c r="C45" s="33" t="s">
+        <v>233</v>
+      </c>
+      <c r="D45" s="32" t="s">
+        <v>234</v>
+      </c>
+      <c r="E45" s="32">
+        <v>-5.0999999999999996</v>
+      </c>
+      <c r="F45" s="32">
+        <v>-39.799999999999997</v>
+      </c>
+      <c r="G45" s="32">
+        <v>-2.1</v>
+      </c>
+      <c r="H45" s="32"/>
+      <c r="I45" s="32">
+        <v>25</v>
+      </c>
+      <c r="J45" s="32"/>
+      <c r="K45" s="32"/>
+      <c r="L45" s="32"/>
+      <c r="M45" s="34">
+        <v>18.144898505714799</v>
+      </c>
+      <c r="N45" s="33" t="s">
+        <v>235</v>
+      </c>
+      <c r="O45" s="32"/>
+      <c r="P45" s="32"/>
+      <c r="Q45" s="32"/>
+      <c r="R45" s="32"/>
+      <c r="S45" s="32"/>
+      <c r="T45" s="32"/>
+      <c r="U45" s="32"/>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A46" s="36" t="s">
+        <v>236</v>
+      </c>
+      <c r="B46" s="35"/>
+      <c r="C46" s="36" t="s">
+        <v>253</v>
+      </c>
+      <c r="D46" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="E46" s="35">
+        <v>0.9</v>
+      </c>
+      <c r="F46" s="35">
+        <v>-43.6</v>
+      </c>
+      <c r="G46" s="35">
+        <v>31.7</v>
+      </c>
+      <c r="H46" s="35"/>
+      <c r="I46" s="35">
+        <v>75.650000000000006</v>
+      </c>
+      <c r="J46" s="35"/>
+      <c r="K46" s="35"/>
+      <c r="L46" s="35"/>
+      <c r="M46" s="37">
+        <v>18.144898505714799</v>
+      </c>
+      <c r="N46" s="36" t="s">
+        <v>237</v>
+      </c>
+      <c r="O46" s="35"/>
+      <c r="P46" s="35"/>
+      <c r="Q46" s="35"/>
+      <c r="R46" s="35"/>
+      <c r="S46" s="35"/>
+      <c r="T46" s="35"/>
+      <c r="U46" s="35"/>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A47" s="39" t="s">
+        <v>238</v>
+      </c>
+      <c r="B47" s="38"/>
+      <c r="C47" s="39" t="s">
+        <v>239</v>
+      </c>
+      <c r="D47" s="38"/>
+      <c r="E47" s="38"/>
+      <c r="F47" s="38">
+        <v>-22.2</v>
+      </c>
+      <c r="G47" s="38">
+        <v>15.5</v>
+      </c>
+      <c r="H47" s="38">
+        <v>3.91</v>
+      </c>
+      <c r="I47" s="38">
+        <v>1180.01</v>
+      </c>
+      <c r="J47" s="38"/>
+      <c r="K47" s="38"/>
+      <c r="L47" s="38"/>
+      <c r="M47" s="42">
+        <v>10.425678473058399</v>
+      </c>
+      <c r="N47" s="39" t="s">
+        <v>240</v>
+      </c>
+      <c r="O47" s="38"/>
+      <c r="P47" s="38"/>
+      <c r="Q47" s="38"/>
+      <c r="R47" s="38"/>
+      <c r="S47" s="38"/>
+      <c r="T47" s="38"/>
+      <c r="U47" s="38"/>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A48" s="39" t="s">
+        <v>241</v>
+      </c>
+      <c r="B48" s="38"/>
+      <c r="C48" s="39" t="s">
+        <v>242</v>
+      </c>
+      <c r="D48" s="38"/>
+      <c r="E48" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="F48" s="38">
+        <v>-16.899999999999999</v>
+      </c>
+      <c r="G48" s="38">
+        <v>20.8</v>
+      </c>
+      <c r="H48" s="38"/>
+      <c r="I48" s="38">
+        <v>2100</v>
+      </c>
+      <c r="J48" s="38"/>
+      <c r="K48" s="38"/>
+      <c r="L48" s="38"/>
+      <c r="M48" s="42">
+        <v>-7.7192200326564304</v>
+      </c>
+      <c r="N48" s="39" t="s">
+        <v>243</v>
+      </c>
+      <c r="O48" s="38"/>
+      <c r="P48" s="38"/>
+      <c r="Q48" s="38"/>
+      <c r="R48" s="38"/>
+      <c r="S48" s="38"/>
+      <c r="T48" s="38"/>
+      <c r="U48" s="38"/>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A49" s="39" t="s">
+        <v>244</v>
+      </c>
+      <c r="B49" s="38"/>
+      <c r="C49" s="39" t="s">
+        <v>245</v>
+      </c>
+      <c r="D49" s="38"/>
+      <c r="E49" s="38"/>
+      <c r="F49" s="38">
+        <v>-33.9</v>
+      </c>
+      <c r="G49" s="38">
+        <v>41.5</v>
+      </c>
+      <c r="H49" s="38">
+        <v>0.216</v>
+      </c>
+      <c r="I49" s="38"/>
+      <c r="J49" s="38">
+        <v>21.9</v>
+      </c>
+      <c r="K49" s="38"/>
+      <c r="L49" s="38"/>
+      <c r="M49" s="41">
+        <v>-5.6324290470476202</v>
+      </c>
+      <c r="N49" s="39" t="s">
+        <v>246</v>
+      </c>
+      <c r="O49" s="38"/>
+      <c r="P49" s="38"/>
+      <c r="Q49" s="38"/>
+      <c r="R49" s="38"/>
+      <c r="S49" s="38"/>
+      <c r="T49" s="38"/>
+      <c r="U49" s="38"/>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A50" s="39" t="s">
+        <v>247</v>
+      </c>
+      <c r="B50" s="38"/>
+      <c r="C50" s="39" t="s">
+        <v>248</v>
+      </c>
+      <c r="D50" s="38"/>
+      <c r="E50" s="38">
+        <v>-1.7</v>
+      </c>
+      <c r="F50" s="38">
+        <v>-38.4</v>
+      </c>
+      <c r="G50" s="38">
+        <v>36.9</v>
+      </c>
+      <c r="H50" s="38"/>
+      <c r="I50" s="38">
+        <v>16.57</v>
+      </c>
+      <c r="J50" s="38"/>
+      <c r="K50" s="38"/>
+      <c r="L50" s="38"/>
+      <c r="M50" s="41">
+        <v>5.6324290470476202</v>
+      </c>
+      <c r="N50" s="39" t="s">
+        <v>249</v>
+      </c>
+      <c r="O50" s="38"/>
+      <c r="P50" s="38"/>
+      <c r="Q50" s="38"/>
+      <c r="R50" s="38"/>
+      <c r="S50" s="38"/>
+      <c r="T50" s="38"/>
+      <c r="U50" s="38"/>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A51" s="39" t="s">
+        <v>250</v>
+      </c>
+      <c r="B51" s="38"/>
+      <c r="C51" s="39" t="s">
+        <v>251</v>
+      </c>
+      <c r="D51" s="38"/>
+      <c r="E51" s="38">
+        <v>1.7</v>
+      </c>
+      <c r="F51" s="38">
+        <v>-27.7</v>
+      </c>
+      <c r="G51" s="38">
+        <v>47.7</v>
+      </c>
+      <c r="H51" s="38">
+        <v>1.77E-2</v>
+      </c>
+      <c r="I51" s="38"/>
+      <c r="J51" s="38">
+        <v>20.437999999999999</v>
+      </c>
+      <c r="K51" s="38"/>
+      <c r="L51" s="38"/>
+      <c r="M51" s="41">
+        <v>-4.7932494260107603</v>
+      </c>
+      <c r="N51" s="39" t="s">
+        <v>246</v>
+      </c>
+      <c r="O51" s="38"/>
+      <c r="P51" s="38"/>
+      <c r="Q51" s="38"/>
+      <c r="R51" s="38"/>
+      <c r="S51" s="38"/>
+      <c r="T51" s="38"/>
+      <c r="U51" s="38"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="43" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="38" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="38">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="38" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="38" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5" s="40">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="40">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="38" t="s">
+        <v>140</v>
+      </c>
+      <c r="B7" s="40">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="38" t="s">
+        <v>141</v>
+      </c>
+      <c r="B8" s="40">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="38" t="s">
+        <v>207</v>
+      </c>
+      <c r="B9" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="38" t="s">
+        <v>208</v>
+      </c>
+      <c r="B10" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="38" t="s">
+        <v>209</v>
+      </c>
+      <c r="B11" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="38" t="s">
+        <v>210</v>
+      </c>
+      <c r="B12" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="38" t="s">
+        <v>211</v>
+      </c>
+      <c r="B13" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="B14" s="40">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="38" t="s">
+        <v>226</v>
+      </c>
+      <c r="B15" s="40">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U43"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
@@ -10426,11 +13223,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B15"/>
     </sheetView>
   </sheetViews>
@@ -10561,12 +13358,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U67"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:XFD22"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
changes to biomass reaction
</commit_message>
<xml_diff>
--- a/KineticModel/data/gtoyall.xlsx
+++ b/KineticModel/data/gtoyall.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25590" windowHeight="7875" firstSheet="3" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25590" windowHeight="7875" firstSheet="4" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="gtoy1" sheetId="2" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1097" uniqueCount="257">
   <si>
     <t>Enzymes</t>
   </si>
@@ -829,10 +829,13 @@
     <t>[c] : 6pgc ---&gt; ru5p-D</t>
   </si>
   <si>
-    <t>[c] : 1.496 3pg + 3.7478 accoa + 0.3610 e4p + 0.0709 f6p + 0.1290 g3p + 0.2050 g6p + 59.8100 h2o + 1.7867 oaa + 0.5191 pep + 2.8328 pyr + 0.8977 r5p --&gt; 4.1182 akg + 3.7478 coa + 59.8100 h</t>
-  </si>
-  <si>
     <t>biomass</t>
+  </si>
+  <si>
+    <t>[c] : 1.496 3pg + 3.7478 accoa + 0.0709 f6p + 0.1290 g3p + 0.2050 g6p + 59.8100 h2o + 1.7867 oaa + 0.5191 pep + 2.8328 pyr --&gt; 4.1182 akg + 3.7478 coa + 59.8100 h</t>
+  </si>
+  <si>
+    <t>420.74,763.07,368.62,420.74,456.46,1,1.31e4,253.05,1.24e4,323.912,763.07,1</t>
   </si>
 </sst>
 </file>
@@ -942,7 +945,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -989,6 +992,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -7470,7 +7476,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U43"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection sqref="A1:U43"/>
     </sheetView>
   </sheetViews>
@@ -9240,16 +9246,16 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U51"/>
+  <dimension ref="A1:U42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection sqref="A1:U51"/>
+    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
+      <selection sqref="A1:U42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="41.140625" customWidth="1"/>
-    <col min="15" max="15" width="13.5703125" customWidth="1"/>
+    <col min="15" max="15" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="18" x14ac:dyDescent="0.35">
@@ -10700,13 +10706,13 @@
         <v>3.48</v>
       </c>
     </row>
-    <row r="35" spans="1:21" ht="75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="44" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B35" s="44"/>
       <c r="C35" s="45" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D35" s="23"/>
       <c r="E35" s="23">
@@ -10725,7 +10731,9 @@
       <c r="L35" s="24"/>
       <c r="M35" s="23"/>
       <c r="N35" s="23"/>
-      <c r="O35" s="23"/>
+      <c r="O35" s="46" t="s">
+        <v>256</v>
+      </c>
       <c r="P35" s="23"/>
       <c r="Q35" s="23"/>
       <c r="R35" s="23"/>
@@ -10808,12 +10816,12 @@
       <c r="U37" s="23"/>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A38" s="27" t="s">
-        <v>126</v>
+      <c r="A38" s="10" t="s">
+        <v>78</v>
       </c>
       <c r="B38" s="27"/>
-      <c r="C38" s="27" t="s">
-        <v>87</v>
+      <c r="C38" s="10" t="s">
+        <v>79</v>
       </c>
       <c r="D38" s="23"/>
       <c r="E38" s="23">
@@ -10823,13 +10831,13 @@
       <c r="G38" s="23"/>
       <c r="H38" s="23"/>
       <c r="I38" s="23"/>
-      <c r="J38" s="23">
-        <v>1</v>
-      </c>
+      <c r="J38" s="23"/>
       <c r="K38" s="23"/>
       <c r="L38" s="23"/>
-      <c r="M38" s="23"/>
-      <c r="N38" s="23"/>
+      <c r="M38" s="18">
+        <v>63.607356573910501</v>
+      </c>
+      <c r="N38" s="16"/>
       <c r="O38" s="23"/>
       <c r="P38" s="23"/>
       <c r="Q38" s="23"/>
@@ -10839,12 +10847,12 @@
       <c r="U38" s="23"/>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A39" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="B39" s="27"/>
-      <c r="C39" s="10" t="s">
-        <v>79</v>
+      <c r="A39" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="B39" s="26"/>
+      <c r="C39" s="25" t="s">
+        <v>129</v>
       </c>
       <c r="D39" s="23"/>
       <c r="E39" s="23">
@@ -10853,15 +10861,21 @@
       <c r="F39" s="23"/>
       <c r="G39" s="23"/>
       <c r="H39" s="23"/>
-      <c r="I39" s="23"/>
-      <c r="J39" s="23"/>
+      <c r="I39" s="24">
+        <v>100</v>
+      </c>
+      <c r="J39" s="24">
+        <v>100</v>
+      </c>
       <c r="K39" s="23"/>
       <c r="L39" s="23"/>
       <c r="M39" s="18">
-        <v>63.607356573910501</v>
+        <v>8.5514960440672301</v>
       </c>
       <c r="N39" s="16"/>
-      <c r="O39" s="23"/>
+      <c r="O39" s="24" t="s">
+        <v>131</v>
+      </c>
       <c r="P39" s="23"/>
       <c r="Q39" s="23"/>
       <c r="R39" s="23"/>
@@ -10871,33 +10885,34 @@
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" s="25" t="s">
-        <v>130</v>
+        <v>73</v>
       </c>
       <c r="B40" s="26"/>
       <c r="C40" s="25" t="s">
-        <v>129</v>
+        <v>74</v>
       </c>
       <c r="D40" s="23"/>
       <c r="E40" s="23">
+        <f>VLOOKUP(A40,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
         <v>0</v>
       </c>
       <c r="F40" s="23"/>
       <c r="G40" s="23"/>
       <c r="H40" s="23"/>
-      <c r="I40" s="24">
-        <v>100</v>
-      </c>
-      <c r="J40" s="24">
-        <v>100</v>
+      <c r="I40" s="23">
+        <v>1</v>
+      </c>
+      <c r="J40" s="23">
+        <v>2</v>
       </c>
       <c r="K40" s="23"/>
       <c r="L40" s="23"/>
       <c r="M40" s="18">
-        <v>8.5514960440672301</v>
+        <v>-13.3040694607334</v>
       </c>
       <c r="N40" s="16"/>
-      <c r="O40" s="24" t="s">
-        <v>131</v>
+      <c r="O40" s="23" t="s">
+        <v>75</v>
       </c>
       <c r="P40" s="23"/>
       <c r="Q40" s="23"/>
@@ -10907,36 +10922,29 @@
       <c r="U40" s="23"/>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A41" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="B41" s="26"/>
-      <c r="C41" s="25" t="s">
-        <v>74</v>
+      <c r="A41" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B41" s="27"/>
+      <c r="C41" s="10" t="s">
+        <v>81</v>
       </c>
       <c r="D41" s="23"/>
       <c r="E41" s="23">
-        <f>VLOOKUP(A41,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
         <v>0</v>
       </c>
       <c r="F41" s="23"/>
       <c r="G41" s="23"/>
       <c r="H41" s="23"/>
-      <c r="I41" s="23">
-        <v>1</v>
-      </c>
-      <c r="J41" s="23">
-        <v>2</v>
-      </c>
+      <c r="I41" s="23"/>
+      <c r="J41" s="23"/>
       <c r="K41" s="23"/>
       <c r="L41" s="23"/>
       <c r="M41" s="18">
-        <v>-13.3040694607334</v>
+        <v>13.304069460733899</v>
       </c>
       <c r="N41" s="16"/>
-      <c r="O41" s="23" t="s">
-        <v>75</v>
-      </c>
+      <c r="O41" s="23"/>
       <c r="P41" s="23"/>
       <c r="Q41" s="23"/>
       <c r="R41" s="23"/>
@@ -10945,28 +10953,33 @@
       <c r="U41" s="23"/>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A42" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="B42" s="27"/>
-      <c r="C42" s="10" t="s">
-        <v>81</v>
+      <c r="A42" s="23" t="s">
+        <v>214</v>
+      </c>
+      <c r="B42" s="23"/>
+      <c r="C42" s="23" t="s">
+        <v>215</v>
       </c>
       <c r="D42" s="23"/>
       <c r="E42" s="23">
-        <v>0</v>
+        <f>VLOOKUP(A42,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>1.3</v>
       </c>
       <c r="F42" s="23"/>
       <c r="G42" s="23"/>
       <c r="H42" s="23"/>
-      <c r="I42" s="23"/>
-      <c r="J42" s="23"/>
+      <c r="I42" s="23">
+        <f>VLOOKUP($A42,[1]ecoliN1!$A$2:$J$84,9,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="J42" s="23">
+        <f>VLOOKUP($A42,[1]ecoliN1!$A$2:$J$84,10,FALSE)</f>
+        <v>0</v>
+      </c>
       <c r="K42" s="23"/>
       <c r="L42" s="23"/>
-      <c r="M42" s="18">
-        <v>13.304069460733899</v>
-      </c>
-      <c r="N42" s="16"/>
+      <c r="M42" s="23"/>
+      <c r="N42" s="23"/>
       <c r="O42" s="23"/>
       <c r="P42" s="23"/>
       <c r="Q42" s="23"/>
@@ -10974,366 +10987,6 @@
       <c r="S42" s="23"/>
       <c r="T42" s="23"/>
       <c r="U42" s="23"/>
-    </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A43" s="23" t="s">
-        <v>214</v>
-      </c>
-      <c r="B43" s="23"/>
-      <c r="C43" s="23" t="s">
-        <v>215</v>
-      </c>
-      <c r="D43" s="23"/>
-      <c r="E43" s="23">
-        <f>VLOOKUP(A43,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
-        <v>1.3</v>
-      </c>
-      <c r="F43" s="23"/>
-      <c r="G43" s="23"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="23">
-        <f>VLOOKUP($A43,[1]ecoliN1!$A$2:$J$84,9,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="J43" s="23">
-        <f>VLOOKUP($A43,[1]ecoliN1!$A$2:$J$84,10,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="K43" s="23"/>
-      <c r="L43" s="23"/>
-      <c r="M43" s="23"/>
-      <c r="N43" s="23"/>
-      <c r="O43" s="23"/>
-      <c r="P43" s="23"/>
-      <c r="Q43" s="23"/>
-      <c r="R43" s="23"/>
-      <c r="S43" s="23"/>
-      <c r="T43" s="23"/>
-      <c r="U43" s="23"/>
-    </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A44" s="30" t="s">
-        <v>229</v>
-      </c>
-      <c r="B44" s="29"/>
-      <c r="C44" s="30" t="s">
-        <v>252</v>
-      </c>
-      <c r="D44" s="29" t="s">
-        <v>169</v>
-      </c>
-      <c r="E44" s="29">
-        <v>-1.6</v>
-      </c>
-      <c r="F44" s="29">
-        <v>-42.6</v>
-      </c>
-      <c r="G44" s="29">
-        <v>35.299999999999997</v>
-      </c>
-      <c r="H44" s="29"/>
-      <c r="I44" s="29">
-        <v>174</v>
-      </c>
-      <c r="J44" s="29"/>
-      <c r="K44" s="29"/>
-      <c r="L44" s="29">
-        <v>0.63</v>
-      </c>
-      <c r="M44" s="31">
-        <v>18.144898505714799</v>
-      </c>
-      <c r="N44" s="30" t="s">
-        <v>230</v>
-      </c>
-      <c r="O44" s="29" t="s">
-        <v>231</v>
-      </c>
-      <c r="P44" s="29"/>
-      <c r="Q44" s="29"/>
-      <c r="R44" s="29"/>
-      <c r="S44" s="29"/>
-      <c r="T44" s="29"/>
-      <c r="U44" s="29"/>
-    </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A45" s="33" t="s">
-        <v>232</v>
-      </c>
-      <c r="B45" s="32"/>
-      <c r="C45" s="33" t="s">
-        <v>233</v>
-      </c>
-      <c r="D45" s="32" t="s">
-        <v>234</v>
-      </c>
-      <c r="E45" s="32">
-        <v>-5.0999999999999996</v>
-      </c>
-      <c r="F45" s="32">
-        <v>-39.799999999999997</v>
-      </c>
-      <c r="G45" s="32">
-        <v>-2.1</v>
-      </c>
-      <c r="H45" s="32"/>
-      <c r="I45" s="32">
-        <v>25</v>
-      </c>
-      <c r="J45" s="32"/>
-      <c r="K45" s="32"/>
-      <c r="L45" s="32"/>
-      <c r="M45" s="34">
-        <v>18.144898505714799</v>
-      </c>
-      <c r="N45" s="33" t="s">
-        <v>235</v>
-      </c>
-      <c r="O45" s="32"/>
-      <c r="P45" s="32"/>
-      <c r="Q45" s="32"/>
-      <c r="R45" s="32"/>
-      <c r="S45" s="32"/>
-      <c r="T45" s="32"/>
-      <c r="U45" s="32"/>
-    </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A46" s="36" t="s">
-        <v>236</v>
-      </c>
-      <c r="B46" s="35"/>
-      <c r="C46" s="36" t="s">
-        <v>253</v>
-      </c>
-      <c r="D46" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="E46" s="35">
-        <v>0.9</v>
-      </c>
-      <c r="F46" s="35">
-        <v>-43.6</v>
-      </c>
-      <c r="G46" s="35">
-        <v>31.7</v>
-      </c>
-      <c r="H46" s="35"/>
-      <c r="I46" s="35">
-        <v>75.650000000000006</v>
-      </c>
-      <c r="J46" s="35"/>
-      <c r="K46" s="35"/>
-      <c r="L46" s="35"/>
-      <c r="M46" s="37">
-        <v>18.144898505714799</v>
-      </c>
-      <c r="N46" s="36" t="s">
-        <v>237</v>
-      </c>
-      <c r="O46" s="35"/>
-      <c r="P46" s="35"/>
-      <c r="Q46" s="35"/>
-      <c r="R46" s="35"/>
-      <c r="S46" s="35"/>
-      <c r="T46" s="35"/>
-      <c r="U46" s="35"/>
-    </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A47" s="39" t="s">
-        <v>238</v>
-      </c>
-      <c r="B47" s="38"/>
-      <c r="C47" s="39" t="s">
-        <v>239</v>
-      </c>
-      <c r="D47" s="38"/>
-      <c r="E47" s="38"/>
-      <c r="F47" s="38">
-        <v>-22.2</v>
-      </c>
-      <c r="G47" s="38">
-        <v>15.5</v>
-      </c>
-      <c r="H47" s="38">
-        <v>3.91</v>
-      </c>
-      <c r="I47" s="38">
-        <v>1180.01</v>
-      </c>
-      <c r="J47" s="38"/>
-      <c r="K47" s="38"/>
-      <c r="L47" s="38"/>
-      <c r="M47" s="42">
-        <v>10.425678473058399</v>
-      </c>
-      <c r="N47" s="39" t="s">
-        <v>240</v>
-      </c>
-      <c r="O47" s="38"/>
-      <c r="P47" s="38"/>
-      <c r="Q47" s="38"/>
-      <c r="R47" s="38"/>
-      <c r="S47" s="38"/>
-      <c r="T47" s="38"/>
-      <c r="U47" s="38"/>
-    </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A48" s="39" t="s">
-        <v>241</v>
-      </c>
-      <c r="B48" s="38"/>
-      <c r="C48" s="39" t="s">
-        <v>242</v>
-      </c>
-      <c r="D48" s="38"/>
-      <c r="E48" s="38">
-        <v>0.5</v>
-      </c>
-      <c r="F48" s="38">
-        <v>-16.899999999999999</v>
-      </c>
-      <c r="G48" s="38">
-        <v>20.8</v>
-      </c>
-      <c r="H48" s="38"/>
-      <c r="I48" s="38">
-        <v>2100</v>
-      </c>
-      <c r="J48" s="38"/>
-      <c r="K48" s="38"/>
-      <c r="L48" s="38"/>
-      <c r="M48" s="42">
-        <v>-7.7192200326564304</v>
-      </c>
-      <c r="N48" s="39" t="s">
-        <v>243</v>
-      </c>
-      <c r="O48" s="38"/>
-      <c r="P48" s="38"/>
-      <c r="Q48" s="38"/>
-      <c r="R48" s="38"/>
-      <c r="S48" s="38"/>
-      <c r="T48" s="38"/>
-      <c r="U48" s="38"/>
-    </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A49" s="39" t="s">
-        <v>244</v>
-      </c>
-      <c r="B49" s="38"/>
-      <c r="C49" s="39" t="s">
-        <v>245</v>
-      </c>
-      <c r="D49" s="38"/>
-      <c r="E49" s="38"/>
-      <c r="F49" s="38">
-        <v>-33.9</v>
-      </c>
-      <c r="G49" s="38">
-        <v>41.5</v>
-      </c>
-      <c r="H49" s="38">
-        <v>0.216</v>
-      </c>
-      <c r="I49" s="38"/>
-      <c r="J49" s="38">
-        <v>21.9</v>
-      </c>
-      <c r="K49" s="38"/>
-      <c r="L49" s="38"/>
-      <c r="M49" s="41">
-        <v>-5.6324290470476202</v>
-      </c>
-      <c r="N49" s="39" t="s">
-        <v>246</v>
-      </c>
-      <c r="O49" s="38"/>
-      <c r="P49" s="38"/>
-      <c r="Q49" s="38"/>
-      <c r="R49" s="38"/>
-      <c r="S49" s="38"/>
-      <c r="T49" s="38"/>
-      <c r="U49" s="38"/>
-    </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A50" s="39" t="s">
-        <v>247</v>
-      </c>
-      <c r="B50" s="38"/>
-      <c r="C50" s="39" t="s">
-        <v>248</v>
-      </c>
-      <c r="D50" s="38"/>
-      <c r="E50" s="38">
-        <v>-1.7</v>
-      </c>
-      <c r="F50" s="38">
-        <v>-38.4</v>
-      </c>
-      <c r="G50" s="38">
-        <v>36.9</v>
-      </c>
-      <c r="H50" s="38"/>
-      <c r="I50" s="38">
-        <v>16.57</v>
-      </c>
-      <c r="J50" s="38"/>
-      <c r="K50" s="38"/>
-      <c r="L50" s="38"/>
-      <c r="M50" s="41">
-        <v>5.6324290470476202</v>
-      </c>
-      <c r="N50" s="39" t="s">
-        <v>249</v>
-      </c>
-      <c r="O50" s="38"/>
-      <c r="P50" s="38"/>
-      <c r="Q50" s="38"/>
-      <c r="R50" s="38"/>
-      <c r="S50" s="38"/>
-      <c r="T50" s="38"/>
-      <c r="U50" s="38"/>
-    </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A51" s="39" t="s">
-        <v>250</v>
-      </c>
-      <c r="B51" s="38"/>
-      <c r="C51" s="39" t="s">
-        <v>251</v>
-      </c>
-      <c r="D51" s="38"/>
-      <c r="E51" s="38">
-        <v>1.7</v>
-      </c>
-      <c r="F51" s="38">
-        <v>-27.7</v>
-      </c>
-      <c r="G51" s="38">
-        <v>47.7</v>
-      </c>
-      <c r="H51" s="38">
-        <v>1.77E-2</v>
-      </c>
-      <c r="I51" s="38"/>
-      <c r="J51" s="38">
-        <v>20.437999999999999</v>
-      </c>
-      <c r="K51" s="38"/>
-      <c r="L51" s="38"/>
-      <c r="M51" s="41">
-        <v>-4.7932494260107603</v>
-      </c>
-      <c r="N51" s="39" t="s">
-        <v>246</v>
-      </c>
-      <c r="O51" s="38"/>
-      <c r="P51" s="38"/>
-      <c r="Q51" s="38"/>
-      <c r="R51" s="38"/>
-      <c r="S51" s="38"/>
-      <c r="T51" s="38"/>
-      <c r="U51" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11479,7 +11132,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U43"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="A28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
@@ -13360,10 +13013,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U67"/>
+  <dimension ref="A1:U75"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="A68" sqref="A68:XFD75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15443,7 +15096,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="65" spans="1:15" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="28" t="s">
         <v>202</v>
       </c>
@@ -15469,7 +15122,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="66" spans="1:15" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="10" t="s">
         <v>205</v>
       </c>
@@ -15485,7 +15138,7 @@
       </c>
       <c r="N66" s="16"/>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A67" s="23" t="s">
         <v>214</v>
       </c>
@@ -15493,6 +15146,330 @@
       <c r="C67" s="23" t="s">
         <v>215</v>
       </c>
+    </row>
+    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A68" s="30" t="s">
+        <v>229</v>
+      </c>
+      <c r="B68" s="29"/>
+      <c r="C68" s="30" t="s">
+        <v>252</v>
+      </c>
+      <c r="D68" s="29" t="s">
+        <v>169</v>
+      </c>
+      <c r="E68" s="29">
+        <v>-1.6</v>
+      </c>
+      <c r="F68" s="29">
+        <v>-42.6</v>
+      </c>
+      <c r="G68" s="29">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="H68" s="29"/>
+      <c r="I68" s="29">
+        <v>174</v>
+      </c>
+      <c r="J68" s="29"/>
+      <c r="K68" s="29"/>
+      <c r="L68" s="29">
+        <v>0.63</v>
+      </c>
+      <c r="M68" s="31">
+        <v>18.144898505714799</v>
+      </c>
+      <c r="N68" s="30" t="s">
+        <v>230</v>
+      </c>
+      <c r="O68" s="29" t="s">
+        <v>231</v>
+      </c>
+      <c r="P68" s="29"/>
+      <c r="Q68" s="29"/>
+      <c r="R68" s="29"/>
+      <c r="S68" s="29"/>
+      <c r="T68" s="29"/>
+      <c r="U68" s="29"/>
+    </row>
+    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A69" s="33" t="s">
+        <v>232</v>
+      </c>
+      <c r="B69" s="32"/>
+      <c r="C69" s="33" t="s">
+        <v>233</v>
+      </c>
+      <c r="D69" s="32" t="s">
+        <v>234</v>
+      </c>
+      <c r="E69" s="32">
+        <v>-5.0999999999999996</v>
+      </c>
+      <c r="F69" s="32">
+        <v>-39.799999999999997</v>
+      </c>
+      <c r="G69" s="32">
+        <v>-2.1</v>
+      </c>
+      <c r="H69" s="32"/>
+      <c r="I69" s="32">
+        <v>25</v>
+      </c>
+      <c r="J69" s="32"/>
+      <c r="K69" s="32"/>
+      <c r="L69" s="32"/>
+      <c r="M69" s="34">
+        <v>18.144898505714799</v>
+      </c>
+      <c r="N69" s="33" t="s">
+        <v>235</v>
+      </c>
+      <c r="O69" s="32"/>
+      <c r="P69" s="32"/>
+      <c r="Q69" s="32"/>
+      <c r="R69" s="32"/>
+      <c r="S69" s="32"/>
+      <c r="T69" s="32"/>
+      <c r="U69" s="32"/>
+    </row>
+    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A70" s="36" t="s">
+        <v>236</v>
+      </c>
+      <c r="B70" s="35"/>
+      <c r="C70" s="36" t="s">
+        <v>253</v>
+      </c>
+      <c r="D70" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="E70" s="35">
+        <v>0.9</v>
+      </c>
+      <c r="F70" s="35">
+        <v>-43.6</v>
+      </c>
+      <c r="G70" s="35">
+        <v>31.7</v>
+      </c>
+      <c r="H70" s="35"/>
+      <c r="I70" s="35">
+        <v>75.650000000000006</v>
+      </c>
+      <c r="J70" s="35"/>
+      <c r="K70" s="35"/>
+      <c r="L70" s="35"/>
+      <c r="M70" s="37">
+        <v>18.144898505714799</v>
+      </c>
+      <c r="N70" s="36" t="s">
+        <v>237</v>
+      </c>
+      <c r="O70" s="35"/>
+      <c r="P70" s="35"/>
+      <c r="Q70" s="35"/>
+      <c r="R70" s="35"/>
+      <c r="S70" s="35"/>
+      <c r="T70" s="35"/>
+      <c r="U70" s="35"/>
+    </row>
+    <row r="71" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A71" s="39" t="s">
+        <v>238</v>
+      </c>
+      <c r="B71" s="38"/>
+      <c r="C71" s="39" t="s">
+        <v>239</v>
+      </c>
+      <c r="D71" s="38"/>
+      <c r="E71" s="38"/>
+      <c r="F71" s="38">
+        <v>-22.2</v>
+      </c>
+      <c r="G71" s="38">
+        <v>15.5</v>
+      </c>
+      <c r="H71" s="38">
+        <v>3.91</v>
+      </c>
+      <c r="I71" s="38">
+        <v>1180.01</v>
+      </c>
+      <c r="J71" s="38"/>
+      <c r="K71" s="38"/>
+      <c r="L71" s="38"/>
+      <c r="M71" s="42">
+        <v>10.425678473058399</v>
+      </c>
+      <c r="N71" s="39" t="s">
+        <v>240</v>
+      </c>
+      <c r="O71" s="38"/>
+      <c r="P71" s="38"/>
+      <c r="Q71" s="38"/>
+      <c r="R71" s="38"/>
+      <c r="S71" s="38"/>
+      <c r="T71" s="38"/>
+      <c r="U71" s="38"/>
+    </row>
+    <row r="72" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A72" s="39" t="s">
+        <v>241</v>
+      </c>
+      <c r="B72" s="38"/>
+      <c r="C72" s="39" t="s">
+        <v>242</v>
+      </c>
+      <c r="D72" s="38"/>
+      <c r="E72" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="F72" s="38">
+        <v>-16.899999999999999</v>
+      </c>
+      <c r="G72" s="38">
+        <v>20.8</v>
+      </c>
+      <c r="H72" s="38"/>
+      <c r="I72" s="38">
+        <v>2100</v>
+      </c>
+      <c r="J72" s="38"/>
+      <c r="K72" s="38"/>
+      <c r="L72" s="38"/>
+      <c r="M72" s="42">
+        <v>-7.7192200326564304</v>
+      </c>
+      <c r="N72" s="39" t="s">
+        <v>243</v>
+      </c>
+      <c r="O72" s="38"/>
+      <c r="P72" s="38"/>
+      <c r="Q72" s="38"/>
+      <c r="R72" s="38"/>
+      <c r="S72" s="38"/>
+      <c r="T72" s="38"/>
+      <c r="U72" s="38"/>
+    </row>
+    <row r="73" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A73" s="39" t="s">
+        <v>244</v>
+      </c>
+      <c r="B73" s="38"/>
+      <c r="C73" s="39" t="s">
+        <v>245</v>
+      </c>
+      <c r="D73" s="38"/>
+      <c r="E73" s="38"/>
+      <c r="F73" s="38">
+        <v>-33.9</v>
+      </c>
+      <c r="G73" s="38">
+        <v>41.5</v>
+      </c>
+      <c r="H73" s="38">
+        <v>0.216</v>
+      </c>
+      <c r="I73" s="38"/>
+      <c r="J73" s="38">
+        <v>21.9</v>
+      </c>
+      <c r="K73" s="38"/>
+      <c r="L73" s="38"/>
+      <c r="M73" s="41">
+        <v>-5.6324290470476202</v>
+      </c>
+      <c r="N73" s="39" t="s">
+        <v>246</v>
+      </c>
+      <c r="O73" s="38"/>
+      <c r="P73" s="38"/>
+      <c r="Q73" s="38"/>
+      <c r="R73" s="38"/>
+      <c r="S73" s="38"/>
+      <c r="T73" s="38"/>
+      <c r="U73" s="38"/>
+    </row>
+    <row r="74" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A74" s="39" t="s">
+        <v>247</v>
+      </c>
+      <c r="B74" s="38"/>
+      <c r="C74" s="39" t="s">
+        <v>248</v>
+      </c>
+      <c r="D74" s="38"/>
+      <c r="E74" s="38">
+        <v>-1.7</v>
+      </c>
+      <c r="F74" s="38">
+        <v>-38.4</v>
+      </c>
+      <c r="G74" s="38">
+        <v>36.9</v>
+      </c>
+      <c r="H74" s="38"/>
+      <c r="I74" s="38">
+        <v>16.57</v>
+      </c>
+      <c r="J74" s="38"/>
+      <c r="K74" s="38"/>
+      <c r="L74" s="38"/>
+      <c r="M74" s="41">
+        <v>5.6324290470476202</v>
+      </c>
+      <c r="N74" s="39" t="s">
+        <v>249</v>
+      </c>
+      <c r="O74" s="38"/>
+      <c r="P74" s="38"/>
+      <c r="Q74" s="38"/>
+      <c r="R74" s="38"/>
+      <c r="S74" s="38"/>
+      <c r="T74" s="38"/>
+      <c r="U74" s="38"/>
+    </row>
+    <row r="75" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A75" s="39" t="s">
+        <v>250</v>
+      </c>
+      <c r="B75" s="38"/>
+      <c r="C75" s="39" t="s">
+        <v>251</v>
+      </c>
+      <c r="D75" s="38"/>
+      <c r="E75" s="38">
+        <v>1.7</v>
+      </c>
+      <c r="F75" s="38">
+        <v>-27.7</v>
+      </c>
+      <c r="G75" s="38">
+        <v>47.7</v>
+      </c>
+      <c r="H75" s="38">
+        <v>1.77E-2</v>
+      </c>
+      <c r="I75" s="38"/>
+      <c r="J75" s="38">
+        <v>20.437999999999999</v>
+      </c>
+      <c r="K75" s="38"/>
+      <c r="L75" s="38"/>
+      <c r="M75" s="41">
+        <v>-4.7932494260107603</v>
+      </c>
+      <c r="N75" s="39" t="s">
+        <v>246</v>
+      </c>
+      <c r="O75" s="38"/>
+      <c r="P75" s="38"/>
+      <c r="Q75" s="38"/>
+      <c r="R75" s="38"/>
+      <c r="S75" s="38"/>
+      <c r="T75" s="38"/>
+      <c r="U75" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
remove extra me1 and Vmax for mdh
</commit_message>
<xml_diff>
--- a/KineticModel/data/gtoyall.xlsx
+++ b/KineticModel/data/gtoyall.xlsx
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1320" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1318" uniqueCount="262">
   <si>
     <t>Enzymes</t>
   </si>
@@ -9500,8 +9500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B29" workbookViewId="0">
-      <selection sqref="A1:U52"/>
+    <sheetView tabSelected="1" topLeftCell="B40" workbookViewId="0">
+      <selection sqref="A1:U51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10288,9 +10288,7 @@
       </c>
       <c r="J18" s="38"/>
       <c r="K18" s="38"/>
-      <c r="L18" s="38">
-        <v>50</v>
-      </c>
+      <c r="L18" s="38"/>
       <c r="M18" s="44">
         <v>3.5679805516174299</v>
       </c>
@@ -11234,283 +11232,247 @@
       <c r="T42" s="38"/>
       <c r="U42" s="38"/>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A43" s="38" t="s">
-        <v>214</v>
-      </c>
-      <c r="B43" s="38"/>
-      <c r="C43" s="38" t="s">
-        <v>215</v>
-      </c>
-      <c r="D43" s="38"/>
+    <row r="43" spans="1:21" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="41" t="s">
+        <v>229</v>
+      </c>
+      <c r="C43" s="41" t="s">
+        <v>252</v>
+      </c>
+      <c r="D43" s="38" t="s">
+        <v>169</v>
+      </c>
       <c r="E43" s="38">
-        <f>VLOOKUP(A43,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
-        <v>1.3</v>
-      </c>
-      <c r="F43" s="38"/>
-      <c r="G43" s="38"/>
-      <c r="H43" s="38"/>
+        <v>-1.6</v>
+      </c>
+      <c r="F43" s="38">
+        <v>-42.6</v>
+      </c>
+      <c r="G43" s="38">
+        <v>35.299999999999997</v>
+      </c>
       <c r="I43" s="38">
-        <f>VLOOKUP($A43,[1]ecoliN1!$A$2:$J$84,9,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="J43" s="38">
-        <f>VLOOKUP($A43,[1]ecoliN1!$A$2:$J$84,10,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="K43" s="38"/>
-      <c r="L43" s="38"/>
-      <c r="M43" s="38"/>
-      <c r="N43" s="38"/>
-      <c r="O43" s="38"/>
-      <c r="P43" s="38"/>
-      <c r="Q43" s="38"/>
-      <c r="R43" s="38"/>
-      <c r="S43" s="38"/>
-      <c r="T43" s="38"/>
-      <c r="U43" s="38"/>
+        <v>174</v>
+      </c>
+      <c r="L43" s="38">
+        <v>0.63</v>
+      </c>
+      <c r="M43" s="44">
+        <v>18.144898505714799</v>
+      </c>
+      <c r="N43" s="41" t="s">
+        <v>230</v>
+      </c>
+      <c r="O43" s="38" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="44" spans="1:21" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="41" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="C44" s="41" t="s">
-        <v>252</v>
+        <v>233</v>
       </c>
       <c r="D44" s="38" t="s">
-        <v>169</v>
+        <v>234</v>
       </c>
       <c r="E44" s="38">
-        <v>-1.6</v>
+        <v>-5.0999999999999996</v>
       </c>
       <c r="F44" s="38">
-        <v>-42.6</v>
+        <v>-39.799999999999997</v>
       </c>
       <c r="G44" s="38">
-        <v>35.299999999999997</v>
+        <v>-2.1</v>
       </c>
       <c r="I44" s="38">
-        <v>174</v>
-      </c>
-      <c r="L44" s="38">
-        <v>0.63</v>
+        <v>25</v>
       </c>
       <c r="M44" s="44">
         <v>18.144898505714799</v>
       </c>
       <c r="N44" s="41" t="s">
-        <v>230</v>
-      </c>
-      <c r="O44" s="38" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
     </row>
     <row r="45" spans="1:21" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="41" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="C45" s="41" t="s">
-        <v>233</v>
+        <v>253</v>
       </c>
       <c r="D45" s="38" t="s">
-        <v>234</v>
+        <v>50</v>
       </c>
       <c r="E45" s="38">
-        <v>-5.0999999999999996</v>
+        <v>0.9</v>
       </c>
       <c r="F45" s="38">
-        <v>-39.799999999999997</v>
+        <v>-43.6</v>
       </c>
       <c r="G45" s="38">
-        <v>-2.1</v>
+        <v>31.7</v>
       </c>
       <c r="I45" s="38">
-        <v>25</v>
+        <v>75.650000000000006</v>
       </c>
       <c r="M45" s="44">
         <v>18.144898505714799</v>
       </c>
       <c r="N45" s="41" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="46" spans="1:21" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="41" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C46" s="41" t="s">
-        <v>253</v>
-      </c>
-      <c r="D46" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="E46" s="38">
-        <v>0.9</v>
+        <v>239</v>
       </c>
       <c r="F46" s="38">
-        <v>-43.6</v>
+        <v>-22.2</v>
       </c>
       <c r="G46" s="38">
-        <v>31.7</v>
+        <v>15.5</v>
+      </c>
+      <c r="H46" s="38">
+        <v>3.91</v>
       </c>
       <c r="I46" s="38">
-        <v>75.650000000000006</v>
-      </c>
-      <c r="M46" s="44">
-        <v>18.144898505714799</v>
+        <v>1180.01</v>
+      </c>
+      <c r="M46" s="45">
+        <v>10.425678473058399</v>
       </c>
       <c r="N46" s="41" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="47" spans="1:21" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="41" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="C47" s="41" t="s">
-        <v>239</v>
+        <v>242</v>
+      </c>
+      <c r="E47" s="38">
+        <v>0.5</v>
       </c>
       <c r="F47" s="38">
-        <v>-22.2</v>
+        <v>-16.899999999999999</v>
       </c>
       <c r="G47" s="38">
-        <v>15.5</v>
-      </c>
-      <c r="H47" s="38">
-        <v>3.91</v>
+        <v>20.8</v>
       </c>
       <c r="I47" s="38">
-        <v>1180.01</v>
+        <v>2100</v>
       </c>
       <c r="M47" s="45">
-        <v>10.425678473058399</v>
+        <v>-7.7192200326564304</v>
       </c>
       <c r="N47" s="41" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
     </row>
     <row r="48" spans="1:21" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="41" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="C48" s="41" t="s">
-        <v>242</v>
-      </c>
-      <c r="E48" s="38">
-        <v>0.5</v>
+        <v>245</v>
       </c>
       <c r="F48" s="38">
-        <v>-16.899999999999999</v>
+        <v>-33.9</v>
       </c>
       <c r="G48" s="38">
-        <v>20.8</v>
-      </c>
-      <c r="I48" s="38">
-        <v>2100</v>
-      </c>
-      <c r="M48" s="45">
-        <v>-7.7192200326564304</v>
+        <v>41.5</v>
+      </c>
+      <c r="H48" s="38">
+        <v>0.216</v>
+      </c>
+      <c r="J48" s="38">
+        <v>21.9</v>
+      </c>
+      <c r="M48" s="44">
+        <v>-5.6324290470476202</v>
       </c>
       <c r="N48" s="41" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
     </row>
     <row r="49" spans="1:14" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="41" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="C49" s="41" t="s">
-        <v>245</v>
+        <v>248</v>
+      </c>
+      <c r="E49" s="38">
+        <v>-1.7</v>
       </c>
       <c r="F49" s="38">
-        <v>-33.9</v>
+        <v>-38.4</v>
       </c>
       <c r="G49" s="38">
-        <v>41.5</v>
-      </c>
-      <c r="H49" s="38">
-        <v>0.216</v>
-      </c>
-      <c r="J49" s="38">
-        <v>21.9</v>
+        <v>36.9</v>
+      </c>
+      <c r="I49" s="38">
+        <v>16.57</v>
       </c>
       <c r="M49" s="44">
-        <v>-5.6324290470476202</v>
+        <v>5.6324290470476202</v>
       </c>
       <c r="N49" s="41" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
     </row>
     <row r="50" spans="1:14" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="41" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="C50" s="41" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="E50" s="38">
-        <v>-1.7</v>
+        <v>1.7</v>
       </c>
       <c r="F50" s="38">
-        <v>-38.4</v>
+        <v>-27.7</v>
       </c>
       <c r="G50" s="38">
-        <v>36.9</v>
-      </c>
-      <c r="I50" s="38">
-        <v>16.57</v>
+        <v>47.7</v>
+      </c>
+      <c r="H50" s="38">
+        <v>1.77E-2</v>
+      </c>
+      <c r="J50" s="38">
+        <v>20.437999999999999</v>
       </c>
       <c r="M50" s="44">
-        <v>5.6324290470476202</v>
+        <v>-4.7932494260107603</v>
       </c>
       <c r="N50" s="41" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="51" spans="1:14" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="41" t="s">
-        <v>250</v>
-      </c>
-      <c r="C51" s="41" t="s">
-        <v>251</v>
+      <c r="A51" s="49" t="s">
+        <v>257</v>
+      </c>
+      <c r="B51" s="52"/>
+      <c r="C51" s="49" t="s">
+        <v>258</v>
       </c>
       <c r="E51" s="38">
-        <v>1.7</v>
-      </c>
-      <c r="F51" s="38">
-        <v>-27.7</v>
-      </c>
-      <c r="G51" s="38">
-        <v>47.7</v>
-      </c>
-      <c r="H51" s="38">
-        <v>1.77E-2</v>
-      </c>
-      <c r="J51" s="38">
-        <v>20.437999999999999</v>
+        <v>0</v>
       </c>
       <c r="M51" s="44">
-        <v>-4.7932494260107603</v>
-      </c>
-      <c r="N51" s="41" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="49" t="s">
-        <v>257</v>
-      </c>
-      <c r="B52" s="52"/>
-      <c r="C52" s="49" t="s">
-        <v>258</v>
-      </c>
-      <c r="E52" s="38">
-        <v>0</v>
-      </c>
-      <c r="M52" s="44">
         <v>63.607356573910501</v>
       </c>
-      <c r="N52" s="41"/>
+      <c r="N51" s="41"/>
     </row>
     <row r="53" spans="1:14" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="49"/>
@@ -15460,7 +15422,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U77"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
change [emet] and add initial [biomass]
</commit_message>
<xml_diff>
--- a/KineticModel/data/gtoyall.xlsx
+++ b/KineticModel/data/gtoyall.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25590" windowHeight="7875" firstSheet="6" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25590" windowHeight="7875" firstSheet="6" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="gtoy1" sheetId="2" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1318" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1319" uniqueCount="263">
   <si>
     <t>Enzymes</t>
   </si>
@@ -853,6 +853,9 @@
   </si>
   <si>
     <t>0.205 g6p[c] + 0.8977 r5p[c]  ---&gt; biomass[e]</t>
+  </si>
+  <si>
+    <t>biomass[e]</t>
   </si>
 </sst>
 </file>
@@ -9500,8 +9503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B40" workbookViewId="0">
-      <selection sqref="A1:U51"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43:C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11518,8 +11521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11536,8 +11539,8 @@
       <c r="A2" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="B2" s="38">
-        <v>10</v>
+      <c r="B2" s="43">
+        <v>2.128E-4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -11585,7 +11588,7 @@
         <v>141</v>
       </c>
       <c r="B8" s="43">
-        <v>55</v>
+        <v>62500</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -11629,7 +11632,12 @@
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B14" s="43"/>
+      <c r="A14" t="s">
+        <v>262</v>
+      </c>
+      <c r="B14" s="43">
+        <v>1.2E-2</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15" s="43"/>

</xml_diff>

<commit_message>
remove gtoy3,4 and 5
</commit_message>
<xml_diff>
--- a/KineticModel/data/gtoyall.xlsx
+++ b/KineticModel/data/gtoyall.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shyam\Documents\Courses\CHE1125Project\IntegratedModels\KineticModel\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shyam\Documents\Courses\CHE1125Project\IntegratedModels\KineticModel\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25590" windowHeight="7875" firstSheet="6" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25590" windowHeight="7875" firstSheet="6" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="gtoy1" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
     <externalReference r:id="rId20"/>
     <externalReference r:id="rId21"/>
   </externalReferences>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1319" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1319" uniqueCount="262">
   <si>
     <t>Enzymes</t>
   </si>
@@ -850,9 +850,6 @@
   </si>
   <si>
     <t>0.205 g6p[c] + 0.8977 r5p[c] + 0.361 e4p[c] + 0.5191 pep[c] + 2.8328 pyr[c] + 0.0709 f6p[c] + 0.129 g3p[c] ---&gt; biomass[e]</t>
-  </si>
-  <si>
-    <t>0.205 g6p[c] + 0.8977 r5p[c]  ---&gt; biomass[e]</t>
   </si>
   <si>
     <t>biomass[e]</t>
@@ -6796,23 +6793,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -6848,23 +6828,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -9503,8 +9466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:U51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10966,7 +10929,7 @@
       </c>
       <c r="B35" s="51"/>
       <c r="C35" s="51" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D35" s="38"/>
       <c r="E35" s="38">
@@ -11521,7 +11484,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B14"/>
     </sheetView>
   </sheetViews>
@@ -11633,7 +11596,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B14" s="43">
         <v>1.2E-2</v>
@@ -11663,7 +11626,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U42"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
@@ -15430,7 +15393,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U77"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
+    <sheetView topLeftCell="A58" workbookViewId="0">
       <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add rxn acs for ac[e] --> accoa[c]
</commit_message>
<xml_diff>
--- a/KineticModel/data/gtoyall.xlsx
+++ b/KineticModel/data/gtoyall.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shyam\Documents\Courses\CHE1125Project\IntegratedModels\KineticModel\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shyam\Documents\Courses\CHE1125Project\IntegratedModels\KineticModel\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1202" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1205" uniqueCount="259">
   <si>
     <t>Enzymes</t>
   </si>
@@ -826,6 +826,18 @@
   </si>
   <si>
     <t>ac[e] + h[e] &lt;==&gt; actp[c] + h[c]</t>
+  </si>
+  <si>
+    <t>7,1,0.16,1</t>
+  </si>
+  <si>
+    <t>ACStr</t>
+  </si>
+  <si>
+    <t>ac[e] ---&gt; accoa[c]</t>
+  </si>
+  <si>
+    <t>0.0167,1</t>
   </si>
 </sst>
 </file>
@@ -16083,16 +16095,18 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U50"/>
+  <dimension ref="A1:U51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection sqref="A1:U50"/>
+    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
+      <selection sqref="A1:U51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="44.42578125" customWidth="1"/>
-    <col min="15" max="15" width="13.5703125" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="3" max="3" width="45.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="15" max="15" width="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="18" x14ac:dyDescent="0.35">
@@ -16225,7 +16239,7 @@
         <v>2.7.2.1</v>
       </c>
       <c r="O3" s="36" t="s">
-        <v>127</v>
+        <v>255</v>
       </c>
       <c r="P3" s="36"/>
       <c r="Q3" s="36"/>
@@ -18133,6 +18147,30 @@
       <c r="T50" s="36"/>
       <c r="U50" s="36"/>
     </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A51" s="45" t="s">
+        <v>256</v>
+      </c>
+      <c r="B51" s="49"/>
+      <c r="C51" s="45" t="s">
+        <v>257</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="I51">
+        <v>24.47</v>
+      </c>
+      <c r="J51">
+        <v>0</v>
+      </c>
+      <c r="L51">
+        <v>1</v>
+      </c>
+      <c r="O51" t="s">
+        <v>258</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18143,7 +18181,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection sqref="A1:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18161,7 +18199,7 @@
         <v>93</v>
       </c>
       <c r="B2" s="41">
-        <v>1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
final working model file before addition of cofactors
</commit_message>
<xml_diff>
--- a/KineticModel/data/gtoyall.xlsx
+++ b/KineticModel/data/gtoyall.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1205" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1203" uniqueCount="259">
   <si>
     <t>Enzymes</t>
   </si>
@@ -16095,10 +16095,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U51"/>
+  <dimension ref="A1:U50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
-      <selection sqref="A1:U51"/>
+    <sheetView tabSelected="1" topLeftCell="B27" workbookViewId="0">
+      <selection sqref="A1:U50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17625,12 +17625,12 @@
       <c r="U36" s="36"/>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A37" s="50" t="s">
-        <v>119</v>
+      <c r="A37" s="47" t="s">
+        <v>78</v>
       </c>
       <c r="B37" s="50"/>
-      <c r="C37" s="50" t="s">
-        <v>87</v>
+      <c r="C37" s="47" t="s">
+        <v>79</v>
       </c>
       <c r="D37" s="36"/>
       <c r="E37" s="36">
@@ -17640,13 +17640,13 @@
       <c r="G37" s="36"/>
       <c r="H37" s="36"/>
       <c r="I37" s="36"/>
-      <c r="J37" s="36">
-        <v>1</v>
-      </c>
+      <c r="J37" s="36"/>
       <c r="K37" s="36"/>
       <c r="L37" s="36"/>
-      <c r="M37" s="36"/>
-      <c r="N37" s="36"/>
+      <c r="M37" s="42">
+        <v>63.607356573910501</v>
+      </c>
+      <c r="N37" s="39"/>
       <c r="O37" s="36"/>
       <c r="P37" s="36"/>
       <c r="Q37" s="36"/>
@@ -17656,12 +17656,12 @@
       <c r="U37" s="36"/>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A38" s="47" t="s">
-        <v>78</v>
-      </c>
-      <c r="B38" s="50"/>
-      <c r="C38" s="47" t="s">
-        <v>79</v>
+      <c r="A38" s="45" t="s">
+        <v>123</v>
+      </c>
+      <c r="B38" s="49"/>
+      <c r="C38" s="45" t="s">
+        <v>122</v>
       </c>
       <c r="D38" s="36"/>
       <c r="E38" s="36">
@@ -17670,15 +17670,21 @@
       <c r="F38" s="36"/>
       <c r="G38" s="36"/>
       <c r="H38" s="36"/>
-      <c r="I38" s="36"/>
-      <c r="J38" s="36"/>
+      <c r="I38" s="41">
+        <v>100</v>
+      </c>
+      <c r="J38" s="41">
+        <v>100</v>
+      </c>
       <c r="K38" s="36"/>
       <c r="L38" s="36"/>
       <c r="M38" s="42">
-        <v>63.607356573910501</v>
+        <v>8.5514960440672301</v>
       </c>
       <c r="N38" s="39"/>
-      <c r="O38" s="36"/>
+      <c r="O38" s="41" t="s">
+        <v>124</v>
+      </c>
       <c r="P38" s="36"/>
       <c r="Q38" s="36"/>
       <c r="R38" s="36"/>
@@ -17688,33 +17694,34 @@
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" s="45" t="s">
-        <v>123</v>
+        <v>73</v>
       </c>
       <c r="B39" s="49"/>
       <c r="C39" s="45" t="s">
-        <v>122</v>
+        <v>74</v>
       </c>
       <c r="D39" s="36"/>
       <c r="E39" s="36">
+        <f>VLOOKUP(A39,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
         <v>0</v>
       </c>
       <c r="F39" s="36"/>
       <c r="G39" s="36"/>
       <c r="H39" s="36"/>
-      <c r="I39" s="41">
-        <v>100</v>
-      </c>
-      <c r="J39" s="41">
-        <v>100</v>
+      <c r="I39" s="36">
+        <v>1</v>
+      </c>
+      <c r="J39" s="36">
+        <v>2</v>
       </c>
       <c r="K39" s="36"/>
       <c r="L39" s="36"/>
       <c r="M39" s="42">
-        <v>8.5514960440672301</v>
+        <v>-13.3040694607334</v>
       </c>
       <c r="N39" s="39"/>
-      <c r="O39" s="41" t="s">
-        <v>124</v>
+      <c r="O39" s="36" t="s">
+        <v>75</v>
       </c>
       <c r="P39" s="36"/>
       <c r="Q39" s="36"/>
@@ -17724,36 +17731,29 @@
       <c r="U39" s="36"/>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A40" s="45" t="s">
-        <v>73</v>
-      </c>
-      <c r="B40" s="49"/>
-      <c r="C40" s="45" t="s">
-        <v>74</v>
+      <c r="A40" s="47" t="s">
+        <v>80</v>
+      </c>
+      <c r="B40" s="50"/>
+      <c r="C40" s="47" t="s">
+        <v>81</v>
       </c>
       <c r="D40" s="36"/>
       <c r="E40" s="36">
-        <f>VLOOKUP(A40,[1]ecoli_core!$A$2:$I$84,6,FALSE)</f>
         <v>0</v>
       </c>
       <c r="F40" s="36"/>
       <c r="G40" s="36"/>
       <c r="H40" s="36"/>
-      <c r="I40" s="36">
-        <v>1</v>
-      </c>
-      <c r="J40" s="36">
-        <v>2</v>
-      </c>
+      <c r="I40" s="36"/>
+      <c r="J40" s="36"/>
       <c r="K40" s="36"/>
       <c r="L40" s="36"/>
       <c r="M40" s="42">
-        <v>-13.3040694607334</v>
+        <v>13.304069460733899</v>
       </c>
       <c r="N40" s="39"/>
-      <c r="O40" s="36" t="s">
-        <v>75</v>
-      </c>
+      <c r="O40" s="36"/>
       <c r="P40" s="36"/>
       <c r="Q40" s="36"/>
       <c r="R40" s="36"/>
@@ -17762,29 +17762,43 @@
       <c r="U40" s="36"/>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A41" s="47" t="s">
-        <v>80</v>
-      </c>
-      <c r="B41" s="50"/>
-      <c r="C41" s="47" t="s">
-        <v>81</v>
-      </c>
-      <c r="D41" s="36"/>
+      <c r="A41" s="39" t="s">
+        <v>221</v>
+      </c>
+      <c r="B41" s="36"/>
+      <c r="C41" s="39" t="s">
+        <v>244</v>
+      </c>
+      <c r="D41" s="36" t="s">
+        <v>161</v>
+      </c>
       <c r="E41" s="36">
-        <v>0</v>
-      </c>
-      <c r="F41" s="36"/>
-      <c r="G41" s="36"/>
+        <v>-1.6</v>
+      </c>
+      <c r="F41" s="36">
+        <v>-42.6</v>
+      </c>
+      <c r="G41" s="36">
+        <v>35.299999999999997</v>
+      </c>
       <c r="H41" s="36"/>
-      <c r="I41" s="36"/>
+      <c r="I41" s="36">
+        <v>174</v>
+      </c>
       <c r="J41" s="36"/>
       <c r="K41" s="36"/>
-      <c r="L41" s="36"/>
+      <c r="L41" s="36">
+        <v>0.63</v>
+      </c>
       <c r="M41" s="42">
-        <v>13.304069460733899</v>
-      </c>
-      <c r="N41" s="39"/>
-      <c r="O41" s="36"/>
+        <v>18.144898505714799</v>
+      </c>
+      <c r="N41" s="39" t="s">
+        <v>222</v>
+      </c>
+      <c r="O41" s="36" t="s">
+        <v>223</v>
+      </c>
       <c r="P41" s="36"/>
       <c r="Q41" s="36"/>
       <c r="R41" s="36"/>
@@ -17794,42 +17808,38 @@
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" s="39" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="B42" s="36"/>
       <c r="C42" s="39" t="s">
-        <v>244</v>
+        <v>225</v>
       </c>
       <c r="D42" s="36" t="s">
-        <v>161</v>
+        <v>226</v>
       </c>
       <c r="E42" s="36">
-        <v>-1.6</v>
+        <v>-5.0999999999999996</v>
       </c>
       <c r="F42" s="36">
-        <v>-42.6</v>
+        <v>-39.799999999999997</v>
       </c>
       <c r="G42" s="36">
-        <v>35.299999999999997</v>
+        <v>-2.1</v>
       </c>
       <c r="H42" s="36"/>
       <c r="I42" s="36">
-        <v>174</v>
+        <v>25</v>
       </c>
       <c r="J42" s="36"/>
       <c r="K42" s="36"/>
-      <c r="L42" s="36">
-        <v>0.63</v>
-      </c>
+      <c r="L42" s="36"/>
       <c r="M42" s="42">
         <v>18.144898505714799</v>
       </c>
       <c r="N42" s="39" t="s">
-        <v>222</v>
-      </c>
-      <c r="O42" s="36" t="s">
-        <v>223</v>
-      </c>
+        <v>227</v>
+      </c>
+      <c r="O42" s="36"/>
       <c r="P42" s="36"/>
       <c r="Q42" s="36"/>
       <c r="R42" s="36"/>
@@ -17839,27 +17849,27 @@
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" s="39" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="B43" s="36"/>
       <c r="C43" s="39" t="s">
-        <v>225</v>
+        <v>245</v>
       </c>
       <c r="D43" s="36" t="s">
-        <v>226</v>
+        <v>50</v>
       </c>
       <c r="E43" s="36">
-        <v>-5.0999999999999996</v>
+        <v>0.9</v>
       </c>
       <c r="F43" s="36">
-        <v>-39.799999999999997</v>
+        <v>-43.6</v>
       </c>
       <c r="G43" s="36">
-        <v>-2.1</v>
+        <v>31.7</v>
       </c>
       <c r="H43" s="36"/>
       <c r="I43" s="36">
-        <v>25</v>
+        <v>75.650000000000006</v>
       </c>
       <c r="J43" s="36"/>
       <c r="K43" s="36"/>
@@ -17868,7 +17878,7 @@
         <v>18.144898505714799</v>
       </c>
       <c r="N43" s="39" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="O43" s="36"/>
       <c r="P43" s="36"/>
@@ -17880,36 +17890,34 @@
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" s="39" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B44" s="36"/>
       <c r="C44" s="39" t="s">
-        <v>245</v>
-      </c>
-      <c r="D44" s="36" t="s">
-        <v>50</v>
-      </c>
-      <c r="E44" s="36">
-        <v>0.9</v>
-      </c>
+        <v>231</v>
+      </c>
+      <c r="D44" s="36"/>
+      <c r="E44" s="36"/>
       <c r="F44" s="36">
-        <v>-43.6</v>
+        <v>-22.2</v>
       </c>
       <c r="G44" s="36">
-        <v>31.7</v>
-      </c>
-      <c r="H44" s="36"/>
+        <v>15.5</v>
+      </c>
+      <c r="H44" s="36">
+        <v>3.91</v>
+      </c>
       <c r="I44" s="36">
-        <v>75.650000000000006</v>
+        <v>1180.01</v>
       </c>
       <c r="J44" s="36"/>
       <c r="K44" s="36"/>
       <c r="L44" s="36"/>
-      <c r="M44" s="42">
-        <v>18.144898505714799</v>
+      <c r="M44" s="43">
+        <v>10.425678473058399</v>
       </c>
       <c r="N44" s="39" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="O44" s="36"/>
       <c r="P44" s="36"/>
@@ -17921,34 +17929,34 @@
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" s="39" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="B45" s="36"/>
       <c r="C45" s="39" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D45" s="36"/>
-      <c r="E45" s="36"/>
+      <c r="E45" s="36">
+        <v>0.5</v>
+      </c>
       <c r="F45" s="36">
-        <v>-22.2</v>
+        <v>-16.899999999999999</v>
       </c>
       <c r="G45" s="36">
-        <v>15.5</v>
-      </c>
-      <c r="H45" s="36">
-        <v>3.91</v>
-      </c>
+        <v>20.8</v>
+      </c>
+      <c r="H45" s="36"/>
       <c r="I45" s="36">
-        <v>1180.01</v>
+        <v>2100</v>
       </c>
       <c r="J45" s="36"/>
       <c r="K45" s="36"/>
       <c r="L45" s="36"/>
       <c r="M45" s="43">
-        <v>10.425678473058399</v>
+        <v>-7.7192200326564304</v>
       </c>
       <c r="N45" s="39" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="O45" s="36"/>
       <c r="P45" s="36"/>
@@ -17960,34 +17968,34 @@
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" s="39" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="B46" s="36"/>
       <c r="C46" s="39" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="D46" s="36"/>
-      <c r="E46" s="36">
-        <v>0.5</v>
-      </c>
+      <c r="E46" s="36"/>
       <c r="F46" s="36">
-        <v>-16.899999999999999</v>
+        <v>-33.9</v>
       </c>
       <c r="G46" s="36">
-        <v>20.8</v>
-      </c>
-      <c r="H46" s="36"/>
-      <c r="I46" s="36">
-        <v>2100</v>
-      </c>
-      <c r="J46" s="36"/>
+        <v>41.5</v>
+      </c>
+      <c r="H46" s="36">
+        <v>0.216</v>
+      </c>
+      <c r="I46" s="36"/>
+      <c r="J46" s="36">
+        <v>21.9</v>
+      </c>
       <c r="K46" s="36"/>
       <c r="L46" s="36"/>
-      <c r="M46" s="43">
-        <v>-7.7192200326564304</v>
+      <c r="M46" s="42">
+        <v>-5.6324290470476202</v>
       </c>
       <c r="N46" s="39" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="O46" s="36"/>
       <c r="P46" s="36"/>
@@ -17999,34 +18007,34 @@
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" s="39" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="B47" s="36"/>
       <c r="C47" s="39" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="D47" s="36"/>
-      <c r="E47" s="36"/>
+      <c r="E47" s="36">
+        <v>-1.7</v>
+      </c>
       <c r="F47" s="36">
-        <v>-33.9</v>
+        <v>-38.4</v>
       </c>
       <c r="G47" s="36">
-        <v>41.5</v>
-      </c>
-      <c r="H47" s="36">
-        <v>0.216</v>
-      </c>
-      <c r="I47" s="36"/>
-      <c r="J47" s="36">
-        <v>21.9</v>
-      </c>
+        <v>36.9</v>
+      </c>
+      <c r="H47" s="36"/>
+      <c r="I47" s="36">
+        <v>16.57</v>
+      </c>
+      <c r="J47" s="36"/>
       <c r="K47" s="36"/>
       <c r="L47" s="36"/>
       <c r="M47" s="42">
-        <v>-5.6324290470476202</v>
+        <v>5.6324290470476202</v>
       </c>
       <c r="N47" s="39" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="O47" s="36"/>
       <c r="P47" s="36"/>
@@ -18038,34 +18046,36 @@
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" s="39" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B48" s="36"/>
       <c r="C48" s="39" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="D48" s="36"/>
       <c r="E48" s="36">
-        <v>-1.7</v>
+        <v>1.7</v>
       </c>
       <c r="F48" s="36">
-        <v>-38.4</v>
+        <v>-27.7</v>
       </c>
       <c r="G48" s="36">
-        <v>36.9</v>
-      </c>
-      <c r="H48" s="36"/>
-      <c r="I48" s="36">
-        <v>16.57</v>
-      </c>
-      <c r="J48" s="36"/>
+        <v>47.7</v>
+      </c>
+      <c r="H48" s="36">
+        <v>1.77E-2</v>
+      </c>
+      <c r="I48" s="36"/>
+      <c r="J48" s="36">
+        <v>20.437999999999999</v>
+      </c>
       <c r="K48" s="36"/>
       <c r="L48" s="36"/>
       <c r="M48" s="42">
-        <v>5.6324290470476202</v>
+        <v>-4.7932494260107603</v>
       </c>
       <c r="N48" s="39" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="O48" s="36"/>
       <c r="P48" s="36"/>
@@ -18076,38 +18086,28 @@
       <c r="U48" s="36"/>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A49" s="39" t="s">
-        <v>242</v>
-      </c>
-      <c r="B49" s="36"/>
-      <c r="C49" s="39" t="s">
-        <v>243</v>
+      <c r="A49" s="47" t="s">
+        <v>249</v>
+      </c>
+      <c r="B49" s="50"/>
+      <c r="C49" s="47" t="s">
+        <v>250</v>
       </c>
       <c r="D49" s="36"/>
       <c r="E49" s="36">
-        <v>1.7</v>
-      </c>
-      <c r="F49" s="36">
-        <v>-27.7</v>
-      </c>
-      <c r="G49" s="36">
-        <v>47.7</v>
-      </c>
-      <c r="H49" s="36">
-        <v>1.77E-2</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F49" s="36"/>
+      <c r="G49" s="36"/>
+      <c r="H49" s="36"/>
       <c r="I49" s="36"/>
-      <c r="J49" s="36">
-        <v>20.437999999999999</v>
-      </c>
+      <c r="J49" s="36"/>
       <c r="K49" s="36"/>
       <c r="L49" s="36"/>
       <c r="M49" s="42">
-        <v>-4.7932494260107603</v>
-      </c>
-      <c r="N49" s="39" t="s">
-        <v>238</v>
-      </c>
+        <v>63.607356573910501</v>
+      </c>
+      <c r="N49" s="39"/>
       <c r="O49" s="36"/>
       <c r="P49" s="36"/>
       <c r="Q49" s="36"/>
@@ -18117,57 +18117,26 @@
       <c r="U49" s="36"/>
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A50" s="47" t="s">
-        <v>249</v>
-      </c>
-      <c r="B50" s="50"/>
-      <c r="C50" s="47" t="s">
-        <v>250</v>
-      </c>
-      <c r="D50" s="36"/>
-      <c r="E50" s="36">
-        <v>0</v>
-      </c>
-      <c r="F50" s="36"/>
-      <c r="G50" s="36"/>
-      <c r="H50" s="36"/>
-      <c r="I50" s="36"/>
-      <c r="J50" s="36"/>
-      <c r="K50" s="36"/>
-      <c r="L50" s="36"/>
-      <c r="M50" s="42">
-        <v>63.607356573910501</v>
-      </c>
-      <c r="N50" s="39"/>
-      <c r="O50" s="36"/>
-      <c r="P50" s="36"/>
-      <c r="Q50" s="36"/>
-      <c r="R50" s="36"/>
-      <c r="S50" s="36"/>
-      <c r="T50" s="36"/>
-      <c r="U50" s="36"/>
-    </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A51" s="45" t="s">
+      <c r="A50" s="45" t="s">
         <v>256</v>
       </c>
-      <c r="B51" s="49"/>
-      <c r="C51" s="45" t="s">
+      <c r="B50" s="49"/>
+      <c r="C50" s="45" t="s">
         <v>257</v>
       </c>
-      <c r="E51">
-        <v>0</v>
-      </c>
-      <c r="I51">
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="I50">
         <v>24.47</v>
       </c>
-      <c r="J51">
-        <v>0</v>
-      </c>
-      <c r="L51">
+      <c r="J50">
+        <v>0</v>
+      </c>
+      <c r="L50">
         <v>1</v>
       </c>
-      <c r="O51" t="s">
+      <c r="O50" t="s">
         <v>258</v>
       </c>
     </row>

</xml_diff>